<commit_message>
Switch to Supabase for frontend data (no more OneDrive dependency)
</commit_message>
<xml_diff>
--- a/data/boiler_data.xlsx
+++ b/data/boiler_data.xlsx
@@ -473,46 +473,46 @@
         <v/>
       </c>
       <c r="E2">
-        <v>10.241090046117634</v>
+        <v>8.890879082729294</v>
       </c>
       <c r="F2">
-        <v>4.92796857648261</v>
+        <v>4.860802673967096</v>
       </c>
       <c r="G2">
-        <v>16.999496815759162</v>
+        <v>16.262873163802105</v>
       </c>
       <c r="H2">
-        <v>0.5214328765695964</v>
+        <v>0.5406844238674164</v>
       </c>
       <c r="I2" t="str">
         <v/>
       </c>
       <c r="J2">
-        <v>8.298306865062429</v>
+        <v>9.783927131683626</v>
       </c>
       <c r="K2">
-        <v>4.04567043462756</v>
+        <v>4.314000747805599</v>
       </c>
       <c r="L2">
-        <v>17.195024418337667</v>
+        <v>15.915711310122166</v>
       </c>
       <c r="M2">
-        <v>0.5712931303885227</v>
+        <v>0.5396326840207543</v>
       </c>
       <c r="N2" t="str">
         <v/>
       </c>
       <c r="O2">
-        <v>7.215784728582721</v>
+        <v>7.635998111301148</v>
       </c>
       <c r="P2">
-        <v>3.8434241681596375</v>
+        <v>3.8784418493370074</v>
       </c>
       <c r="Q2">
-        <v>12.5269323938524</v>
+        <v>12.365960909623045</v>
       </c>
       <c r="R2">
-        <v>0.5243591589440632</v>
+        <v>0.5101097837002457</v>
       </c>
     </row>
     <row r="3">
@@ -529,46 +529,46 @@
         <v/>
       </c>
       <c r="E3">
-        <v>9.021427508378059</v>
+        <v>8.881976679506145</v>
       </c>
       <c r="F3">
-        <v>4.721142925296914</v>
+        <v>5.096826099790759</v>
       </c>
       <c r="G3">
-        <v>18.018818282240073</v>
+        <v>18.021003610426416</v>
       </c>
       <c r="H3">
-        <v>0.5850956161117566</v>
+        <v>0.5935862898771422</v>
       </c>
       <c r="I3" t="str">
         <v/>
       </c>
       <c r="J3">
-        <v>9.199169116588298</v>
+        <v>8.132007452878128</v>
       </c>
       <c r="K3">
-        <v>4.485906147583037</v>
+        <v>4.710474877508848</v>
       </c>
       <c r="L3">
-        <v>16.243945941412385</v>
+        <v>15.81302367919253</v>
       </c>
       <c r="M3">
-        <v>0.5855275642134534</v>
+        <v>0.5086228356615505</v>
       </c>
       <c r="N3" t="str">
         <v/>
       </c>
       <c r="O3">
-        <v>6.72030526356007</v>
+        <v>7.570248217895283</v>
       </c>
       <c r="P3">
-        <v>3.3850682177305784</v>
+        <v>3.687352753792666</v>
       </c>
       <c r="Q3">
-        <v>13.0871562208356</v>
+        <v>13.301607622400496</v>
       </c>
       <c r="R3">
-        <v>0.5730914579456682</v>
+        <v>0.4921138130260491</v>
       </c>
     </row>
     <row r="4">
@@ -585,46 +585,46 @@
         <v/>
       </c>
       <c r="E4">
-        <v>10.331185978188044</v>
+        <v>9.54402311863312</v>
       </c>
       <c r="F4">
-        <v>4.459561690630157</v>
+        <v>4.442814379062537</v>
       </c>
       <c r="G4">
-        <v>17.933980145549153</v>
+        <v>16.11082866909953</v>
       </c>
       <c r="H4">
-        <v>0.5831365881533761</v>
+        <v>0.5143677605090159</v>
       </c>
       <c r="I4" t="str">
         <v/>
       </c>
       <c r="J4">
-        <v>8.8965687504212</v>
+        <v>9.06702678904676</v>
       </c>
       <c r="K4">
-        <v>4.155395186092768</v>
+        <v>4.473103914188908</v>
       </c>
       <c r="L4">
-        <v>16.546056075265536</v>
+        <v>15.513979887096045</v>
       </c>
       <c r="M4">
-        <v>0.520370219078963</v>
+        <v>0.5376438732558</v>
       </c>
       <c r="N4" t="str">
         <v/>
       </c>
       <c r="O4">
-        <v>7.762800671931718</v>
+        <v>7.027579971452461</v>
       </c>
       <c r="P4">
-        <v>3.6150497551706975</v>
+        <v>3.8954912176166747</v>
       </c>
       <c r="Q4">
-        <v>12.70870448456691</v>
+        <v>12.151227071482356</v>
       </c>
       <c r="R4">
-        <v>0.4800381217881781</v>
+        <v>0.5686818076117262</v>
       </c>
     </row>
     <row r="5">
@@ -641,46 +641,46 @@
         <v/>
       </c>
       <c r="E5">
-        <v>9.26716781201302</v>
+        <v>10.197742271205428</v>
       </c>
       <c r="F5">
-        <v>4.990035802910194</v>
+        <v>4.48280776095761</v>
       </c>
       <c r="G5">
-        <v>17.300639532542895</v>
+        <v>17.231068231476435</v>
       </c>
       <c r="H5">
-        <v>0.5137662463204309</v>
+        <v>0.5577103768995016</v>
       </c>
       <c r="I5" t="str">
         <v/>
       </c>
       <c r="J5">
-        <v>8.110483363627567</v>
+        <v>8.18462858111702</v>
       </c>
       <c r="K5">
-        <v>4.160986241657172</v>
+        <v>4.268772982097925</v>
       </c>
       <c r="L5">
-        <v>15.434312169777124</v>
+        <v>15.285068797459298</v>
       </c>
       <c r="M5">
-        <v>0.5541284940344335</v>
+        <v>0.5338370960177631</v>
       </c>
       <c r="N5" t="str">
         <v/>
       </c>
       <c r="O5">
-        <v>7.929803068162862</v>
+        <v>6.9159688177660446</v>
       </c>
       <c r="P5">
-        <v>3.540416454059512</v>
+        <v>3.8711647868173404</v>
       </c>
       <c r="Q5">
-        <v>13.321576204918564</v>
+        <v>13.56057052828054</v>
       </c>
       <c r="R5">
-        <v>0.48172294047605124</v>
+        <v>0.5713048955723024</v>
       </c>
     </row>
     <row r="6">
@@ -697,46 +697,46 @@
         <v/>
       </c>
       <c r="E6">
-        <v>9.635629718477125</v>
+        <v>9.79094259978337</v>
       </c>
       <c r="F6">
-        <v>4.981454725759133</v>
+        <v>5.081617269103159</v>
       </c>
       <c r="G6">
-        <v>17.39313301744866</v>
+        <v>18.010812065097834</v>
       </c>
       <c r="H6">
-        <v>0.5155042206040699</v>
+        <v>0.5340949804719686</v>
       </c>
       <c r="I6" t="str">
         <v/>
       </c>
       <c r="J6">
-        <v>9.501131667517399</v>
+        <v>7.872970310729137</v>
       </c>
       <c r="K6">
-        <v>4.042412883453536</v>
+        <v>4.336477088201533</v>
       </c>
       <c r="L6">
-        <v>16.001660682391837</v>
+        <v>16.924309856414</v>
       </c>
       <c r="M6">
-        <v>0.5384286454076778</v>
+        <v>0.532738173826799</v>
       </c>
       <c r="N6" t="str">
         <v/>
       </c>
       <c r="O6">
-        <v>6.949479815887563</v>
+        <v>6.518215542731838</v>
       </c>
       <c r="P6">
-        <v>3.456701221097033</v>
+        <v>3.3304672508688635</v>
       </c>
       <c r="Q6">
-        <v>12.167429497651245</v>
+        <v>12.363989096272617</v>
       </c>
       <c r="R6">
-        <v>0.5381141567504131</v>
+        <v>0.48883777226223607</v>
       </c>
     </row>
     <row r="7">
@@ -753,46 +753,46 @@
         <v/>
       </c>
       <c r="E7">
-        <v>8.523279098550958</v>
+        <v>10.194116088834194</v>
       </c>
       <c r="F7">
-        <v>4.429184707897594</v>
+        <v>4.736965403330786</v>
       </c>
       <c r="G7">
-        <v>18.014107275488247</v>
+        <v>16.301422758772585</v>
       </c>
       <c r="H7">
-        <v>0.5792445900601628</v>
+        <v>0.5398276204846395</v>
       </c>
       <c r="I7" t="str">
         <v/>
       </c>
       <c r="J7">
-        <v>8.0791107580912</v>
+        <v>9.528315857669007</v>
       </c>
       <c r="K7">
-        <v>4.340283163971477</v>
+        <v>4.429305461282567</v>
       </c>
       <c r="L7">
-        <v>17.071711191355895</v>
+        <v>17.095573295754445</v>
       </c>
       <c r="M7">
-        <v>0.5454932483097441</v>
+        <v>0.5612503047318183</v>
       </c>
       <c r="N7" t="str">
         <v/>
       </c>
       <c r="O7">
-        <v>6.990491306079681</v>
+        <v>7.317304279458927</v>
       </c>
       <c r="P7">
-        <v>3.670183114638906</v>
+        <v>3.2068443533653794</v>
       </c>
       <c r="Q7">
-        <v>12.983901832930773</v>
+        <v>12.435066858949668</v>
       </c>
       <c r="R7">
-        <v>0.504554422425871</v>
+        <v>0.5114050724486651</v>
       </c>
     </row>
     <row r="8">
@@ -809,46 +809,46 @@
         <v/>
       </c>
       <c r="E8">
-        <v>10.260165521223602</v>
+        <v>8.939499215264243</v>
       </c>
       <c r="F8">
-        <v>4.609427966585642</v>
+        <v>4.821389861785144</v>
       </c>
       <c r="G8">
-        <v>16.638418484356936</v>
+        <v>18.020685606585502</v>
       </c>
       <c r="H8">
-        <v>0.5410974892349376</v>
+        <v>0.5613330002774817</v>
       </c>
       <c r="I8" t="str">
         <v/>
       </c>
       <c r="J8">
-        <v>8.71463359520235</v>
+        <v>8.077296136731643</v>
       </c>
       <c r="K8">
-        <v>4.24026662038497</v>
+        <v>4.355132817381211</v>
       </c>
       <c r="L8">
-        <v>17.18808690574038</v>
+        <v>16.123171551751504</v>
       </c>
       <c r="M8">
-        <v>0.5340243226391459</v>
+        <v>0.5713544848434626</v>
       </c>
       <c r="N8" t="str">
         <v/>
       </c>
       <c r="O8">
-        <v>6.956658022813552</v>
+        <v>6.753526965039562</v>
       </c>
       <c r="P8">
-        <v>3.2195789557408774</v>
+        <v>3.6667216712042427</v>
       </c>
       <c r="Q8">
-        <v>12.294391563422126</v>
+        <v>12.173787158267409</v>
       </c>
       <c r="R8">
-        <v>0.5436675062392442</v>
+        <v>0.5067615302138856</v>
       </c>
     </row>
     <row r="9">
@@ -865,46 +865,46 @@
         <v/>
       </c>
       <c r="E9">
-        <v>8.704475069405008</v>
+        <v>10.342881116979747</v>
       </c>
       <c r="F9">
-        <v>4.211941401229401</v>
+        <v>4.420858287029077</v>
       </c>
       <c r="G9">
-        <v>17.539615638373505</v>
+        <v>16.553228452630897</v>
       </c>
       <c r="H9">
-        <v>0.586965541816998</v>
+        <v>0.5174544951950707</v>
       </c>
       <c r="I9" t="str">
         <v/>
       </c>
       <c r="J9">
-        <v>8.102323401288338</v>
+        <v>8.303209671721357</v>
       </c>
       <c r="K9">
-        <v>4.552976676461911</v>
+        <v>4.307335760306129</v>
       </c>
       <c r="L9">
-        <v>15.722348108963333</v>
+        <v>16.611832001616765</v>
       </c>
       <c r="M9">
-        <v>0.5265336742463005</v>
+        <v>0.5685344730127614</v>
       </c>
       <c r="N9" t="str">
         <v/>
       </c>
       <c r="O9">
-        <v>7.43186923884161</v>
+        <v>7.949198700673985</v>
       </c>
       <c r="P9">
-        <v>3.946879976078715</v>
+        <v>3.4703579339599457</v>
       </c>
       <c r="Q9">
-        <v>12.579151451363227</v>
+        <v>13.567678014891918</v>
       </c>
       <c r="R9">
-        <v>0.5680009576470995</v>
+        <v>0.5556699136136738</v>
       </c>
     </row>
     <row r="10">
@@ -921,46 +921,46 @@
         <v/>
       </c>
       <c r="E10">
-        <v>8.727015656887458</v>
+        <v>9.837248460295834</v>
       </c>
       <c r="F10">
-        <v>4.7339806624472</v>
+        <v>4.867396038901182</v>
       </c>
       <c r="G10">
-        <v>17.80321018970091</v>
+        <v>18.00864132879815</v>
       </c>
       <c r="H10">
-        <v>0.5033809226980677</v>
+        <v>0.5694647423574528</v>
       </c>
       <c r="I10" t="str">
         <v/>
       </c>
       <c r="J10">
-        <v>9.081591525934964</v>
+        <v>8.920250175700836</v>
       </c>
       <c r="K10">
-        <v>4.337030167926278</v>
+        <v>4.68225397642</v>
       </c>
       <c r="L10">
-        <v>16.04284678104461</v>
+        <v>16.71068318493939</v>
       </c>
       <c r="M10">
-        <v>0.5490931364924643</v>
+        <v>0.580518283035966</v>
       </c>
       <c r="N10" t="str">
         <v/>
       </c>
       <c r="O10">
-        <v>7.471371891944919</v>
+        <v>7.949757007091181</v>
       </c>
       <c r="P10">
-        <v>3.5234354339531384</v>
+        <v>3.4938054378411194</v>
       </c>
       <c r="Q10">
-        <v>13.25580589136259</v>
+        <v>12.374382209219664</v>
       </c>
       <c r="R10">
-        <v>0.5081839718155982</v>
+        <v>0.5620532040134144</v>
       </c>
     </row>
     <row r="11">
@@ -977,46 +977,46 @@
         <v/>
       </c>
       <c r="E11">
-        <v>9.766088529869153</v>
+        <v>10.0333083203245</v>
       </c>
       <c r="F11">
-        <v>5.057938312707524</v>
+        <v>4.364016872499079</v>
       </c>
       <c r="G11">
-        <v>17.861333131106</v>
+        <v>17.826664350125487</v>
       </c>
       <c r="H11">
-        <v>0.5013179925061837</v>
+        <v>0.5013524647584686</v>
       </c>
       <c r="I11" t="str">
         <v/>
       </c>
       <c r="J11">
-        <v>9.062643877135798</v>
+        <v>8.018410675885042</v>
       </c>
       <c r="K11">
-        <v>4.626951729899622</v>
+        <v>4.042041592331923</v>
       </c>
       <c r="L11">
-        <v>15.807971987068054</v>
+        <v>15.285673620340262</v>
       </c>
       <c r="M11">
-        <v>0.5305864544295144</v>
+        <v>0.5571736779326993</v>
       </c>
       <c r="N11" t="str">
         <v/>
       </c>
       <c r="O11">
-        <v>7.308857076042441</v>
+        <v>6.604005281411325</v>
       </c>
       <c r="P11">
-        <v>3.90608797525047</v>
+        <v>3.223704599454152</v>
       </c>
       <c r="Q11">
-        <v>13.054405925079346</v>
+        <v>13.513337094273476</v>
       </c>
       <c r="R11">
-        <v>0.5595371715236351</v>
+        <v>0.5192341562925644</v>
       </c>
     </row>
     <row r="12">
@@ -1033,46 +1033,46 @@
         <v/>
       </c>
       <c r="E12">
-        <v>8.518476109145963</v>
+        <v>9.187997532389485</v>
       </c>
       <c r="F12">
-        <v>4.795990457256729</v>
+        <v>4.267861458867716</v>
       </c>
       <c r="G12">
-        <v>16.624422610119282</v>
+        <v>18.060920024373452</v>
       </c>
       <c r="H12">
-        <v>0.5330472297579346</v>
+        <v>0.5280341586280326</v>
       </c>
       <c r="I12" t="str">
         <v/>
       </c>
       <c r="J12">
-        <v>9.488923313832602</v>
+        <v>8.125250287171138</v>
       </c>
       <c r="K12">
-        <v>4.6525147553897</v>
+        <v>4.130131069453505</v>
       </c>
       <c r="L12">
-        <v>15.807441027920712</v>
+        <v>16.219926206925148</v>
       </c>
       <c r="M12">
-        <v>0.5285763637556574</v>
+        <v>0.4914712540260468</v>
       </c>
       <c r="N12" t="str">
         <v/>
       </c>
       <c r="O12">
-        <v>7.455280604343574</v>
+        <v>7.024067904499752</v>
       </c>
       <c r="P12">
-        <v>3.223150577291657</v>
+        <v>3.770997511181889</v>
       </c>
       <c r="Q12">
-        <v>13.355947490846267</v>
+        <v>12.754349834000937</v>
       </c>
       <c r="R12">
-        <v>0.49360106411751714</v>
+        <v>0.5345744457575683</v>
       </c>
     </row>
     <row r="13">
@@ -1089,46 +1089,46 @@
         <v/>
       </c>
       <c r="E13">
-        <v>8.786616280817112</v>
+        <v>8.587445958663187</v>
       </c>
       <c r="F13">
-        <v>4.393109418763677</v>
+        <v>5.055690521905313</v>
       </c>
       <c r="G13">
-        <v>17.791984367857726</v>
+        <v>16.34833841618239</v>
       </c>
       <c r="H13">
-        <v>0.5219560959274976</v>
+        <v>0.5522648364791506</v>
       </c>
       <c r="I13" t="str">
         <v/>
       </c>
       <c r="J13">
-        <v>7.847892308353563</v>
+        <v>8.395012864261343</v>
       </c>
       <c r="K13">
-        <v>4.834426524274363</v>
+        <v>4.802020714739774</v>
       </c>
       <c r="L13">
-        <v>16.952185114950986</v>
+        <v>17.155577925384204</v>
       </c>
       <c r="M13">
-        <v>0.563934777928829</v>
+        <v>0.49452771294766495</v>
       </c>
       <c r="N13" t="str">
         <v/>
       </c>
       <c r="O13">
-        <v>6.862860032080204</v>
+        <v>7.805783781537004</v>
       </c>
       <c r="P13">
-        <v>3.2472299157484423</v>
+        <v>3.8017567715641736</v>
       </c>
       <c r="Q13">
-        <v>12.161797956341502</v>
+        <v>12.960991516598671</v>
       </c>
       <c r="R13">
-        <v>0.5685532129157272</v>
+        <v>0.5360845239984741</v>
       </c>
     </row>
     <row r="14">
@@ -1145,46 +1145,46 @@
         <v/>
       </c>
       <c r="E14">
-        <v>9.736096492043906</v>
+        <v>8.86547260325833</v>
       </c>
       <c r="F14">
-        <v>4.961772006533763</v>
+        <v>4.943758573755068</v>
       </c>
       <c r="G14">
-        <v>17.04439915367243</v>
+        <v>17.440073163762843</v>
       </c>
       <c r="H14">
-        <v>0.5091411551707192</v>
+        <v>0.5861469124167833</v>
       </c>
       <c r="I14" t="str">
         <v/>
       </c>
       <c r="J14">
-        <v>8.165512431881233</v>
+        <v>9.205731384531518</v>
       </c>
       <c r="K14">
-        <v>4.30281049846301</v>
+        <v>4.177115602786635</v>
       </c>
       <c r="L14">
-        <v>15.319701451177409</v>
+        <v>15.404941257041193</v>
       </c>
       <c r="M14">
-        <v>0.5074883635965547</v>
+        <v>0.5806198111927044</v>
       </c>
       <c r="N14" t="str">
         <v/>
       </c>
       <c r="O14">
-        <v>7.951257615506269</v>
+        <v>6.6860215457636905</v>
       </c>
       <c r="P14">
-        <v>3.44591470578815</v>
+        <v>3.847460195207458</v>
       </c>
       <c r="Q14">
-        <v>13.460834535998883</v>
+        <v>13.103910508778466</v>
       </c>
       <c r="R14">
-        <v>0.5401941971381369</v>
+        <v>0.5139483046238648</v>
       </c>
     </row>
     <row r="15">
@@ -1201,46 +1201,46 @@
         <v/>
       </c>
       <c r="E15">
-        <v>9.920196004153132</v>
+        <v>10.072024632731829</v>
       </c>
       <c r="F15">
-        <v>4.746835260548218</v>
+        <v>4.650685134477794</v>
       </c>
       <c r="G15">
-        <v>17.967488579112835</v>
+        <v>16.942989163237904</v>
       </c>
       <c r="H15">
-        <v>0.5049424220028601</v>
+        <v>0.591352378640242</v>
       </c>
       <c r="I15" t="str">
         <v/>
       </c>
       <c r="J15">
-        <v>8.765444706602477</v>
+        <v>8.986602135979986</v>
       </c>
       <c r="K15">
-        <v>4.081631249048172</v>
+        <v>4.389775897643873</v>
       </c>
       <c r="L15">
-        <v>16.204272421265436</v>
+        <v>16.611161033567534</v>
       </c>
       <c r="M15">
-        <v>0.5114883518387647</v>
+        <v>0.5185586059496093</v>
       </c>
       <c r="N15" t="str">
         <v/>
       </c>
       <c r="O15">
-        <v>7.162937601103474</v>
+        <v>7.374141110509665</v>
       </c>
       <c r="P15">
-        <v>3.621212745060849</v>
+        <v>3.3450459429435915</v>
       </c>
       <c r="Q15">
-        <v>13.487420375233139</v>
+        <v>12.317410317416945</v>
       </c>
       <c r="R15">
-        <v>0.5272023019025703</v>
+        <v>0.5421913382909656</v>
       </c>
     </row>
     <row r="16">
@@ -1257,46 +1257,46 @@
         <v/>
       </c>
       <c r="E16">
-        <v>9.4272663320269</v>
+        <v>8.806021836603096</v>
       </c>
       <c r="F16">
-        <v>4.743809952827472</v>
+        <v>4.709417084263038</v>
       </c>
       <c r="G16">
-        <v>16.371733253553316</v>
+        <v>16.298980506723996</v>
       </c>
       <c r="H16">
-        <v>0.5738404760587019</v>
+        <v>0.5920802764901839</v>
       </c>
       <c r="I16" t="str">
         <v/>
       </c>
       <c r="J16">
-        <v>9.405171042226387</v>
+        <v>8.18281745068473</v>
       </c>
       <c r="K16">
-        <v>4.445162079829676</v>
+        <v>3.9297701196522947</v>
       </c>
       <c r="L16">
-        <v>16.805162750508853</v>
+        <v>16.501206007668415</v>
       </c>
       <c r="M16">
-        <v>0.5791132907409307</v>
+        <v>0.5600751074805936</v>
       </c>
       <c r="N16" t="str">
         <v/>
       </c>
       <c r="O16">
-        <v>6.659251188725008</v>
+        <v>7.283845286945162</v>
       </c>
       <c r="P16">
-        <v>3.2519278465087242</v>
+        <v>3.584846716194323</v>
       </c>
       <c r="Q16">
-        <v>13.532925641005633</v>
+        <v>12.67335161363835</v>
       </c>
       <c r="R16">
-        <v>0.5312890267819108</v>
+        <v>0.5052221268800259</v>
       </c>
     </row>
     <row r="17">
@@ -1313,46 +1313,46 @@
         <v/>
       </c>
       <c r="E17">
-        <v>10.192454739837098</v>
+        <v>9.899588959692268</v>
       </c>
       <c r="F17">
-        <v>4.56424351056053</v>
+        <v>4.795351984660146</v>
       </c>
       <c r="G17">
-        <v>17.94921918174313</v>
+        <v>17.978802503640313</v>
       </c>
       <c r="H17">
-        <v>0.5071965174691637</v>
+        <v>0.5122458513500773</v>
       </c>
       <c r="I17" t="str">
         <v/>
       </c>
       <c r="J17">
-        <v>9.264866464374501</v>
+        <v>7.841043499853786</v>
       </c>
       <c r="K17">
-        <v>4.878954234830068</v>
+        <v>4.110194729193563</v>
       </c>
       <c r="L17">
-        <v>16.415139831029137</v>
+        <v>16.118809001407385</v>
       </c>
       <c r="M17">
-        <v>0.5142667004019161</v>
+        <v>0.5383236221541379</v>
       </c>
       <c r="N17" t="str">
         <v/>
       </c>
       <c r="O17">
-        <v>7.076772352661766</v>
+        <v>7.167506068784217</v>
       </c>
       <c r="P17">
-        <v>3.4446857520327923</v>
+        <v>3.975164503726287</v>
       </c>
       <c r="Q17">
-        <v>13.517006707259617</v>
+        <v>13.014436951719828</v>
       </c>
       <c r="R17">
-        <v>0.5347142410433523</v>
+        <v>0.5160830690832596</v>
       </c>
     </row>
     <row r="18">
@@ -1369,46 +1369,46 @@
         <v/>
       </c>
       <c r="E18">
-        <v>10.348216717061687</v>
+        <v>9.966425239610707</v>
       </c>
       <c r="F18">
-        <v>4.84466767437556</v>
+        <v>4.734033836455168</v>
       </c>
       <c r="G18">
-        <v>17.977897912419895</v>
+        <v>17.17269066039714</v>
       </c>
       <c r="H18">
-        <v>0.5282022370674334</v>
+        <v>0.5799750900492464</v>
       </c>
       <c r="I18" t="str">
         <v/>
       </c>
       <c r="J18">
-        <v>9.110110360258552</v>
+        <v>8.290074510960608</v>
       </c>
       <c r="K18">
-        <v>4.602467126931376</v>
+        <v>3.9231220684610317</v>
       </c>
       <c r="L18">
-        <v>15.898749137190219</v>
+        <v>17.057557258182666</v>
       </c>
       <c r="M18">
-        <v>0.5777822761476561</v>
+        <v>0.5557191067968404</v>
       </c>
       <c r="N18" t="str">
         <v/>
       </c>
       <c r="O18">
-        <v>7.327396966277919</v>
+        <v>7.9523279719127435</v>
       </c>
       <c r="P18">
-        <v>3.9204844038982376</v>
+        <v>3.6878895536054626</v>
       </c>
       <c r="Q18">
-        <v>13.390701994661589</v>
+        <v>12.478377289035137</v>
       </c>
       <c r="R18">
-        <v>0.5563653513843357</v>
+        <v>0.5282393342976428</v>
       </c>
     </row>
     <row r="19">
@@ -1425,46 +1425,46 @@
         <v/>
       </c>
       <c r="E19">
-        <v>9.88764445358243</v>
+        <v>9.767619752954257</v>
       </c>
       <c r="F19">
-        <v>4.9767221574756935</v>
+        <v>4.817905530642235</v>
       </c>
       <c r="G19">
-        <v>17.931938890004787</v>
+        <v>17.062614841150683</v>
       </c>
       <c r="H19">
-        <v>0.5031410949597788</v>
+        <v>0.5144433350244292</v>
       </c>
       <c r="I19" t="str">
         <v/>
       </c>
       <c r="J19">
-        <v>8.189906365069577</v>
+        <v>7.942162634049533</v>
       </c>
       <c r="K19">
-        <v>4.056276592001384</v>
+        <v>4.6477044508021</v>
       </c>
       <c r="L19">
-        <v>16.038714944849065</v>
+        <v>15.255397669133503</v>
       </c>
       <c r="M19">
-        <v>0.5545015704571298</v>
+        <v>0.5282667404382885</v>
       </c>
       <c r="N19" t="str">
         <v/>
       </c>
       <c r="O19">
-        <v>7.872152711555697</v>
+        <v>7.052777031933765</v>
       </c>
       <c r="P19">
-        <v>3.763063142867747</v>
+        <v>3.725657901011739</v>
       </c>
       <c r="Q19">
-        <v>13.113941696177918</v>
+        <v>12.568333493145236</v>
       </c>
       <c r="R19">
-        <v>0.5496911414759924</v>
+        <v>0.5374411327406361</v>
       </c>
     </row>
     <row r="20">
@@ -1481,46 +1481,46 @@
         <v/>
       </c>
       <c r="E20">
-        <v>10.341474999522642</v>
+        <v>8.925658444505702</v>
       </c>
       <c r="F20">
-        <v>4.876902050423262</v>
+        <v>4.225950031274283</v>
       </c>
       <c r="G20">
-        <v>17.672990551284908</v>
+        <v>16.36875235393963</v>
       </c>
       <c r="H20">
-        <v>0.5599507211430685</v>
+        <v>0.5425329361170296</v>
       </c>
       <c r="I20" t="str">
         <v/>
       </c>
       <c r="J20">
-        <v>9.384902669247467</v>
+        <v>9.192695662361434</v>
       </c>
       <c r="K20">
-        <v>4.007853207844923</v>
+        <v>4.126908671072094</v>
       </c>
       <c r="L20">
-        <v>16.163423648919334</v>
+        <v>15.244402969985824</v>
       </c>
       <c r="M20">
-        <v>0.5646791467013693</v>
+        <v>0.575423885522899</v>
       </c>
       <c r="N20" t="str">
         <v/>
       </c>
       <c r="O20">
-        <v>6.916875632956135</v>
+        <v>6.711198564880504</v>
       </c>
       <c r="P20">
-        <v>3.9610661549535324</v>
+        <v>3.976839449330586</v>
       </c>
       <c r="Q20">
-        <v>12.601352765536943</v>
+        <v>13.162614216781874</v>
       </c>
       <c r="R20">
-        <v>0.5384041142648961</v>
+        <v>0.5708011275226565</v>
       </c>
     </row>
     <row r="21">
@@ -1537,46 +1537,46 @@
         <v/>
       </c>
       <c r="E21">
-        <v>9.914329637873257</v>
+        <v>10.229734778691213</v>
       </c>
       <c r="F21">
-        <v>4.224855631795792</v>
+        <v>4.285686460593996</v>
       </c>
       <c r="G21">
-        <v>16.748959607138563</v>
+        <v>17.723664862812278</v>
       </c>
       <c r="H21">
-        <v>0.5642864697552844</v>
+        <v>0.5608648450077026</v>
       </c>
       <c r="I21" t="str">
         <v/>
       </c>
       <c r="J21">
-        <v>8.020031004087532</v>
+        <v>8.652225118381267</v>
       </c>
       <c r="K21">
-        <v>4.621891284204932</v>
+        <v>4.6719501496088265</v>
       </c>
       <c r="L21">
-        <v>16.81064324789179</v>
+        <v>16.046732561399676</v>
       </c>
       <c r="M21">
-        <v>0.5215280455314364</v>
+        <v>0.5832737979675064</v>
       </c>
       <c r="N21" t="str">
         <v/>
       </c>
       <c r="O21">
-        <v>7.846337941021252</v>
+        <v>7.67454528074467</v>
       </c>
       <c r="P21">
-        <v>3.891245022513334</v>
+        <v>3.6133592258981495</v>
       </c>
       <c r="Q21">
-        <v>12.357609559465631</v>
+        <v>13.499259383082117</v>
       </c>
       <c r="R21">
-        <v>0.5418332673123627</v>
+        <v>0.5133668023296021</v>
       </c>
     </row>
     <row r="22">
@@ -1593,46 +1593,46 @@
         <v/>
       </c>
       <c r="E22">
-        <v>8.819590953484965</v>
+        <v>10.253231134077996</v>
       </c>
       <c r="F22">
-        <v>4.582573824061802</v>
+        <v>4.2182336204016675</v>
       </c>
       <c r="G22">
-        <v>17.932163724686145</v>
+        <v>16.71533228494345</v>
       </c>
       <c r="H22">
-        <v>0.5265823222450684</v>
+        <v>0.5423395055365258</v>
       </c>
       <c r="I22" t="str">
         <v/>
       </c>
       <c r="J22">
-        <v>9.799337033727829</v>
+        <v>8.51732198581433</v>
       </c>
       <c r="K22">
-        <v>4.223842872402985</v>
+        <v>3.9841177861331003</v>
       </c>
       <c r="L22">
-        <v>16.91883760491464</v>
+        <v>15.791723924401571</v>
       </c>
       <c r="M22">
-        <v>0.5856492123298507</v>
+        <v>0.5490668771887272</v>
       </c>
       <c r="N22" t="str">
         <v/>
       </c>
       <c r="O22">
-        <v>7.861374274270635</v>
+        <v>7.481695916739408</v>
       </c>
       <c r="P22">
-        <v>3.958920472233506</v>
+        <v>3.2262380811758216</v>
       </c>
       <c r="Q22">
-        <v>13.252374422734977</v>
+        <v>13.123273290111456</v>
       </c>
       <c r="R22">
-        <v>0.5717708142006083</v>
+        <v>0.5448441315057434</v>
       </c>
     </row>
     <row r="23">
@@ -1649,46 +1649,46 @@
         <v/>
       </c>
       <c r="E23">
-        <v>10.314728206067208</v>
+        <v>9.38507401376092</v>
       </c>
       <c r="F23">
-        <v>4.374611232281187</v>
+        <v>4.598605429220312</v>
       </c>
       <c r="G23">
-        <v>16.556305264095226</v>
+        <v>16.715140283472934</v>
       </c>
       <c r="H23">
-        <v>0.5757212142932612</v>
+        <v>0.5199875725253049</v>
       </c>
       <c r="I23" t="str">
         <v/>
       </c>
       <c r="J23">
-        <v>7.857873410981266</v>
+        <v>9.101607957905323</v>
       </c>
       <c r="K23">
-        <v>4.278985905594484</v>
+        <v>4.732781244841226</v>
       </c>
       <c r="L23">
-        <v>16.873762962515688</v>
+        <v>15.759689570254274</v>
       </c>
       <c r="M23">
-        <v>0.5861474448958244</v>
+        <v>0.5442213093658559</v>
       </c>
       <c r="N23" t="str">
         <v/>
       </c>
       <c r="O23">
-        <v>7.08192800216289</v>
+        <v>7.476137117455097</v>
       </c>
       <c r="P23">
-        <v>3.9230527349104833</v>
+        <v>3.4466018090954442</v>
       </c>
       <c r="Q23">
-        <v>13.427721429055286</v>
+        <v>12.470594532675975</v>
       </c>
       <c r="R23">
-        <v>0.5007872055846412</v>
+        <v>0.5616405132954619</v>
       </c>
     </row>
     <row r="24">
@@ -1705,46 +1705,46 @@
         <v/>
       </c>
       <c r="E24">
-        <v>8.722558926626204</v>
+        <v>8.667315716544277</v>
       </c>
       <c r="F24">
-        <v>5.029594730013132</v>
+        <v>4.68499795503043</v>
       </c>
       <c r="G24">
-        <v>16.176942862730815</v>
+        <v>17.36607246259243</v>
       </c>
       <c r="H24">
-        <v>0.5911244655490299</v>
+        <v>0.5216818203057187</v>
       </c>
       <c r="I24" t="str">
         <v/>
       </c>
       <c r="J24">
-        <v>7.853412890324982</v>
+        <v>9.050753214201395</v>
       </c>
       <c r="K24">
-        <v>4.530591429303258</v>
+        <v>4.647335095323891</v>
       </c>
       <c r="L24">
-        <v>15.284741038622553</v>
+        <v>15.486134537229226</v>
       </c>
       <c r="M24">
-        <v>0.5187190185022423</v>
+        <v>0.5454943214115809</v>
       </c>
       <c r="N24" t="str">
         <v/>
       </c>
       <c r="O24">
-        <v>6.864865450022789</v>
+        <v>7.9871689096325955</v>
       </c>
       <c r="P24">
-        <v>3.4414904812447316</v>
+        <v>3.3791809359698037</v>
       </c>
       <c r="Q24">
-        <v>12.989595549192359</v>
+        <v>13.570077319877887</v>
       </c>
       <c r="R24">
-        <v>0.5441828000013165</v>
+        <v>0.573541612325708</v>
       </c>
     </row>
     <row r="25">
@@ -1761,46 +1761,46 @@
         <v/>
       </c>
       <c r="E25">
-        <v>8.91040993396602</v>
+        <v>10.217945052741289</v>
       </c>
       <c r="F25">
-        <v>4.30989958648258</v>
+        <v>4.462924369362575</v>
       </c>
       <c r="G25">
-        <v>17.16387487103041</v>
+        <v>18.09883351423739</v>
       </c>
       <c r="H25">
-        <v>0.5082731187872878</v>
+        <v>0.5066200813460591</v>
       </c>
       <c r="I25" t="str">
         <v/>
       </c>
       <c r="J25">
-        <v>8.75419404575516</v>
+        <v>9.691835716598794</v>
       </c>
       <c r="K25">
-        <v>4.138894977677489</v>
+        <v>4.138508924775939</v>
       </c>
       <c r="L25">
-        <v>16.888741593751554</v>
+        <v>16.0689519465586</v>
       </c>
       <c r="M25">
-        <v>0.49978984814414246</v>
+        <v>0.5061920128049211</v>
       </c>
       <c r="N25" t="str">
         <v/>
       </c>
       <c r="O25">
-        <v>7.814078413921103</v>
+        <v>7.381367232743108</v>
       </c>
       <c r="P25">
-        <v>3.600102183692865</v>
+        <v>3.5402760341693202</v>
       </c>
       <c r="Q25">
-        <v>13.55187358711099</v>
+        <v>13.439786848608348</v>
       </c>
       <c r="R25">
-        <v>0.52986779728941</v>
+        <v>0.5134422334023999</v>
       </c>
     </row>
     <row r="26">
@@ -1817,46 +1817,46 @@
         <v/>
       </c>
       <c r="E26">
-        <v>8.557999267289432</v>
+        <v>9.996783985415663</v>
       </c>
       <c r="F26">
-        <v>4.375099054392716</v>
+        <v>4.563395895368483</v>
       </c>
       <c r="G26">
-        <v>16.16298187718517</v>
+        <v>16.45110755113595</v>
       </c>
       <c r="H26">
-        <v>0.5320079142773738</v>
+        <v>0.546256149169632</v>
       </c>
       <c r="I26" t="str">
         <v/>
       </c>
       <c r="J26">
-        <v>9.424309917992625</v>
+        <v>8.771109426427639</v>
       </c>
       <c r="K26">
-        <v>4.376384986158828</v>
+        <v>4.069571176779293</v>
       </c>
       <c r="L26">
-        <v>16.905578666460542</v>
+        <v>16.974704147181168</v>
       </c>
       <c r="M26">
-        <v>0.5670963478356338</v>
+        <v>0.5875892805299717</v>
       </c>
       <c r="N26" t="str">
         <v/>
       </c>
       <c r="O26">
-        <v>7.747350537163991</v>
+        <v>7.059599150079948</v>
       </c>
       <c r="P26">
-        <v>3.8620793113045595</v>
+        <v>3.3821838006747553</v>
       </c>
       <c r="Q26">
-        <v>12.849500657084944</v>
+        <v>12.792298009005684</v>
       </c>
       <c r="R26">
-        <v>0.5210100074855343</v>
+        <v>0.5402210502258178</v>
       </c>
     </row>
     <row r="27">
@@ -1873,46 +1873,46 @@
         <v/>
       </c>
       <c r="E27">
-        <v>9.535234827158657</v>
+        <v>10.036604203878682</v>
       </c>
       <c r="F27">
-        <v>4.221832336628857</v>
+        <v>4.461783255964593</v>
       </c>
       <c r="G27">
-        <v>17.655397814151904</v>
+        <v>17.50944509558804</v>
       </c>
       <c r="H27">
-        <v>0.5662638237298345</v>
+        <v>0.5440585914837007</v>
       </c>
       <c r="I27" t="str">
         <v/>
       </c>
       <c r="J27">
-        <v>8.141075484748296</v>
+        <v>9.23242894483856</v>
       </c>
       <c r="K27">
-        <v>4.113961447029932</v>
+        <v>4.524065678714591</v>
       </c>
       <c r="L27">
-        <v>16.32280096379093</v>
+        <v>16.004302765436215</v>
       </c>
       <c r="M27">
-        <v>0.49126284036270873</v>
+        <v>0.5198961008770517</v>
       </c>
       <c r="N27" t="str">
         <v/>
       </c>
       <c r="O27">
-        <v>6.875825369258055</v>
+        <v>7.3431532347699315</v>
       </c>
       <c r="P27">
-        <v>3.473511798903413</v>
+        <v>3.406755495543352</v>
       </c>
       <c r="Q27">
-        <v>13.159231991455695</v>
+        <v>12.81053159927983</v>
       </c>
       <c r="R27">
-        <v>0.4944858929484282</v>
+        <v>0.571919360320509</v>
       </c>
     </row>
     <row r="28">
@@ -1929,46 +1929,46 @@
         <v/>
       </c>
       <c r="E28">
-        <v>9.354624506755183</v>
+        <v>9.756261872937637</v>
       </c>
       <c r="F28">
-        <v>4.829210342367326</v>
+        <v>4.987131489305716</v>
       </c>
       <c r="G28">
-        <v>16.40279181405149</v>
+        <v>16.63431348237822</v>
       </c>
       <c r="H28">
-        <v>0.5726632147021289</v>
+        <v>0.5537269713560518</v>
       </c>
       <c r="I28" t="str">
         <v/>
       </c>
       <c r="J28">
-        <v>7.870738455079817</v>
+        <v>8.473766042875083</v>
       </c>
       <c r="K28">
-        <v>4.884522021842383</v>
+        <v>4.875093620903228</v>
       </c>
       <c r="L28">
-        <v>15.270123670615018</v>
+        <v>15.609915115546107</v>
       </c>
       <c r="M28">
-        <v>0.5027065042250725</v>
+        <v>0.5588499628402962</v>
       </c>
       <c r="N28" t="str">
         <v/>
       </c>
       <c r="O28">
-        <v>7.741162774399743</v>
+        <v>7.879953196230106</v>
       </c>
       <c r="P28">
-        <v>3.989865996435233</v>
+        <v>3.798553436281022</v>
       </c>
       <c r="Q28">
-        <v>12.83448169019049</v>
+        <v>12.497715287223594</v>
       </c>
       <c r="R28">
-        <v>0.48898293961788836</v>
+        <v>0.5378513551707186</v>
       </c>
     </row>
     <row r="29">
@@ -1985,46 +1985,46 @@
         <v/>
       </c>
       <c r="E29">
-        <v>9.155839972504795</v>
+        <v>8.589530196553236</v>
       </c>
       <c r="F29">
-        <v>5.026109598606016</v>
+        <v>4.491913251316739</v>
       </c>
       <c r="G29">
-        <v>16.622821369009603</v>
+        <v>16.19257275805485</v>
       </c>
       <c r="H29">
-        <v>0.5379061453325047</v>
+        <v>0.5359350455280916</v>
       </c>
       <c r="I29" t="str">
         <v/>
       </c>
       <c r="J29">
-        <v>8.666046977445266</v>
+        <v>8.138336105843045</v>
       </c>
       <c r="K29">
-        <v>3.9903458711407316</v>
+        <v>4.3132185100906195</v>
       </c>
       <c r="L29">
-        <v>16.01977988880306</v>
+        <v>15.927957278183532</v>
       </c>
       <c r="M29">
-        <v>0.5858514039723859</v>
+        <v>0.5710748813397635</v>
       </c>
       <c r="N29" t="str">
         <v/>
       </c>
       <c r="O29">
-        <v>6.993800363820615</v>
+        <v>6.725307292880875</v>
       </c>
       <c r="P29">
-        <v>3.606245911436601</v>
+        <v>3.955222138886622</v>
       </c>
       <c r="Q29">
-        <v>12.439522049959516</v>
+        <v>13.17036400688035</v>
       </c>
       <c r="R29">
-        <v>0.5040607919910848</v>
+        <v>0.5553906312411376</v>
       </c>
     </row>
     <row r="30">
@@ -2041,46 +2041,46 @@
         <v/>
       </c>
       <c r="E30">
-        <v>10.419114099626526</v>
+        <v>9.304901138573086</v>
       </c>
       <c r="F30">
-        <v>4.675752436540359</v>
+        <v>4.658414772230708</v>
       </c>
       <c r="G30">
-        <v>16.452756650449153</v>
+        <v>17.50230408416781</v>
       </c>
       <c r="H30">
-        <v>0.5842203678314571</v>
+        <v>0.5434302527941387</v>
       </c>
       <c r="I30" t="str">
         <v/>
       </c>
       <c r="J30">
-        <v>8.375230765261442</v>
+        <v>8.28689100333604</v>
       </c>
       <c r="K30">
-        <v>4.76461869041598</v>
+        <v>4.005716382349902</v>
       </c>
       <c r="L30">
-        <v>15.952668370149567</v>
+        <v>15.664650659108737</v>
       </c>
       <c r="M30">
-        <v>0.5488989516619361</v>
+        <v>0.5152684757474443</v>
       </c>
       <c r="N30" t="str">
         <v/>
       </c>
       <c r="O30">
-        <v>7.56901232963391</v>
+        <v>7.652462735405818</v>
       </c>
       <c r="P30">
-        <v>3.72223534868725</v>
+        <v>3.440975931701281</v>
       </c>
       <c r="Q30">
-        <v>12.24566362580933</v>
+        <v>12.957845206627495</v>
       </c>
       <c r="R30">
-        <v>0.5341816497901</v>
+        <v>0.4885068797103458</v>
       </c>
     </row>
     <row r="31">
@@ -2097,46 +2097,46 @@
         <v/>
       </c>
       <c r="E31">
-        <v>10.12164148499829</v>
+        <v>9.541103127304616</v>
       </c>
       <c r="F31">
-        <v>5.144159472626347</v>
+        <v>4.2053508960903265</v>
       </c>
       <c r="G31">
-        <v>16.849246688337086</v>
+        <v>17.263020626415987</v>
       </c>
       <c r="H31">
-        <v>0.5898700151713214</v>
+        <v>0.5608005411058954</v>
       </c>
       <c r="I31" t="str">
         <v/>
       </c>
       <c r="J31">
-        <v>9.22952586621889</v>
+        <v>9.035905067332262</v>
       </c>
       <c r="K31">
-        <v>4.7800483577096236</v>
+        <v>3.9391643119850457</v>
       </c>
       <c r="L31">
-        <v>16.63200013132993</v>
+        <v>16.776459495342213</v>
       </c>
       <c r="M31">
-        <v>0.5302070783513707</v>
+        <v>0.5611853678315802</v>
       </c>
       <c r="N31" t="str">
         <v/>
       </c>
       <c r="O31">
-        <v>7.355806576788686</v>
+        <v>7.948524034184543</v>
       </c>
       <c r="P31">
-        <v>3.8485996467729637</v>
+        <v>3.6492198760778076</v>
       </c>
       <c r="Q31">
-        <v>12.433676885889525</v>
+        <v>13.405404958015495</v>
       </c>
       <c r="R31">
-        <v>0.5555003596758409</v>
+        <v>0.5423770810033065</v>
       </c>
     </row>
     <row r="32">
@@ -2153,46 +2153,46 @@
         <v/>
       </c>
       <c r="E32">
-        <v>8.79040023369754</v>
+        <v>10.060972577574393</v>
       </c>
       <c r="F32">
-        <v>4.468147901066375</v>
+        <v>4.623837209531875</v>
       </c>
       <c r="G32">
-        <v>17.024960397109886</v>
+        <v>17.569888232097036</v>
       </c>
       <c r="H32">
-        <v>0.5696754515459965</v>
+        <v>0.5312761247486628</v>
       </c>
       <c r="I32" t="str">
         <v/>
       </c>
       <c r="J32">
-        <v>8.067206644669085</v>
+        <v>8.543762898286978</v>
       </c>
       <c r="K32">
-        <v>4.212887400600583</v>
+        <v>4.441367831504565</v>
       </c>
       <c r="L32">
-        <v>16.290595954746003</v>
+        <v>15.53889174346469</v>
       </c>
       <c r="M32">
-        <v>0.5513469037485438</v>
+        <v>0.5178880107484211</v>
       </c>
       <c r="N32" t="str">
         <v/>
       </c>
       <c r="O32">
-        <v>6.964707794965356</v>
+        <v>7.623100607419497</v>
       </c>
       <c r="P32">
-        <v>3.484122327214653</v>
+        <v>3.8862583292002024</v>
       </c>
       <c r="Q32">
-        <v>13.416233090843239</v>
+        <v>12.674769143610302</v>
       </c>
       <c r="R32">
-        <v>0.5245253824677241</v>
+        <v>0.5351220918363079</v>
       </c>
     </row>
     <row r="33">
@@ -2209,46 +2209,46 @@
         <v/>
       </c>
       <c r="E33">
-        <v>8.789919544256515</v>
+        <v>8.69353460497618</v>
       </c>
       <c r="F33">
-        <v>4.694605441807713</v>
+        <v>4.2873692648109625</v>
       </c>
       <c r="G33">
-        <v>17.434501968066364</v>
+        <v>17.18896935543167</v>
       </c>
       <c r="H33">
-        <v>0.5802765619848099</v>
+        <v>0.5113380491835895</v>
       </c>
       <c r="I33" t="str">
         <v/>
       </c>
       <c r="J33">
-        <v>9.073285811453403</v>
+        <v>8.46634291707002</v>
       </c>
       <c r="K33">
-        <v>4.622118358894502</v>
+        <v>4.526572597850238</v>
       </c>
       <c r="L33">
-        <v>16.101730873899847</v>
+        <v>16.29428965415421</v>
       </c>
       <c r="M33">
-        <v>0.5203039494037532</v>
+        <v>0.55860159057688</v>
       </c>
       <c r="N33" t="str">
         <v/>
       </c>
       <c r="O33">
-        <v>7.426846378136857</v>
+        <v>7.749797456965489</v>
       </c>
       <c r="P33">
-        <v>3.3083152715410526</v>
+        <v>3.3649190239911215</v>
       </c>
       <c r="Q33">
-        <v>13.598840259824666</v>
+        <v>13.285147494861025</v>
       </c>
       <c r="R33">
-        <v>0.5133913389650299</v>
+        <v>0.4901596342646192</v>
       </c>
     </row>
     <row r="34">
@@ -2265,46 +2265,46 @@
         <v/>
       </c>
       <c r="E34">
-        <v>9.355881700832409</v>
+        <v>9.140256745991751</v>
       </c>
       <c r="F34">
-        <v>4.699416918169447</v>
+        <v>4.377269824460811</v>
       </c>
       <c r="G34">
-        <v>16.796603368494896</v>
+        <v>17.982881296391586</v>
       </c>
       <c r="H34">
-        <v>0.5604590145969247</v>
+        <v>0.521819352159246</v>
       </c>
       <c r="I34" t="str">
         <v/>
       </c>
       <c r="J34">
-        <v>8.177410638738124</v>
+        <v>8.562307084437947</v>
       </c>
       <c r="K34">
-        <v>4.000333178022401</v>
+        <v>4.206799780931254</v>
       </c>
       <c r="L34">
-        <v>16.48235257954531</v>
+        <v>15.21939157897986</v>
       </c>
       <c r="M34">
-        <v>0.5035360434269243</v>
+        <v>0.5392559099063317</v>
       </c>
       <c r="N34" t="str">
         <v/>
       </c>
       <c r="O34">
-        <v>7.087867418424459</v>
+        <v>7.37908755223786</v>
       </c>
       <c r="P34">
-        <v>3.5024783276859117</v>
+        <v>3.344723679986817</v>
       </c>
       <c r="Q34">
-        <v>13.556266936906276</v>
+        <v>13.098307121563133</v>
       </c>
       <c r="R34">
-        <v>0.5323282184134341</v>
+        <v>0.5365826425774884</v>
       </c>
     </row>
     <row r="35">
@@ -2321,46 +2321,46 @@
         <v/>
       </c>
       <c r="E35">
-        <v>9.801041807936157</v>
+        <v>10.364944655492435</v>
       </c>
       <c r="F35">
-        <v>4.669034237525041</v>
+        <v>4.272670987323693</v>
       </c>
       <c r="G35">
-        <v>17.33106533571915</v>
+        <v>16.914136881475127</v>
       </c>
       <c r="H35">
-        <v>0.5602370917661831</v>
+        <v>0.5577723969375664</v>
       </c>
       <c r="I35" t="str">
         <v/>
       </c>
       <c r="J35">
-        <v>9.000360206894667</v>
+        <v>8.318681460716128</v>
       </c>
       <c r="K35">
-        <v>4.476695270930607</v>
+        <v>4.1207236182888405</v>
       </c>
       <c r="L35">
-        <v>17.144715010858157</v>
+        <v>16.509110847730103</v>
       </c>
       <c r="M35">
-        <v>0.4910064889614224</v>
+        <v>0.5639549056748725</v>
       </c>
       <c r="N35" t="str">
         <v/>
       </c>
       <c r="O35">
-        <v>7.594008014158531</v>
+        <v>7.684758868726161</v>
       </c>
       <c r="P35">
-        <v>3.9733169851127115</v>
+        <v>3.653469743762933</v>
       </c>
       <c r="Q35">
-        <v>12.821948423627381</v>
+        <v>13.513511037414876</v>
       </c>
       <c r="R35">
-        <v>0.5751229035744633</v>
+        <v>0.5795857670353356</v>
       </c>
     </row>
     <row r="36">
@@ -2377,46 +2377,46 @@
         <v/>
       </c>
       <c r="E36">
-        <v>10.216124373591416</v>
+        <v>8.948783448649946</v>
       </c>
       <c r="F36">
-        <v>4.200807303991139</v>
+        <v>4.829669118062611</v>
       </c>
       <c r="G36">
-        <v>17.920165682024756</v>
+        <v>17.956254210556278</v>
       </c>
       <c r="H36">
-        <v>0.5008066644366492</v>
+        <v>0.5618310311288851</v>
       </c>
       <c r="I36" t="str">
         <v/>
       </c>
       <c r="J36">
-        <v>8.332403870304471</v>
+        <v>8.831227335505965</v>
       </c>
       <c r="K36">
-        <v>3.968030636465204</v>
+        <v>4.758245703397466</v>
       </c>
       <c r="L36">
-        <v>17.15836941887785</v>
+        <v>16.02126693551922</v>
       </c>
       <c r="M36">
-        <v>0.5019150156739633</v>
+        <v>0.5027171703681039</v>
       </c>
       <c r="N36" t="str">
         <v/>
       </c>
       <c r="O36">
-        <v>6.888624307562515</v>
+        <v>7.62226467633072</v>
       </c>
       <c r="P36">
-        <v>3.860374313409817</v>
+        <v>3.6543889099294318</v>
       </c>
       <c r="Q36">
-        <v>13.502137188921012</v>
+        <v>12.454878259704248</v>
       </c>
       <c r="R36">
-        <v>0.4817185595111724</v>
+        <v>0.506974486232755</v>
       </c>
     </row>
     <row r="37">
@@ -2433,46 +2433,46 @@
         <v/>
       </c>
       <c r="E37">
-        <v>10.186596211774022</v>
+        <v>9.533483026389927</v>
       </c>
       <c r="F37">
-        <v>4.9487055567024125</v>
+        <v>5.132684920496776</v>
       </c>
       <c r="G37">
-        <v>17.852473242669905</v>
+        <v>16.39605539087894</v>
       </c>
       <c r="H37">
-        <v>0.5038299362276935</v>
+        <v>0.5439434854022666</v>
       </c>
       <c r="I37" t="str">
         <v/>
       </c>
       <c r="J37">
-        <v>8.011216675662038</v>
+        <v>7.994607091555122</v>
       </c>
       <c r="K37">
-        <v>4.8905688684980015</v>
+        <v>4.379388364676492</v>
       </c>
       <c r="L37">
-        <v>15.414548109022682</v>
+        <v>16.290574005407862</v>
       </c>
       <c r="M37">
-        <v>0.5249098414061388</v>
+        <v>0.5081811317636921</v>
       </c>
       <c r="N37" t="str">
         <v/>
       </c>
       <c r="O37">
-        <v>6.742883220797033</v>
+        <v>7.044436569764973</v>
       </c>
       <c r="P37">
-        <v>3.285276452971228</v>
+        <v>3.9168676938920743</v>
       </c>
       <c r="Q37">
-        <v>12.624111584260124</v>
+        <v>13.1730981929243</v>
       </c>
       <c r="R37">
-        <v>0.5231335469866449</v>
+        <v>0.5532584823758159</v>
       </c>
     </row>
     <row r="38">
@@ -2489,46 +2489,46 @@
         <v/>
       </c>
       <c r="E38">
-        <v>9.823069481428378</v>
+        <v>8.586795814054934</v>
       </c>
       <c r="F38">
-        <v>4.987155039006015</v>
+        <v>5.184248554045529</v>
       </c>
       <c r="G38">
-        <v>17.4777036224494</v>
+        <v>18.043256862779135</v>
       </c>
       <c r="H38">
-        <v>0.5111905860480943</v>
+        <v>0.5582853864178063</v>
       </c>
       <c r="I38" t="str">
         <v/>
       </c>
       <c r="J38">
-        <v>7.978341562099268</v>
+        <v>9.522282575424212</v>
       </c>
       <c r="K38">
-        <v>4.856711887667875</v>
+        <v>3.9898896894742504</v>
       </c>
       <c r="L38">
-        <v>16.508840816551725</v>
+        <v>16.955681317105146</v>
       </c>
       <c r="M38">
-        <v>0.5176457319805166</v>
+        <v>0.49605139698682604</v>
       </c>
       <c r="N38" t="str">
         <v/>
       </c>
       <c r="O38">
-        <v>7.161421043104637</v>
+        <v>6.632583553951388</v>
       </c>
       <c r="P38">
-        <v>3.8873783043849124</v>
+        <v>3.4920438068588306</v>
       </c>
       <c r="Q38">
-        <v>13.19777111953889</v>
+        <v>13.000741187688167</v>
       </c>
       <c r="R38">
-        <v>0.4944019754811033</v>
+        <v>0.5609597139967775</v>
       </c>
     </row>
     <row r="39">
@@ -2545,46 +2545,46 @@
         <v/>
       </c>
       <c r="E39">
-        <v>10.23790866319777</v>
+        <v>9.803511843206865</v>
       </c>
       <c r="F39">
-        <v>5.060753792788395</v>
+        <v>4.295862322055623</v>
       </c>
       <c r="G39">
-        <v>17.91444022998773</v>
+        <v>17.200372838359538</v>
       </c>
       <c r="H39">
-        <v>0.5415090008708853</v>
+        <v>0.5977047852380439</v>
       </c>
       <c r="I39" t="str">
         <v/>
       </c>
       <c r="J39">
-        <v>9.48146114346896</v>
+        <v>9.793366771908518</v>
       </c>
       <c r="K39">
-        <v>4.605940815999374</v>
+        <v>4.2255300530445705</v>
       </c>
       <c r="L39">
-        <v>16.222030086559535</v>
+        <v>16.922564801624723</v>
       </c>
       <c r="M39">
-        <v>0.5256538823426173</v>
+        <v>0.5596582822820284</v>
       </c>
       <c r="N39" t="str">
         <v/>
       </c>
       <c r="O39">
-        <v>7.502658089532032</v>
+        <v>6.982580405971595</v>
       </c>
       <c r="P39">
-        <v>3.431401894365111</v>
+        <v>3.679531714873604</v>
       </c>
       <c r="Q39">
-        <v>12.184406423934618</v>
+        <v>12.834619983222014</v>
       </c>
       <c r="R39">
-        <v>0.48988676981741186</v>
+        <v>0.579781371438439</v>
       </c>
     </row>
     <row r="40">
@@ -2601,46 +2601,46 @@
         <v/>
       </c>
       <c r="E40">
-        <v>9.57819381092457</v>
+        <v>9.474565743171773</v>
       </c>
       <c r="F40">
-        <v>5.149180410098171</v>
+        <v>5.085592029183051</v>
       </c>
       <c r="G40">
-        <v>17.45448404180616</v>
+        <v>17.69506447812562</v>
       </c>
       <c r="H40">
-        <v>0.552845869628795</v>
+        <v>0.5777502883966469</v>
       </c>
       <c r="I40" t="str">
         <v/>
       </c>
       <c r="J40">
-        <v>8.19947726689816</v>
+        <v>8.365052810542913</v>
       </c>
       <c r="K40">
-        <v>3.9065480125021566</v>
+        <v>4.642017650360726</v>
       </c>
       <c r="L40">
-        <v>15.214331388617257</v>
+        <v>16.414342220484734</v>
       </c>
       <c r="M40">
-        <v>0.5056903047264574</v>
+        <v>0.5474281419451429</v>
       </c>
       <c r="N40" t="str">
         <v/>
       </c>
       <c r="O40">
-        <v>7.194660193829163</v>
+        <v>7.467035891522745</v>
       </c>
       <c r="P40">
-        <v>3.686919953471364</v>
+        <v>3.5952240260182498</v>
       </c>
       <c r="Q40">
-        <v>12.273225988266</v>
+        <v>13.264552232505588</v>
       </c>
       <c r="R40">
-        <v>0.49318429296372157</v>
+        <v>0.5782582242784803</v>
       </c>
     </row>
     <row r="41">
@@ -2657,46 +2657,46 @@
         <v/>
       </c>
       <c r="E41">
-        <v>10.241332026852536</v>
+        <v>10.19556710520868</v>
       </c>
       <c r="F41">
-        <v>4.407120512681547</v>
+        <v>4.8787579726693675</v>
       </c>
       <c r="G41">
-        <v>17.50681943293366</v>
+        <v>16.261284298110535</v>
       </c>
       <c r="H41">
-        <v>0.5746773748767069</v>
+        <v>0.5796179109583787</v>
       </c>
       <c r="I41" t="str">
         <v/>
       </c>
       <c r="J41">
-        <v>9.149971927665538</v>
+        <v>8.12841681455992</v>
       </c>
       <c r="K41">
-        <v>4.861563336572873</v>
+        <v>3.984983462516689</v>
       </c>
       <c r="L41">
-        <v>15.445002096282252</v>
+        <v>15.280388834244437</v>
       </c>
       <c r="M41">
-        <v>0.5136873368657984</v>
+        <v>0.5520890200825566</v>
       </c>
       <c r="N41" t="str">
         <v/>
       </c>
       <c r="O41">
-        <v>7.236085480805291</v>
+        <v>7.525840741351396</v>
       </c>
       <c r="P41">
-        <v>3.7145888230422672</v>
+        <v>3.642621778048538</v>
       </c>
       <c r="Q41">
-        <v>12.953738060742252</v>
+        <v>12.680219076278819</v>
       </c>
       <c r="R41">
-        <v>0.516956029176671</v>
+        <v>0.48916928024323714</v>
       </c>
     </row>
     <row r="42">
@@ -2713,46 +2713,46 @@
         <v/>
       </c>
       <c r="E42">
-        <v>10.166706348278808</v>
+        <v>9.549351917747439</v>
       </c>
       <c r="F42">
-        <v>4.548487713830953</v>
+        <v>5.086344367549514</v>
       </c>
       <c r="G42">
-        <v>17.839243346263252</v>
+        <v>17.65320635668287</v>
       </c>
       <c r="H42">
-        <v>0.5194163645670511</v>
+        <v>0.5474559588977508</v>
       </c>
       <c r="I42" t="str">
         <v/>
       </c>
       <c r="J42">
-        <v>9.536818836519208</v>
+        <v>9.529163261969645</v>
       </c>
       <c r="K42">
-        <v>4.356836415032611</v>
+        <v>4.389912372670374</v>
       </c>
       <c r="L42">
-        <v>17.145622283650162</v>
+        <v>15.600034326171837</v>
       </c>
       <c r="M42">
-        <v>0.5513376267718887</v>
+        <v>0.5505363587222272</v>
       </c>
       <c r="N42" t="str">
         <v/>
       </c>
       <c r="O42">
-        <v>7.320524020134352</v>
+        <v>7.989596666736526</v>
       </c>
       <c r="P42">
-        <v>3.8323371750622806</v>
+        <v>3.293628260944886</v>
       </c>
       <c r="Q42">
-        <v>12.558020812236585</v>
+        <v>12.617984223312249</v>
       </c>
       <c r="R42">
-        <v>0.5649771066555896</v>
+        <v>0.48948071916727703</v>
       </c>
     </row>
     <row r="43">
@@ -2769,46 +2769,46 @@
         <v/>
       </c>
       <c r="E43">
-        <v>8.79239408932614</v>
+        <v>10.077202686820737</v>
       </c>
       <c r="F43">
-        <v>4.7542858173182685</v>
+        <v>4.778709515514971</v>
       </c>
       <c r="G43">
-        <v>16.476754187693803</v>
+        <v>16.763091191234505</v>
       </c>
       <c r="H43">
-        <v>0.5470358106172929</v>
+        <v>0.5873647585222648</v>
       </c>
       <c r="I43" t="str">
         <v/>
       </c>
       <c r="J43">
-        <v>8.820742605409581</v>
+        <v>8.59648278532867</v>
       </c>
       <c r="K43">
-        <v>4.594067513280571</v>
+        <v>4.702074010950706</v>
       </c>
       <c r="L43">
-        <v>17.076477900171</v>
+        <v>16.89584737877562</v>
       </c>
       <c r="M43">
-        <v>0.5324293181393975</v>
+        <v>0.5430942151175446</v>
       </c>
       <c r="N43" t="str">
         <v/>
       </c>
       <c r="O43">
-        <v>7.55525973302979</v>
+        <v>7.209094373505758</v>
       </c>
       <c r="P43">
-        <v>3.5478871076687883</v>
+        <v>3.8135822514883926</v>
       </c>
       <c r="Q43">
-        <v>12.768000160687894</v>
+        <v>12.910344198064543</v>
       </c>
       <c r="R43">
-        <v>0.559699454518491</v>
+        <v>0.5152371105982535</v>
       </c>
     </row>
     <row r="44">
@@ -2825,46 +2825,46 @@
         <v/>
       </c>
       <c r="E44">
-        <v>9.394963454953489</v>
+        <v>9.499424144239317</v>
       </c>
       <c r="F44">
-        <v>4.537290753059368</v>
+        <v>4.610092270529298</v>
       </c>
       <c r="G44">
-        <v>17.05770987705567</v>
+        <v>16.64719622536645</v>
       </c>
       <c r="H44">
-        <v>0.591282484185722</v>
+        <v>0.5196651114454464</v>
       </c>
       <c r="I44" t="str">
         <v/>
       </c>
       <c r="J44">
-        <v>9.59677211378371</v>
+        <v>8.612876727728032</v>
       </c>
       <c r="K44">
-        <v>4.065296333846706</v>
+        <v>4.365911051779112</v>
       </c>
       <c r="L44">
-        <v>16.606263466620366</v>
+        <v>15.84420492689867</v>
       </c>
       <c r="M44">
-        <v>0.5724610746133338</v>
+        <v>0.5328745422954171</v>
       </c>
       <c r="N44" t="str">
         <v/>
       </c>
       <c r="O44">
-        <v>6.73008574032986</v>
+        <v>7.009914383747221</v>
       </c>
       <c r="P44">
-        <v>3.8868669837155205</v>
+        <v>3.8384423457717647</v>
       </c>
       <c r="Q44">
-        <v>12.181756760473833</v>
+        <v>12.910284984073106</v>
       </c>
       <c r="R44">
-        <v>0.5768494311832615</v>
+        <v>0.5149106803237911</v>
       </c>
     </row>
     <row r="45">
@@ -2881,46 +2881,46 @@
         <v/>
       </c>
       <c r="E45">
-        <v>9.191473397053214</v>
+        <v>9.582027280154808</v>
       </c>
       <c r="F45">
-        <v>5.109388813948554</v>
+        <v>4.464762230639137</v>
       </c>
       <c r="G45">
-        <v>16.28885842746881</v>
+        <v>16.748564244376425</v>
       </c>
       <c r="H45">
-        <v>0.538705868458607</v>
+        <v>0.532413461907918</v>
       </c>
       <c r="I45" t="str">
         <v/>
       </c>
       <c r="J45">
-        <v>9.103790299077723</v>
+        <v>8.677366648709876</v>
       </c>
       <c r="K45">
-        <v>4.82742659553079</v>
+        <v>4.697167412305107</v>
       </c>
       <c r="L45">
-        <v>16.230422158938442</v>
+        <v>15.890827582220476</v>
       </c>
       <c r="M45">
-        <v>0.5747748841874234</v>
+        <v>0.5514177588964283</v>
       </c>
       <c r="N45" t="str">
         <v/>
       </c>
       <c r="O45">
-        <v>7.492233327387236</v>
+        <v>6.712767281402583</v>
       </c>
       <c r="P45">
-        <v>3.956972456878177</v>
+        <v>3.3431093770058755</v>
       </c>
       <c r="Q45">
-        <v>13.342572050183126</v>
+        <v>12.697306744514188</v>
       </c>
       <c r="R45">
-        <v>0.5598243512607534</v>
+        <v>0.5721675519919451</v>
       </c>
     </row>
     <row r="46">
@@ -2937,46 +2937,46 @@
         <v/>
       </c>
       <c r="E46">
-        <v>9.38000211950029</v>
+        <v>9.983462381991682</v>
       </c>
       <c r="F46">
-        <v>4.6394019602454835</v>
+        <v>4.21412789037065</v>
       </c>
       <c r="G46">
-        <v>17.728904060113663</v>
+        <v>16.407024144753837</v>
       </c>
       <c r="H46">
-        <v>0.5955512682265881</v>
+        <v>0.5995758396681398</v>
       </c>
       <c r="I46" t="str">
         <v/>
       </c>
       <c r="J46">
-        <v>9.0508117006841</v>
+        <v>9.14156643051589</v>
       </c>
       <c r="K46">
-        <v>4.028385001959252</v>
+        <v>4.411475186624611</v>
       </c>
       <c r="L46">
-        <v>16.720281376664953</v>
+        <v>16.849300093137472</v>
       </c>
       <c r="M46">
-        <v>0.5671217006803064</v>
+        <v>0.5035573679276764</v>
       </c>
       <c r="N46" t="str">
         <v/>
       </c>
       <c r="O46">
-        <v>6.7165093666561395</v>
+        <v>7.441324529048438</v>
       </c>
       <c r="P46">
-        <v>3.408672488985812</v>
+        <v>3.6784129243405648</v>
       </c>
       <c r="Q46">
-        <v>12.676070550175728</v>
+        <v>12.401536627190492</v>
       </c>
       <c r="R46">
-        <v>0.517042623677334</v>
+        <v>0.49280998637279394</v>
       </c>
     </row>
     <row r="47">
@@ -2993,46 +2993,46 @@
         <v/>
       </c>
       <c r="E47">
-        <v>9.79819550615485</v>
+        <v>10.450267771372282</v>
       </c>
       <c r="F47">
-        <v>4.837608451661827</v>
+        <v>5.155243608863016</v>
       </c>
       <c r="G47">
-        <v>16.995379654636682</v>
+        <v>16.613320040528837</v>
       </c>
       <c r="H47">
-        <v>0.5743332199714006</v>
+        <v>0.5439057561264986</v>
       </c>
       <c r="I47" t="str">
         <v/>
       </c>
       <c r="J47">
-        <v>8.997859843741168</v>
+        <v>7.951164087041872</v>
       </c>
       <c r="K47">
-        <v>4.772395511856895</v>
+        <v>4.301970270018838</v>
       </c>
       <c r="L47">
-        <v>15.449368751353427</v>
+        <v>16.472068224315336</v>
       </c>
       <c r="M47">
-        <v>0.5211198658813339</v>
+        <v>0.5268839097371112</v>
       </c>
       <c r="N47" t="str">
         <v/>
       </c>
       <c r="O47">
-        <v>7.048062036129496</v>
+        <v>7.695562515903177</v>
       </c>
       <c r="P47">
-        <v>3.656074477665351</v>
+        <v>3.8129748665734895</v>
       </c>
       <c r="Q47">
-        <v>12.823457523856115</v>
+        <v>12.745557713231491</v>
       </c>
       <c r="R47">
-        <v>0.5574470588559847</v>
+        <v>0.49946796904611307</v>
       </c>
     </row>
     <row r="48">
@@ -3049,46 +3049,46 @@
         <v/>
       </c>
       <c r="E48">
-        <v>10.110365974817874</v>
+        <v>9.007334738075432</v>
       </c>
       <c r="F48">
-        <v>4.61776876271101</v>
+        <v>4.5332220485479935</v>
       </c>
       <c r="G48">
-        <v>16.816283797744408</v>
+        <v>17.125808713354928</v>
       </c>
       <c r="H48">
-        <v>0.5622094831480872</v>
+        <v>0.5433181014332384</v>
       </c>
       <c r="I48" t="str">
         <v/>
       </c>
       <c r="J48">
-        <v>9.799624307374327</v>
+        <v>9.050115228507412</v>
       </c>
       <c r="K48">
-        <v>4.345710190877516</v>
+        <v>4.178386537747832</v>
       </c>
       <c r="L48">
-        <v>15.755783222233019</v>
+        <v>15.38759393623966</v>
       </c>
       <c r="M48">
-        <v>0.5205783567714072</v>
+        <v>0.5871262890794179</v>
       </c>
       <c r="N48" t="str">
         <v/>
       </c>
       <c r="O48">
-        <v>7.308245152641434</v>
+        <v>6.568787202544417</v>
       </c>
       <c r="P48">
-        <v>3.871476847457326</v>
+        <v>3.776522092295986</v>
       </c>
       <c r="Q48">
-        <v>12.820923985458784</v>
+        <v>12.845718264384882</v>
       </c>
       <c r="R48">
-        <v>0.4888653532510633</v>
+        <v>0.5371924368533673</v>
       </c>
     </row>
     <row r="49">
@@ -3105,46 +3105,46 @@
         <v/>
       </c>
       <c r="E49">
-        <v>8.706746451377583</v>
+        <v>9.831861323994744</v>
       </c>
       <c r="F49">
-        <v>4.8260233728758255</v>
+        <v>4.8599630792052775</v>
       </c>
       <c r="G49">
-        <v>17.5197580959272</v>
+        <v>16.578941261552945</v>
       </c>
       <c r="H49">
-        <v>0.5079411388225648</v>
+        <v>0.5455234513248458</v>
       </c>
       <c r="I49" t="str">
         <v/>
       </c>
       <c r="J49">
-        <v>8.681583885497112</v>
+        <v>7.890595784012489</v>
       </c>
       <c r="K49">
-        <v>4.599295025099206</v>
+        <v>4.119739827943118</v>
       </c>
       <c r="L49">
-        <v>15.882813782904572</v>
+        <v>17.031968987031675</v>
       </c>
       <c r="M49">
-        <v>0.5551080520270242</v>
+        <v>0.5601409743027091</v>
       </c>
       <c r="N49" t="str">
         <v/>
       </c>
       <c r="O49">
-        <v>6.985020036148578</v>
+        <v>6.655395614541062</v>
       </c>
       <c r="P49">
-        <v>3.8447888591305834</v>
+        <v>3.658126948615738</v>
       </c>
       <c r="Q49">
-        <v>12.482434880715703</v>
+        <v>12.727612749347475</v>
       </c>
       <c r="R49">
-        <v>0.544579488814951</v>
+        <v>0.5478405324081892</v>
       </c>
     </row>
     <row r="50">
@@ -3161,46 +3161,46 @@
         <v/>
       </c>
       <c r="E50">
-        <v>9.390412777363924</v>
+        <v>8.832223698550534</v>
       </c>
       <c r="F50">
-        <v>4.392993280638003</v>
+        <v>4.985055525359675</v>
       </c>
       <c r="G50">
-        <v>17.383862565428334</v>
+        <v>16.42831711366116</v>
       </c>
       <c r="H50">
-        <v>0.5417331695520143</v>
+        <v>0.5631135495112662</v>
       </c>
       <c r="I50" t="str">
         <v/>
       </c>
       <c r="J50">
-        <v>8.795735334201556</v>
+        <v>9.28477916940886</v>
       </c>
       <c r="K50">
-        <v>4.70059848415557</v>
+        <v>4.593174443638386</v>
       </c>
       <c r="L50">
-        <v>16.706573546064767</v>
+        <v>16.360474445629766</v>
       </c>
       <c r="M50">
-        <v>0.537831910397596</v>
+        <v>0.5110033543519533</v>
       </c>
       <c r="N50" t="str">
         <v/>
       </c>
       <c r="O50">
-        <v>6.557840532260878</v>
+        <v>7.149901535111988</v>
       </c>
       <c r="P50">
-        <v>3.354212022929624</v>
+        <v>3.56956273817465</v>
       </c>
       <c r="Q50">
-        <v>13.3311957925097</v>
+        <v>12.46015811227765</v>
       </c>
       <c r="R50">
-        <v>0.48505037231695347</v>
+        <v>0.48548364246442294</v>
       </c>
     </row>
     <row r="51">
@@ -3352,7 +3352,7 @@
         <v/>
       </c>
       <c r="G2">
-        <v>46.696918167109736</v>
+        <v>49.42763511197316</v>
       </c>
       <c r="H2" t="str">
         <v/>
@@ -3370,7 +3370,7 @@
         <v/>
       </c>
       <c r="M2">
-        <v>47.014296645318</v>
+        <v>52.455314186217656</v>
       </c>
       <c r="N2" t="str">
         <v/>
@@ -3388,7 +3388,7 @@
         <v/>
       </c>
       <c r="S2">
-        <v>38.90006757337865</v>
+        <v>39.955746373192554</v>
       </c>
     </row>
     <row r="3">
@@ -3411,7 +3411,7 @@
         <v/>
       </c>
       <c r="G3">
-        <v>54.73713485522092</v>
+        <v>50.09800053116695</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -3429,7 +3429,7 @@
         <v/>
       </c>
       <c r="M3">
-        <v>46.36981830454278</v>
+        <v>50.28944034938305</v>
       </c>
       <c r="N3" t="str">
         <v/>
@@ -3447,7 +3447,7 @@
         <v/>
       </c>
       <c r="S3">
-        <v>42.27734836804885</v>
+        <v>40.40421389867618</v>
       </c>
     </row>
     <row r="4">
@@ -3470,7 +3470,7 @@
         <v/>
       </c>
       <c r="G4">
-        <v>52.28515475916017</v>
+        <v>48.96116858382221</v>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -3488,7 +3488,7 @@
         <v/>
       </c>
       <c r="M4">
-        <v>47.198276494350814</v>
+        <v>46.586418718680264</v>
       </c>
       <c r="N4" t="str">
         <v/>
@@ -3506,7 +3506,7 @@
         <v/>
       </c>
       <c r="S4">
-        <v>40.95370726097335</v>
+        <v>44.04266232989725</v>
       </c>
     </row>
     <row r="5">
@@ -3529,7 +3529,7 @@
         <v/>
       </c>
       <c r="G5">
-        <v>51.66833253810743</v>
+        <v>49.052872490271476</v>
       </c>
       <c r="H5" t="str">
         <v/>
@@ -3547,7 +3547,7 @@
         <v/>
       </c>
       <c r="M5">
-        <v>45.18265257293493</v>
+        <v>48.099711620083035</v>
       </c>
       <c r="N5" t="str">
         <v/>
@@ -3565,7 +3565,7 @@
         <v/>
       </c>
       <c r="S5">
-        <v>46.44505634655825</v>
+        <v>44.06209405119817</v>
       </c>
     </row>
     <row r="6">
@@ -3588,7 +3588,7 @@
         <v/>
       </c>
       <c r="G6">
-        <v>47.42261306897805</v>
+        <v>50.99751567089476</v>
       </c>
       <c r="H6" t="str">
         <v/>
@@ -3606,7 +3606,7 @@
         <v/>
       </c>
       <c r="M6">
-        <v>47.982056736425186</v>
+        <v>47.93018328119957</v>
       </c>
       <c r="N6" t="str">
         <v/>
@@ -3624,7 +3624,7 @@
         <v/>
       </c>
       <c r="S6">
-        <v>40.59171103919155</v>
+        <v>43.51249858495219</v>
       </c>
     </row>
     <row r="7">
@@ -3647,7 +3647,7 @@
         <v/>
       </c>
       <c r="G7">
-        <v>47.25187076122767</v>
+        <v>52.99982077248394</v>
       </c>
       <c r="H7" t="str">
         <v/>
@@ -3665,7 +3665,7 @@
         <v/>
       </c>
       <c r="M7">
-        <v>47.32773811995365</v>
+        <v>47.98395649034834</v>
       </c>
       <c r="N7" t="str">
         <v/>
@@ -3683,7 +3683,7 @@
         <v/>
       </c>
       <c r="S7">
-        <v>41.2293959268251</v>
+        <v>43.054087469852675</v>
       </c>
     </row>
     <row r="8">
@@ -3706,7 +3706,7 @@
         <v/>
       </c>
       <c r="G8">
-        <v>54.912564778085084</v>
+        <v>49.115783693973235</v>
       </c>
       <c r="H8" t="str">
         <v/>
@@ -3724,7 +3724,7 @@
         <v/>
       </c>
       <c r="M8">
-        <v>48.819428027426426</v>
+        <v>43.54406373564431</v>
       </c>
       <c r="N8" t="str">
         <v/>
@@ -3742,7 +3742,7 @@
         <v/>
       </c>
       <c r="S8">
-        <v>41.56326103482039</v>
+        <v>46.42898897279961</v>
       </c>
     </row>
     <row r="9">
@@ -3765,7 +3765,7 @@
         <v/>
       </c>
       <c r="G9">
-        <v>54.22902140853628</v>
+        <v>47.110600505638345</v>
       </c>
       <c r="H9" t="str">
         <v/>
@@ -3783,7 +3783,7 @@
         <v/>
       </c>
       <c r="M9">
-        <v>50.880867882747495</v>
+        <v>46.83701622991458</v>
       </c>
       <c r="N9" t="str">
         <v/>
@@ -3801,7 +3801,7 @@
         <v/>
       </c>
       <c r="S9">
-        <v>44.04673728539759</v>
+        <v>42.88188730008475</v>
       </c>
     </row>
     <row r="10">
@@ -3824,7 +3824,7 @@
         <v/>
       </c>
       <c r="G10">
-        <v>48.851446266343906</v>
+        <v>45.35778772261802</v>
       </c>
       <c r="H10" t="str">
         <v/>
@@ -3842,7 +3842,7 @@
         <v/>
       </c>
       <c r="M10">
-        <v>44.47987916163773</v>
+        <v>49.61188601215326</v>
       </c>
       <c r="N10" t="str">
         <v/>
@@ -3860,7 +3860,7 @@
         <v/>
       </c>
       <c r="S10">
-        <v>46.033995179184444</v>
+        <v>39.45018263184124</v>
       </c>
     </row>
     <row r="11">
@@ -3883,7 +3883,7 @@
         <v/>
       </c>
       <c r="G11">
-        <v>52.39327733943924</v>
+        <v>51.573208850321464</v>
       </c>
       <c r="H11" t="str">
         <v/>
@@ -3901,7 +3901,7 @@
         <v/>
       </c>
       <c r="M11">
-        <v>51.15765196372792</v>
+        <v>48.57479980226539</v>
       </c>
       <c r="N11" t="str">
         <v/>
@@ -3919,7 +3919,7 @@
         <v/>
       </c>
       <c r="S11">
-        <v>40.08547818447389</v>
+        <v>39.20040431099746</v>
       </c>
     </row>
     <row r="12">
@@ -3942,7 +3942,7 @@
         <v/>
       </c>
       <c r="G12">
-        <v>46.71323647219895</v>
+        <v>45.53559745721631</v>
       </c>
       <c r="H12" t="str">
         <v/>
@@ -3960,7 +3960,7 @@
         <v/>
       </c>
       <c r="M12">
-        <v>45.82826327051814</v>
+        <v>46.61297409247642</v>
       </c>
       <c r="N12" t="str">
         <v/>
@@ -3978,7 +3978,7 @@
         <v/>
       </c>
       <c r="S12">
-        <v>42.85540187504952</v>
+        <v>40.36457283284539</v>
       </c>
     </row>
     <row r="13">
@@ -4001,7 +4001,7 @@
         <v/>
       </c>
       <c r="G13">
-        <v>46.90711985517883</v>
+        <v>55.13226366325132</v>
       </c>
       <c r="H13" t="str">
         <v/>
@@ -4019,7 +4019,7 @@
         <v/>
       </c>
       <c r="M13">
-        <v>47.28016264646567</v>
+        <v>45.55130929192699</v>
       </c>
       <c r="N13" t="str">
         <v/>
@@ -4037,7 +4037,7 @@
         <v/>
       </c>
       <c r="S13">
-        <v>41.180114793610926</v>
+        <v>41.359222305299085</v>
       </c>
     </row>
     <row r="14">
@@ -4060,7 +4060,7 @@
         <v/>
       </c>
       <c r="G14">
-        <v>50.881587113076286</v>
+        <v>54.70723639898268</v>
       </c>
       <c r="H14" t="str">
         <v/>
@@ -4078,7 +4078,7 @@
         <v/>
       </c>
       <c r="M14">
-        <v>45.188346165343546</v>
+        <v>46.0606827998326</v>
       </c>
       <c r="N14" t="str">
         <v/>
@@ -4096,7 +4096,7 @@
         <v/>
       </c>
       <c r="S14">
-        <v>41.93645167958523</v>
+        <v>43.79974559526443</v>
       </c>
     </row>
     <row r="15">
@@ -4119,7 +4119,7 @@
         <v/>
       </c>
       <c r="G15">
-        <v>49.969050082057926</v>
+        <v>45.30611411347109</v>
       </c>
       <c r="H15" t="str">
         <v/>
@@ -4137,7 +4137,7 @@
         <v/>
       </c>
       <c r="M15">
-        <v>47.875991852556076</v>
+        <v>48.5310595810064</v>
       </c>
       <c r="N15" t="str">
         <v/>
@@ -4155,7 +4155,7 @@
         <v/>
       </c>
       <c r="S15">
-        <v>39.736544476673714</v>
+        <v>39.685083113319976</v>
       </c>
     </row>
     <row r="16">
@@ -4178,7 +4178,7 @@
         <v/>
       </c>
       <c r="G16">
-        <v>52.24850801300449</v>
+        <v>47.68477522646253</v>
       </c>
       <c r="H16" t="str">
         <v/>
@@ -4196,7 +4196,7 @@
         <v/>
       </c>
       <c r="M16">
-        <v>47.162585527382355</v>
+        <v>44.49247888559448</v>
       </c>
       <c r="N16" t="str">
         <v/>
@@ -4214,7 +4214,7 @@
         <v/>
       </c>
       <c r="S16">
-        <v>46.49837793475867</v>
+        <v>40.545262656133545</v>
       </c>
     </row>
     <row r="17">
@@ -4237,7 +4237,7 @@
         <v/>
       </c>
       <c r="G17">
-        <v>54.34950666204116</v>
+        <v>48.629183056147575</v>
       </c>
       <c r="H17" t="str">
         <v/>
@@ -4255,7 +4255,7 @@
         <v/>
       </c>
       <c r="M17">
-        <v>50.09039989140497</v>
+        <v>44.614164187725414</v>
       </c>
       <c r="N17" t="str">
         <v/>
@@ -4273,7 +4273,7 @@
         <v/>
       </c>
       <c r="S17">
-        <v>40.74075516749905</v>
+        <v>41.69472801503769</v>
       </c>
     </row>
     <row r="18">
@@ -4296,7 +4296,7 @@
         <v/>
       </c>
       <c r="G18">
-        <v>49.4802078300999</v>
+        <v>53.370498131666</v>
       </c>
       <c r="H18" t="str">
         <v/>
@@ -4314,7 +4314,7 @@
         <v/>
       </c>
       <c r="M18">
-        <v>42.90740895103469</v>
+        <v>50.620836897733604</v>
       </c>
       <c r="N18" t="str">
         <v/>
@@ -4332,7 +4332,7 @@
         <v/>
       </c>
       <c r="S18">
-        <v>40.1483768059784</v>
+        <v>39.037975341716184</v>
       </c>
     </row>
     <row r="19">
@@ -4355,7 +4355,7 @@
         <v/>
       </c>
       <c r="G19">
-        <v>51.89210268797861</v>
+        <v>51.97251273943515</v>
       </c>
       <c r="H19" t="str">
         <v/>
@@ -4373,7 +4373,7 @@
         <v/>
       </c>
       <c r="M19">
-        <v>44.62172970027777</v>
+        <v>43.082869471627895</v>
       </c>
       <c r="N19" t="str">
         <v/>
@@ -4391,7 +4391,7 @@
         <v/>
       </c>
       <c r="S19">
-        <v>43.88508743337679</v>
+        <v>41.20757582554017</v>
       </c>
     </row>
     <row r="20">
@@ -4414,7 +4414,7 @@
         <v/>
       </c>
       <c r="G20">
-        <v>49.91575376710753</v>
+        <v>46.87986926900526</v>
       </c>
       <c r="H20" t="str">
         <v/>
@@ -4432,7 +4432,7 @@
         <v/>
       </c>
       <c r="M20">
-        <v>45.27397532567566</v>
+        <v>52.05941534660474</v>
       </c>
       <c r="N20" t="str">
         <v/>
@@ -4450,7 +4450,7 @@
         <v/>
       </c>
       <c r="S20">
-        <v>39.578809162279924</v>
+        <v>42.17321748846993</v>
       </c>
     </row>
     <row r="21">
@@ -4473,7 +4473,7 @@
         <v/>
       </c>
       <c r="G21">
-        <v>47.57695232516655</v>
+        <v>47.70621777334443</v>
       </c>
       <c r="H21" t="str">
         <v/>
@@ -4491,7 +4491,7 @@
         <v/>
       </c>
       <c r="M21">
-        <v>44.33950241025582</v>
+        <v>45.00121867015578</v>
       </c>
       <c r="N21" t="str">
         <v/>
@@ -4509,7 +4509,7 @@
         <v/>
       </c>
       <c r="S21">
-        <v>41.73635338294714</v>
+        <v>41.62689887171869</v>
       </c>
     </row>
     <row r="22">
@@ -4532,7 +4532,7 @@
         <v/>
       </c>
       <c r="G22">
-        <v>54.80488165313688</v>
+        <v>47.96766431773255</v>
       </c>
       <c r="H22" t="str">
         <v/>
@@ -4550,7 +4550,7 @@
         <v/>
       </c>
       <c r="M22">
-        <v>48.3987907813469</v>
+        <v>44.49947270922644</v>
       </c>
       <c r="N22" t="str">
         <v/>
@@ -4568,7 +4568,7 @@
         <v/>
       </c>
       <c r="S22">
-        <v>39.654798858836365</v>
+        <v>40.41462641999761</v>
       </c>
     </row>
     <row r="23">
@@ -4591,7 +4591,7 @@
         <v/>
       </c>
       <c r="G23">
-        <v>46.8513425200225</v>
+        <v>48.72358615464392</v>
       </c>
       <c r="H23" t="str">
         <v/>
@@ -4609,7 +4609,7 @@
         <v/>
       </c>
       <c r="M23">
-        <v>46.148008818132105</v>
+        <v>44.844541030911316</v>
       </c>
       <c r="N23" t="str">
         <v/>
@@ -4627,7 +4627,7 @@
         <v/>
       </c>
       <c r="S23">
-        <v>41.20572391674489</v>
+        <v>39.293355431410184</v>
       </c>
     </row>
     <row r="24">
@@ -4650,7 +4650,7 @@
         <v/>
       </c>
       <c r="G24">
-        <v>46.38558301345042</v>
+        <v>45.49251475951473</v>
       </c>
       <c r="H24" t="str">
         <v/>
@@ -4668,7 +4668,7 @@
         <v/>
       </c>
       <c r="M24">
-        <v>50.028254013601675</v>
+        <v>48.903461394696315</v>
       </c>
       <c r="N24" t="str">
         <v/>
@@ -4686,7 +4686,7 @@
         <v/>
       </c>
       <c r="S24">
-        <v>40.51240148847907</v>
+        <v>41.91202255497997</v>
       </c>
     </row>
     <row r="25">
@@ -4709,7 +4709,7 @@
         <v/>
       </c>
       <c r="G25">
-        <v>51.96094332932693</v>
+        <v>54.1091123128735</v>
       </c>
       <c r="H25" t="str">
         <v/>
@@ -4727,7 +4727,7 @@
         <v/>
       </c>
       <c r="M25">
-        <v>44.43478227639306</v>
+        <v>48.16750674403616</v>
       </c>
       <c r="N25" t="str">
         <v/>
@@ -4745,7 +4745,7 @@
         <v/>
       </c>
       <c r="S25">
-        <v>46.26873634877937</v>
+        <v>46.30423696628382</v>
       </c>
     </row>
     <row r="26">
@@ -4768,7 +4768,7 @@
         <v/>
       </c>
       <c r="G26">
-        <v>55.04625479819071</v>
+        <v>54.402830322385746</v>
       </c>
       <c r="H26" t="str">
         <v/>
@@ -4786,7 +4786,7 @@
         <v/>
       </c>
       <c r="M26">
-        <v>52.69886042604206</v>
+        <v>50.984120374073605</v>
       </c>
       <c r="N26" t="str">
         <v/>
@@ -4804,7 +4804,7 @@
         <v/>
       </c>
       <c r="S26">
-        <v>40.245434964597465</v>
+        <v>40.53991172954838</v>
       </c>
     </row>
     <row r="27">
@@ -4827,7 +4827,7 @@
         <v/>
       </c>
       <c r="G27">
-        <v>49.43932152896708</v>
+        <v>53.38332583519702</v>
       </c>
       <c r="H27" t="str">
         <v/>
@@ -4845,7 +4845,7 @@
         <v/>
       </c>
       <c r="M27">
-        <v>51.666543442266125</v>
+        <v>48.57866675258636</v>
       </c>
       <c r="N27" t="str">
         <v/>
@@ -4863,7 +4863,7 @@
         <v/>
       </c>
       <c r="S27">
-        <v>42.10791205255843</v>
+        <v>41.974146059673885</v>
       </c>
     </row>
     <row r="28">
@@ -4886,7 +4886,7 @@
         <v/>
       </c>
       <c r="G28">
-        <v>48.87140507535452</v>
+        <v>50.540995138865796</v>
       </c>
       <c r="H28" t="str">
         <v/>
@@ -4904,7 +4904,7 @@
         <v/>
       </c>
       <c r="M28">
-        <v>49.895505721770505</v>
+        <v>45.37029014803934</v>
       </c>
       <c r="N28" t="str">
         <v/>
@@ -4922,7 +4922,7 @@
         <v/>
       </c>
       <c r="S28">
-        <v>38.779579045888305</v>
+        <v>44.23301076147891</v>
       </c>
     </row>
     <row r="29">
@@ -4945,7 +4945,7 @@
         <v/>
       </c>
       <c r="G29">
-        <v>45.68152648386699</v>
+        <v>49.18606606153606</v>
       </c>
       <c r="H29" t="str">
         <v/>
@@ -4963,7 +4963,7 @@
         <v/>
       </c>
       <c r="M29">
-        <v>52.39152691610036</v>
+        <v>45.99120824712232</v>
       </c>
       <c r="N29" t="str">
         <v/>
@@ -4981,7 +4981,7 @@
         <v/>
       </c>
       <c r="S29">
-        <v>43.115686813070425</v>
+        <v>40.57092138377021</v>
       </c>
     </row>
     <row r="30">
@@ -5004,7 +5004,7 @@
         <v/>
       </c>
       <c r="G30">
-        <v>46.53425744280775</v>
+        <v>49.50607854289086</v>
       </c>
       <c r="H30" t="str">
         <v/>
@@ -5022,7 +5022,7 @@
         <v/>
       </c>
       <c r="M30">
-        <v>50.55058325354425</v>
+        <v>44.80956955103379</v>
       </c>
       <c r="N30" t="str">
         <v/>
@@ -5040,7 +5040,7 @@
         <v/>
       </c>
       <c r="S30">
-        <v>44.67409718712305</v>
+        <v>40.57917797479901</v>
       </c>
     </row>
     <row r="31">
@@ -5063,7 +5063,7 @@
         <v/>
       </c>
       <c r="G31">
-        <v>54.658843403798805</v>
+        <v>51.153975811472336</v>
       </c>
       <c r="H31" t="str">
         <v/>
@@ -5081,7 +5081,7 @@
         <v/>
       </c>
       <c r="M31">
-        <v>44.918960626130804</v>
+        <v>50.646733415561755</v>
       </c>
       <c r="N31" t="str">
         <v/>
@@ -5099,7 +5099,7 @@
         <v/>
       </c>
       <c r="S31">
-        <v>41.9774605459035</v>
+        <v>46.300844822705514</v>
       </c>
     </row>
     <row r="32">
@@ -5122,7 +5122,7 @@
         <v/>
       </c>
       <c r="G32">
-        <v>47.43856255512155</v>
+        <v>52.620967280537165</v>
       </c>
       <c r="H32" t="str">
         <v/>
@@ -5140,7 +5140,7 @@
         <v/>
       </c>
       <c r="M32">
-        <v>43.88371055553789</v>
+        <v>47.86339880532037</v>
       </c>
       <c r="N32" t="str">
         <v/>
@@ -5158,7 +5158,7 @@
         <v/>
       </c>
       <c r="S32">
-        <v>45.20821376274664</v>
+        <v>40.27450372531635</v>
       </c>
     </row>
     <row r="33">
@@ -5181,7 +5181,7 @@
         <v/>
       </c>
       <c r="G33">
-        <v>45.25687093542806</v>
+        <v>51.84944061744528</v>
       </c>
       <c r="H33" t="str">
         <v/>
@@ -5199,7 +5199,7 @@
         <v/>
       </c>
       <c r="M33">
-        <v>51.51427897728776</v>
+        <v>44.98957742204439</v>
       </c>
       <c r="N33" t="str">
         <v/>
@@ -5217,7 +5217,7 @@
         <v/>
       </c>
       <c r="S33">
-        <v>45.14962581790318</v>
+        <v>38.68057879787189</v>
       </c>
     </row>
     <row r="34">
@@ -5240,7 +5240,7 @@
         <v/>
       </c>
       <c r="G34">
-        <v>48.51978365373</v>
+        <v>53.37622294892312</v>
       </c>
       <c r="H34" t="str">
         <v/>
@@ -5258,7 +5258,7 @@
         <v/>
       </c>
       <c r="M34">
-        <v>44.91923326580175</v>
+        <v>46.0462889308675</v>
       </c>
       <c r="N34" t="str">
         <v/>
@@ -5276,7 +5276,7 @@
         <v/>
       </c>
       <c r="S34">
-        <v>45.670521288306844</v>
+        <v>38.9361873255138</v>
       </c>
     </row>
     <row r="35">
@@ -5299,7 +5299,7 @@
         <v/>
       </c>
       <c r="G35">
-        <v>50.43076217090942</v>
+        <v>47.63081495554006</v>
       </c>
       <c r="H35" t="str">
         <v/>
@@ -5317,7 +5317,7 @@
         <v/>
       </c>
       <c r="M35">
-        <v>47.78152747332795</v>
+        <v>45.074688528647606</v>
       </c>
       <c r="N35" t="str">
         <v/>
@@ -5335,7 +5335,7 @@
         <v/>
       </c>
       <c r="S35">
-        <v>38.846205657271774</v>
+        <v>40.92780712877597</v>
       </c>
     </row>
     <row r="36">
@@ -5358,7 +5358,7 @@
         <v/>
       </c>
       <c r="G36">
-        <v>48.6996463964785</v>
+        <v>51.45007610556587</v>
       </c>
       <c r="H36" t="str">
         <v/>
@@ -5376,7 +5376,7 @@
         <v/>
       </c>
       <c r="M36">
-        <v>48.360791328758744</v>
+        <v>44.590502967317896</v>
       </c>
       <c r="N36" t="str">
         <v/>
@@ -5394,7 +5394,7 @@
         <v/>
       </c>
       <c r="S36">
-        <v>42.18981135588543</v>
+        <v>43.41478258586556</v>
       </c>
     </row>
     <row r="37">
@@ -5417,7 +5417,7 @@
         <v/>
       </c>
       <c r="G37">
-        <v>46.42794974200339</v>
+        <v>50.639683477488994</v>
       </c>
       <c r="H37" t="str">
         <v/>
@@ -5435,7 +5435,7 @@
         <v/>
       </c>
       <c r="M37">
-        <v>42.98362454049117</v>
+        <v>52.09285166730199</v>
       </c>
       <c r="N37" t="str">
         <v/>
@@ -5453,7 +5453,7 @@
         <v/>
       </c>
       <c r="S37">
-        <v>43.651043649898355</v>
+        <v>44.10154040756977</v>
       </c>
     </row>
     <row r="38">
@@ -5476,7 +5476,7 @@
         <v/>
       </c>
       <c r="G38">
-        <v>51.92659164449297</v>
+        <v>50.577949287480045</v>
       </c>
       <c r="H38" t="str">
         <v/>
@@ -5494,7 +5494,7 @@
         <v/>
       </c>
       <c r="M38">
-        <v>43.532478025136555</v>
+        <v>47.00594491645188</v>
       </c>
       <c r="N38" t="str">
         <v/>
@@ -5512,7 +5512,7 @@
         <v/>
       </c>
       <c r="S38">
-        <v>43.47370446420899</v>
+        <v>45.356723999295376</v>
       </c>
     </row>
     <row r="39">
@@ -5535,7 +5535,7 @@
         <v/>
       </c>
       <c r="G39">
-        <v>47.445007402096905</v>
+        <v>45.8028518064862</v>
       </c>
       <c r="H39" t="str">
         <v/>
@@ -5553,7 +5553,7 @@
         <v/>
       </c>
       <c r="M39">
-        <v>45.39001242051026</v>
+        <v>48.376819604043924</v>
       </c>
       <c r="N39" t="str">
         <v/>
@@ -5571,7 +5571,7 @@
         <v/>
       </c>
       <c r="S39">
-        <v>46.13499504102005</v>
+        <v>41.10930998189455</v>
       </c>
     </row>
     <row r="40">
@@ -5594,7 +5594,7 @@
         <v/>
       </c>
       <c r="G40">
-        <v>46.005321496475005</v>
+        <v>54.86990132917187</v>
       </c>
       <c r="H40" t="str">
         <v/>
@@ -5612,7 +5612,7 @@
         <v/>
       </c>
       <c r="M40">
-        <v>50.09635280566417</v>
+        <v>52.058448229950685</v>
       </c>
       <c r="N40" t="str">
         <v/>
@@ -5630,7 +5630,7 @@
         <v/>
       </c>
       <c r="S40">
-        <v>39.44931869715753</v>
+        <v>43.683499052913454</v>
       </c>
     </row>
     <row r="41">
@@ -5653,7 +5653,7 @@
         <v/>
       </c>
       <c r="G41">
-        <v>53.483371893546064</v>
+        <v>54.093891813862626</v>
       </c>
       <c r="H41" t="str">
         <v/>
@@ -5671,7 +5671,7 @@
         <v/>
       </c>
       <c r="M41">
-        <v>52.79790097411143</v>
+        <v>45.75464760543013</v>
       </c>
       <c r="N41" t="str">
         <v/>
@@ -5689,7 +5689,7 @@
         <v/>
       </c>
       <c r="S41">
-        <v>40.10414418826863</v>
+        <v>40.14181958332547</v>
       </c>
     </row>
     <row r="42">
@@ -5712,7 +5712,7 @@
         <v/>
       </c>
       <c r="G42">
-        <v>52.434590601072095</v>
+        <v>47.83217119631583</v>
       </c>
       <c r="H42" t="str">
         <v/>
@@ -5730,7 +5730,7 @@
         <v/>
       </c>
       <c r="M42">
-        <v>47.708689222218794</v>
+        <v>46.54144811263626</v>
       </c>
       <c r="N42" t="str">
         <v/>
@@ -5748,7 +5748,7 @@
         <v/>
       </c>
       <c r="S42">
-        <v>46.48248504075941</v>
+        <v>44.984959435198206</v>
       </c>
     </row>
     <row r="43">
@@ -5771,7 +5771,7 @@
         <v/>
       </c>
       <c r="G43">
-        <v>47.822561165961154</v>
+        <v>54.55552656539735</v>
       </c>
       <c r="H43" t="str">
         <v/>
@@ -5789,7 +5789,7 @@
         <v/>
       </c>
       <c r="M43">
-        <v>49.90925106739281</v>
+        <v>52.52610097830062</v>
       </c>
       <c r="N43" t="str">
         <v/>
@@ -5807,7 +5807,7 @@
         <v/>
       </c>
       <c r="S43">
-        <v>43.77393566852563</v>
+        <v>44.94853768181892</v>
       </c>
     </row>
     <row r="44">
@@ -5830,7 +5830,7 @@
         <v/>
       </c>
       <c r="G44">
-        <v>51.292621715573695</v>
+        <v>50.48265320512077</v>
       </c>
       <c r="H44" t="str">
         <v/>
@@ -5848,7 +5848,7 @@
         <v/>
       </c>
       <c r="M44">
-        <v>43.83464026586211</v>
+        <v>52.362666107299916</v>
       </c>
       <c r="N44" t="str">
         <v/>
@@ -5866,7 +5866,7 @@
         <v/>
       </c>
       <c r="S44">
-        <v>42.28983018084616</v>
+        <v>42.72065063190793</v>
       </c>
     </row>
     <row r="45">
@@ -5889,7 +5889,7 @@
         <v/>
       </c>
       <c r="G45">
-        <v>54.584557693343044</v>
+        <v>45.650522267688146</v>
       </c>
       <c r="H45" t="str">
         <v/>
@@ -5907,7 +5907,7 @@
         <v/>
       </c>
       <c r="M45">
-        <v>51.412121739439044</v>
+        <v>45.31525259061344</v>
       </c>
       <c r="N45" t="str">
         <v/>
@@ -5925,7 +5925,7 @@
         <v/>
       </c>
       <c r="S45">
-        <v>42.28096993540244</v>
+        <v>42.272025299712645</v>
       </c>
     </row>
     <row r="46">
@@ -5948,7 +5948,7 @@
         <v/>
       </c>
       <c r="G46">
-        <v>53.587994106125144</v>
+        <v>48.835552403401564</v>
       </c>
       <c r="H46" t="str">
         <v/>
@@ -5966,7 +5966,7 @@
         <v/>
       </c>
       <c r="M46">
-        <v>46.35062717868454</v>
+        <v>49.0008544574271</v>
       </c>
       <c r="N46" t="str">
         <v/>
@@ -5984,7 +5984,7 @@
         <v/>
       </c>
       <c r="S46">
-        <v>44.21600840507206</v>
+        <v>46.269195777149335</v>
       </c>
     </row>
     <row r="47">
@@ -6007,7 +6007,7 @@
         <v/>
       </c>
       <c r="G47">
-        <v>50.93218166222342</v>
+        <v>46.56778267630679</v>
       </c>
       <c r="H47" t="str">
         <v/>
@@ -6025,7 +6025,7 @@
         <v/>
       </c>
       <c r="M47">
-        <v>45.549220590171586</v>
+        <v>43.49800947910513</v>
       </c>
       <c r="N47" t="str">
         <v/>
@@ -6043,7 +6043,7 @@
         <v/>
       </c>
       <c r="S47">
-        <v>40.284451416773074</v>
+        <v>39.326702269403434</v>
       </c>
     </row>
     <row r="48">
@@ -6066,7 +6066,7 @@
         <v/>
       </c>
       <c r="G48">
-        <v>53.791029218321746</v>
+        <v>45.638426735697855</v>
       </c>
       <c r="H48" t="str">
         <v/>
@@ -6084,7 +6084,7 @@
         <v/>
       </c>
       <c r="M48">
-        <v>45.64469802935522</v>
+        <v>48.59605045346241</v>
       </c>
       <c r="N48" t="str">
         <v/>
@@ -6102,7 +6102,7 @@
         <v/>
       </c>
       <c r="S48">
-        <v>45.657945119550476</v>
+        <v>42.81128033506619</v>
       </c>
     </row>
     <row r="49">
@@ -6125,7 +6125,7 @@
         <v/>
       </c>
       <c r="G49">
-        <v>45.559031730008904</v>
+        <v>52.09905008787595</v>
       </c>
       <c r="H49" t="str">
         <v/>
@@ -6143,7 +6143,7 @@
         <v/>
       </c>
       <c r="M49">
-        <v>47.857535680324986</v>
+        <v>51.06203455642046</v>
       </c>
       <c r="N49" t="str">
         <v/>
@@ -6161,7 +6161,7 @@
         <v/>
       </c>
       <c r="S49">
-        <v>39.22269594450999</v>
+        <v>39.90509730544293</v>
       </c>
     </row>
     <row r="50">
@@ -6184,7 +6184,7 @@
         <v/>
       </c>
       <c r="G50">
-        <v>50.38332609398349</v>
+        <v>53.113617146592645</v>
       </c>
       <c r="H50" t="str">
         <v/>
@@ -6202,7 +6202,7 @@
         <v/>
       </c>
       <c r="M50">
-        <v>50.10471868332391</v>
+        <v>49.87348266362866</v>
       </c>
       <c r="N50" t="str">
         <v/>
@@ -6220,7 +6220,7 @@
         <v/>
       </c>
       <c r="S50">
-        <v>44.922253557280804</v>
+        <v>40.91630382393551</v>
       </c>
     </row>
     <row r="51">

</xml_diff>

<commit_message>
Update with real boiler data
</commit_message>
<xml_diff>
--- a/data/boiler_data.xlsx
+++ b/data/boiler_data.xlsx
@@ -473,46 +473,46 @@
         <v/>
       </c>
       <c r="E2">
-        <v>8.890879082729294</v>
+        <v>9.132840149109207</v>
       </c>
       <c r="F2">
-        <v>4.860802673967096</v>
+        <v>4.455027111619026</v>
       </c>
       <c r="G2">
-        <v>16.262873163802105</v>
+        <v>16.51700414304068</v>
       </c>
       <c r="H2">
-        <v>0.5406844238674164</v>
+        <v>0.5523291223622915</v>
       </c>
       <c r="I2" t="str">
         <v/>
       </c>
       <c r="J2">
-        <v>9.783927131683626</v>
+        <v>9.106871913205241</v>
       </c>
       <c r="K2">
-        <v>4.314000747805599</v>
+        <v>4.651498447185209</v>
       </c>
       <c r="L2">
-        <v>15.915711310122166</v>
+        <v>15.57122709362954</v>
       </c>
       <c r="M2">
-        <v>0.5396326840207543</v>
+        <v>0.4905850783828389</v>
       </c>
       <c r="N2" t="str">
         <v/>
       </c>
       <c r="O2">
-        <v>7.635998111301148</v>
+        <v>6.7348949957603095</v>
       </c>
       <c r="P2">
-        <v>3.8784418493370074</v>
+        <v>3.5801439586279677</v>
       </c>
       <c r="Q2">
-        <v>12.365960909623045</v>
+        <v>13.117156240649848</v>
       </c>
       <c r="R2">
-        <v>0.5101097837002457</v>
+        <v>0.5260529402757772</v>
       </c>
     </row>
     <row r="3">
@@ -529,46 +529,46 @@
         <v/>
       </c>
       <c r="E3">
-        <v>8.881976679506145</v>
+        <v>9.225704555046683</v>
       </c>
       <c r="F3">
-        <v>5.096826099790759</v>
+        <v>4.654677386855184</v>
       </c>
       <c r="G3">
-        <v>18.021003610426416</v>
+        <v>16.784737323911394</v>
       </c>
       <c r="H3">
-        <v>0.5935862898771422</v>
+        <v>0.5933825469022809</v>
       </c>
       <c r="I3" t="str">
         <v/>
       </c>
       <c r="J3">
-        <v>8.132007452878128</v>
+        <v>8.767076006706272</v>
       </c>
       <c r="K3">
-        <v>4.710474877508848</v>
+        <v>4.8969354178491065</v>
       </c>
       <c r="L3">
-        <v>15.81302367919253</v>
+        <v>16.496101600953637</v>
       </c>
       <c r="M3">
-        <v>0.5086228356615505</v>
+        <v>0.518143704816091</v>
       </c>
       <c r="N3" t="str">
         <v/>
       </c>
       <c r="O3">
-        <v>7.570248217895283</v>
+        <v>7.6610485621250834</v>
       </c>
       <c r="P3">
-        <v>3.687352753792666</v>
+        <v>3.7303373484403273</v>
       </c>
       <c r="Q3">
-        <v>13.301607622400496</v>
+        <v>13.363354370412079</v>
       </c>
       <c r="R3">
-        <v>0.4921138130260491</v>
+        <v>0.5593024981937204</v>
       </c>
     </row>
     <row r="4">
@@ -585,46 +585,46 @@
         <v/>
       </c>
       <c r="E4">
-        <v>9.54402311863312</v>
+        <v>10.014789310734953</v>
       </c>
       <c r="F4">
-        <v>4.442814379062537</v>
+        <v>4.340839598565718</v>
       </c>
       <c r="G4">
-        <v>16.11082866909953</v>
+        <v>16.217299537091936</v>
       </c>
       <c r="H4">
-        <v>0.5143677605090159</v>
+        <v>0.5696139049358899</v>
       </c>
       <c r="I4" t="str">
         <v/>
       </c>
       <c r="J4">
-        <v>9.06702678904676</v>
+        <v>9.603851928391864</v>
       </c>
       <c r="K4">
-        <v>4.473103914188908</v>
+        <v>4.016504464767127</v>
       </c>
       <c r="L4">
-        <v>15.513979887096045</v>
+        <v>15.398820801703426</v>
       </c>
       <c r="M4">
-        <v>0.5376438732558</v>
+        <v>0.516460054848047</v>
       </c>
       <c r="N4" t="str">
         <v/>
       </c>
       <c r="O4">
-        <v>7.027579971452461</v>
+        <v>7.806369993063056</v>
       </c>
       <c r="P4">
-        <v>3.8954912176166747</v>
+        <v>3.3471619316831407</v>
       </c>
       <c r="Q4">
-        <v>12.151227071482356</v>
+        <v>13.333205879744476</v>
       </c>
       <c r="R4">
-        <v>0.5686818076117262</v>
+        <v>0.5788694071994186</v>
       </c>
     </row>
     <row r="5">
@@ -641,46 +641,46 @@
         <v/>
       </c>
       <c r="E5">
-        <v>10.197742271205428</v>
+        <v>9.06944952119089</v>
       </c>
       <c r="F5">
-        <v>4.48280776095761</v>
+        <v>4.505019615183823</v>
       </c>
       <c r="G5">
-        <v>17.231068231476435</v>
+        <v>17.020129406443107</v>
       </c>
       <c r="H5">
-        <v>0.5577103768995016</v>
+        <v>0.5622469501819493</v>
       </c>
       <c r="I5" t="str">
         <v/>
       </c>
       <c r="J5">
-        <v>8.18462858111702</v>
+        <v>8.408502782415535</v>
       </c>
       <c r="K5">
-        <v>4.268772982097925</v>
+        <v>4.714095736862777</v>
       </c>
       <c r="L5">
-        <v>15.285068797459298</v>
+        <v>15.58697163389578</v>
       </c>
       <c r="M5">
-        <v>0.5338370960177631</v>
+        <v>0.5154826262995087</v>
       </c>
       <c r="N5" t="str">
         <v/>
       </c>
       <c r="O5">
-        <v>6.9159688177660446</v>
+        <v>7.352572836825668</v>
       </c>
       <c r="P5">
-        <v>3.8711647868173404</v>
+        <v>3.7345511897280863</v>
       </c>
       <c r="Q5">
-        <v>13.56057052828054</v>
+        <v>12.471524397681714</v>
       </c>
       <c r="R5">
-        <v>0.5713048955723024</v>
+        <v>0.5504932108551336</v>
       </c>
     </row>
     <row r="6">
@@ -697,46 +697,46 @@
         <v/>
       </c>
       <c r="E6">
-        <v>9.79094259978337</v>
+        <v>10.099150962832814</v>
       </c>
       <c r="F6">
-        <v>5.081617269103159</v>
+        <v>4.748413032961232</v>
       </c>
       <c r="G6">
-        <v>18.010812065097834</v>
+        <v>17.10492376131761</v>
       </c>
       <c r="H6">
-        <v>0.5340949804719686</v>
+        <v>0.5894014347394702</v>
       </c>
       <c r="I6" t="str">
         <v/>
       </c>
       <c r="J6">
-        <v>7.872970310729137</v>
+        <v>9.448374489052304</v>
       </c>
       <c r="K6">
-        <v>4.336477088201533</v>
+        <v>4.289802972745735</v>
       </c>
       <c r="L6">
-        <v>16.924309856414</v>
+        <v>16.45741912589199</v>
       </c>
       <c r="M6">
-        <v>0.532738173826799</v>
+        <v>0.5074201123243939</v>
       </c>
       <c r="N6" t="str">
         <v/>
       </c>
       <c r="O6">
-        <v>6.518215542731838</v>
+        <v>7.983959932688135</v>
       </c>
       <c r="P6">
-        <v>3.3304672508688635</v>
+        <v>3.259942794948668</v>
       </c>
       <c r="Q6">
-        <v>12.363989096272617</v>
+        <v>13.48020199947697</v>
       </c>
       <c r="R6">
-        <v>0.48883777226223607</v>
+        <v>0.5399019453850553</v>
       </c>
     </row>
     <row r="7">
@@ -753,46 +753,46 @@
         <v/>
       </c>
       <c r="E7">
-        <v>10.194116088834194</v>
+        <v>10.289069317123515</v>
       </c>
       <c r="F7">
-        <v>4.736965403330786</v>
+        <v>5.083901073651989</v>
       </c>
       <c r="G7">
-        <v>16.301422758772585</v>
+        <v>17.237238404562294</v>
       </c>
       <c r="H7">
-        <v>0.5398276204846395</v>
+        <v>0.5024071867577697</v>
       </c>
       <c r="I7" t="str">
         <v/>
       </c>
       <c r="J7">
-        <v>9.528315857669007</v>
+        <v>8.366654259997775</v>
       </c>
       <c r="K7">
-        <v>4.429305461282567</v>
+        <v>4.8118335502890135</v>
       </c>
       <c r="L7">
-        <v>17.095573295754445</v>
+        <v>16.81353383905171</v>
       </c>
       <c r="M7">
-        <v>0.5612503047318183</v>
+        <v>0.4920758764217669</v>
       </c>
       <c r="N7" t="str">
         <v/>
       </c>
       <c r="O7">
-        <v>7.317304279458927</v>
+        <v>6.602838370716001</v>
       </c>
       <c r="P7">
-        <v>3.2068443533653794</v>
+        <v>3.5821612770084204</v>
       </c>
       <c r="Q7">
-        <v>12.435066858949668</v>
+        <v>12.221175676174271</v>
       </c>
       <c r="R7">
-        <v>0.5114050724486651</v>
+        <v>0.4976999004403809</v>
       </c>
     </row>
     <row r="8">
@@ -809,46 +809,46 @@
         <v/>
       </c>
       <c r="E8">
-        <v>8.939499215264243</v>
+        <v>8.56580858077187</v>
       </c>
       <c r="F8">
-        <v>4.821389861785144</v>
+        <v>5.012980766052019</v>
       </c>
       <c r="G8">
-        <v>18.020685606585502</v>
+        <v>16.459646788315794</v>
       </c>
       <c r="H8">
-        <v>0.5613330002774817</v>
+        <v>0.5161267500079324</v>
       </c>
       <c r="I8" t="str">
         <v/>
       </c>
       <c r="J8">
-        <v>8.077296136731643</v>
+        <v>9.124653311450826</v>
       </c>
       <c r="K8">
-        <v>4.355132817381211</v>
+        <v>4.166342612408445</v>
       </c>
       <c r="L8">
-        <v>16.123171551751504</v>
+        <v>16.955395186197432</v>
       </c>
       <c r="M8">
-        <v>0.5713544848434626</v>
+        <v>0.5819026412002151</v>
       </c>
       <c r="N8" t="str">
         <v/>
       </c>
       <c r="O8">
-        <v>6.753526965039562</v>
+        <v>7.507576219738063</v>
       </c>
       <c r="P8">
-        <v>3.6667216712042427</v>
+        <v>3.481204137690495</v>
       </c>
       <c r="Q8">
-        <v>12.173787158267409</v>
+        <v>13.496039386476484</v>
       </c>
       <c r="R8">
-        <v>0.5067615302138856</v>
+        <v>0.48436503573167394</v>
       </c>
     </row>
     <row r="9">
@@ -865,46 +865,46 @@
         <v/>
       </c>
       <c r="E9">
-        <v>10.342881116979747</v>
+        <v>9.402456424135563</v>
       </c>
       <c r="F9">
-        <v>4.420858287029077</v>
+        <v>4.899244594053365</v>
       </c>
       <c r="G9">
-        <v>16.553228452630897</v>
+        <v>18.008087779528967</v>
       </c>
       <c r="H9">
-        <v>0.5174544951950707</v>
+        <v>0.5794173544482641</v>
       </c>
       <c r="I9" t="str">
         <v/>
       </c>
       <c r="J9">
-        <v>8.303209671721357</v>
+        <v>9.131968923154474</v>
       </c>
       <c r="K9">
-        <v>4.307335760306129</v>
+        <v>3.923518968006828</v>
       </c>
       <c r="L9">
-        <v>16.611832001616765</v>
+        <v>16.84584839234836</v>
       </c>
       <c r="M9">
-        <v>0.5685344730127614</v>
+        <v>0.5696598329797763</v>
       </c>
       <c r="N9" t="str">
         <v/>
       </c>
       <c r="O9">
-        <v>7.949198700673985</v>
+        <v>6.701112967272509</v>
       </c>
       <c r="P9">
-        <v>3.4703579339599457</v>
+        <v>3.468068193072838</v>
       </c>
       <c r="Q9">
-        <v>13.567678014891918</v>
+        <v>12.767227034180365</v>
       </c>
       <c r="R9">
-        <v>0.5556699136136738</v>
+        <v>0.5749910025685105</v>
       </c>
     </row>
     <row r="10">
@@ -921,46 +921,46 @@
         <v/>
       </c>
       <c r="E10">
-        <v>9.837248460295834</v>
+        <v>10.12181503828183</v>
       </c>
       <c r="F10">
-        <v>4.867396038901182</v>
+        <v>4.841972016955538</v>
       </c>
       <c r="G10">
-        <v>18.00864132879815</v>
+        <v>17.34336265484933</v>
       </c>
       <c r="H10">
-        <v>0.5694647423574528</v>
+        <v>0.5375518602957811</v>
       </c>
       <c r="I10" t="str">
         <v/>
       </c>
       <c r="J10">
-        <v>8.920250175700836</v>
+        <v>9.735279139027341</v>
       </c>
       <c r="K10">
-        <v>4.68225397642</v>
+        <v>4.030205239525226</v>
       </c>
       <c r="L10">
-        <v>16.71068318493939</v>
+        <v>15.2549470949152</v>
       </c>
       <c r="M10">
-        <v>0.580518283035966</v>
+        <v>0.5059176237361791</v>
       </c>
       <c r="N10" t="str">
         <v/>
       </c>
       <c r="O10">
-        <v>7.949757007091181</v>
+        <v>7.473038829157042</v>
       </c>
       <c r="P10">
-        <v>3.4938054378411194</v>
+        <v>3.6671591862375426</v>
       </c>
       <c r="Q10">
-        <v>12.374382209219664</v>
+        <v>13.510653787439704</v>
       </c>
       <c r="R10">
-        <v>0.5620532040134144</v>
+        <v>0.5086004802463872</v>
       </c>
     </row>
     <row r="11">
@@ -977,46 +977,46 @@
         <v/>
       </c>
       <c r="E11">
-        <v>10.0333083203245</v>
+        <v>8.501147443262173</v>
       </c>
       <c r="F11">
-        <v>4.364016872499079</v>
+        <v>5.065068623983479</v>
       </c>
       <c r="G11">
-        <v>17.826664350125487</v>
+        <v>16.864205631340386</v>
       </c>
       <c r="H11">
-        <v>0.5013524647584686</v>
+        <v>0.5542305137235434</v>
       </c>
       <c r="I11" t="str">
         <v/>
       </c>
       <c r="J11">
-        <v>8.018410675885042</v>
+        <v>9.30207857345809</v>
       </c>
       <c r="K11">
-        <v>4.042041592331923</v>
+        <v>4.029314234265675</v>
       </c>
       <c r="L11">
-        <v>15.285673620340262</v>
+        <v>15.851042865631314</v>
       </c>
       <c r="M11">
-        <v>0.5571736779326993</v>
+        <v>0.5559085852541489</v>
       </c>
       <c r="N11" t="str">
         <v/>
       </c>
       <c r="O11">
-        <v>6.604005281411325</v>
+        <v>7.11394254712137</v>
       </c>
       <c r="P11">
-        <v>3.223704599454152</v>
+        <v>3.3634413675218378</v>
       </c>
       <c r="Q11">
-        <v>13.513337094273476</v>
+        <v>13.154719133684187</v>
       </c>
       <c r="R11">
-        <v>0.5192341562925644</v>
+        <v>0.5602019751217974</v>
       </c>
     </row>
     <row r="12">
@@ -1033,46 +1033,46 @@
         <v/>
       </c>
       <c r="E12">
-        <v>9.187997532389485</v>
+        <v>10.117543867192051</v>
       </c>
       <c r="F12">
-        <v>4.267861458867716</v>
+        <v>4.869052441192461</v>
       </c>
       <c r="G12">
-        <v>18.060920024373452</v>
+        <v>17.92065380856405</v>
       </c>
       <c r="H12">
-        <v>0.5280341586280326</v>
+        <v>0.5807263201518753</v>
       </c>
       <c r="I12" t="str">
         <v/>
       </c>
       <c r="J12">
-        <v>8.125250287171138</v>
+        <v>8.978806708430138</v>
       </c>
       <c r="K12">
-        <v>4.130131069453505</v>
+        <v>4.238000066019834</v>
       </c>
       <c r="L12">
-        <v>16.219926206925148</v>
+        <v>16.8149864334859</v>
       </c>
       <c r="M12">
-        <v>0.4914712540260468</v>
+        <v>0.5305122279900012</v>
       </c>
       <c r="N12" t="str">
         <v/>
       </c>
       <c r="O12">
-        <v>7.024067904499752</v>
+        <v>7.743668678869486</v>
       </c>
       <c r="P12">
-        <v>3.770997511181889</v>
+        <v>3.6590243661201827</v>
       </c>
       <c r="Q12">
-        <v>12.754349834000937</v>
+        <v>12.748799566622122</v>
       </c>
       <c r="R12">
-        <v>0.5345744457575683</v>
+        <v>0.5234315750124525</v>
       </c>
     </row>
     <row r="13">
@@ -1089,46 +1089,46 @@
         <v/>
       </c>
       <c r="E13">
-        <v>8.587445958663187</v>
+        <v>9.190699184306043</v>
       </c>
       <c r="F13">
-        <v>5.055690521905313</v>
+        <v>4.234353285818713</v>
       </c>
       <c r="G13">
-        <v>16.34833841618239</v>
+        <v>16.84118234076213</v>
       </c>
       <c r="H13">
-        <v>0.5522648364791506</v>
+        <v>0.5287766709806073</v>
       </c>
       <c r="I13" t="str">
         <v/>
       </c>
       <c r="J13">
-        <v>8.395012864261343</v>
+        <v>7.904234242941</v>
       </c>
       <c r="K13">
-        <v>4.802020714739774</v>
+        <v>3.9228973930354707</v>
       </c>
       <c r="L13">
-        <v>17.155577925384204</v>
+        <v>15.474379532397867</v>
       </c>
       <c r="M13">
-        <v>0.49452771294766495</v>
+        <v>0.5547778452880805</v>
       </c>
       <c r="N13" t="str">
         <v/>
       </c>
       <c r="O13">
-        <v>7.805783781537004</v>
+        <v>7.794449153912069</v>
       </c>
       <c r="P13">
-        <v>3.8017567715641736</v>
+        <v>3.3216471075356804</v>
       </c>
       <c r="Q13">
-        <v>12.960991516598671</v>
+        <v>13.013133987563354</v>
       </c>
       <c r="R13">
-        <v>0.5360845239984741</v>
+        <v>0.5773123105310125</v>
       </c>
     </row>
     <row r="14">
@@ -1145,46 +1145,46 @@
         <v/>
       </c>
       <c r="E14">
-        <v>8.86547260325833</v>
+        <v>9.606947406637868</v>
       </c>
       <c r="F14">
-        <v>4.943758573755068</v>
+        <v>5.011643568524335</v>
       </c>
       <c r="G14">
-        <v>17.440073163762843</v>
+        <v>16.429701043913383</v>
       </c>
       <c r="H14">
-        <v>0.5861469124167833</v>
+        <v>0.5295609436159836</v>
       </c>
       <c r="I14" t="str">
         <v/>
       </c>
       <c r="J14">
-        <v>9.205731384531518</v>
+        <v>9.194111830671519</v>
       </c>
       <c r="K14">
-        <v>4.177115602786635</v>
+        <v>4.447876889640256</v>
       </c>
       <c r="L14">
-        <v>15.404941257041193</v>
+        <v>15.895033884393193</v>
       </c>
       <c r="M14">
-        <v>0.5806198111927044</v>
+        <v>0.5248059601000297</v>
       </c>
       <c r="N14" t="str">
         <v/>
       </c>
       <c r="O14">
-        <v>6.6860215457636905</v>
+        <v>7.009889603764871</v>
       </c>
       <c r="P14">
-        <v>3.847460195207458</v>
+        <v>3.2942953170097926</v>
       </c>
       <c r="Q14">
-        <v>13.103910508778466</v>
+        <v>13.355566112264395</v>
       </c>
       <c r="R14">
-        <v>0.5139483046238648</v>
+        <v>0.5688520380049835</v>
       </c>
     </row>
     <row r="15">
@@ -1201,46 +1201,46 @@
         <v/>
       </c>
       <c r="E15">
-        <v>10.072024632731829</v>
+        <v>8.873924757245874</v>
       </c>
       <c r="F15">
-        <v>4.650685134477794</v>
+        <v>4.584631238349367</v>
       </c>
       <c r="G15">
-        <v>16.942989163237904</v>
+        <v>16.90183653071174</v>
       </c>
       <c r="H15">
-        <v>0.591352378640242</v>
+        <v>0.5681547959648542</v>
       </c>
       <c r="I15" t="str">
         <v/>
       </c>
       <c r="J15">
-        <v>8.986602135979986</v>
+        <v>9.762470579809193</v>
       </c>
       <c r="K15">
-        <v>4.389775897643873</v>
+        <v>4.865270833257868</v>
       </c>
       <c r="L15">
-        <v>16.611161033567534</v>
+        <v>17.078154512780767</v>
       </c>
       <c r="M15">
-        <v>0.5185586059496093</v>
+        <v>0.5425529564339594</v>
       </c>
       <c r="N15" t="str">
         <v/>
       </c>
       <c r="O15">
-        <v>7.374141110509665</v>
+        <v>7.688471031537349</v>
       </c>
       <c r="P15">
-        <v>3.3450459429435915</v>
+        <v>3.6874849169091806</v>
       </c>
       <c r="Q15">
-        <v>12.317410317416945</v>
+        <v>12.576909458854177</v>
       </c>
       <c r="R15">
-        <v>0.5421913382909656</v>
+        <v>0.5153397436852175</v>
       </c>
     </row>
     <row r="16">
@@ -1257,46 +1257,46 @@
         <v/>
       </c>
       <c r="E16">
-        <v>8.806021836603096</v>
+        <v>9.804688375545963</v>
       </c>
       <c r="F16">
-        <v>4.709417084263038</v>
+        <v>4.58148732335162</v>
       </c>
       <c r="G16">
-        <v>16.298980506723996</v>
+        <v>17.253131325905827</v>
       </c>
       <c r="H16">
-        <v>0.5920802764901839</v>
+        <v>0.5546292361761973</v>
       </c>
       <c r="I16" t="str">
         <v/>
       </c>
       <c r="J16">
-        <v>8.18281745068473</v>
+        <v>9.28842469488092</v>
       </c>
       <c r="K16">
-        <v>3.9297701196522947</v>
+        <v>4.727480423512902</v>
       </c>
       <c r="L16">
-        <v>16.501206007668415</v>
+        <v>15.358420913934248</v>
       </c>
       <c r="M16">
-        <v>0.5600751074805936</v>
+        <v>0.5848692704229008</v>
       </c>
       <c r="N16" t="str">
         <v/>
       </c>
       <c r="O16">
-        <v>7.283845286945162</v>
+        <v>7.078761789269267</v>
       </c>
       <c r="P16">
-        <v>3.584846716194323</v>
+        <v>3.346222567117718</v>
       </c>
       <c r="Q16">
-        <v>12.67335161363835</v>
+        <v>13.286438773600295</v>
       </c>
       <c r="R16">
-        <v>0.5052221268800259</v>
+        <v>0.5393625599171752</v>
       </c>
     </row>
     <row r="17">
@@ -1313,46 +1313,46 @@
         <v/>
       </c>
       <c r="E17">
-        <v>9.899588959692268</v>
+        <v>10.215895062464483</v>
       </c>
       <c r="F17">
-        <v>4.795351984660146</v>
+        <v>4.340634346908095</v>
       </c>
       <c r="G17">
-        <v>17.978802503640313</v>
+        <v>16.5287294831667</v>
       </c>
       <c r="H17">
-        <v>0.5122458513500773</v>
+        <v>0.5117447382277576</v>
       </c>
       <c r="I17" t="str">
         <v/>
       </c>
       <c r="J17">
-        <v>7.841043499853786</v>
+        <v>7.920371617005072</v>
       </c>
       <c r="K17">
-        <v>4.110194729193563</v>
+        <v>4.8841834206784425</v>
       </c>
       <c r="L17">
-        <v>16.118809001407385</v>
+        <v>16.07583148898697</v>
       </c>
       <c r="M17">
-        <v>0.5383236221541379</v>
+        <v>0.5454334881717177</v>
       </c>
       <c r="N17" t="str">
         <v/>
       </c>
       <c r="O17">
-        <v>7.167506068784217</v>
+        <v>6.9449294289431265</v>
       </c>
       <c r="P17">
-        <v>3.975164503726287</v>
+        <v>3.3301876961009707</v>
       </c>
       <c r="Q17">
-        <v>13.014436951719828</v>
+        <v>13.442738961404306</v>
       </c>
       <c r="R17">
-        <v>0.5160830690832596</v>
+        <v>0.5390151233404982</v>
       </c>
     </row>
     <row r="18">
@@ -1369,46 +1369,46 @@
         <v/>
       </c>
       <c r="E18">
-        <v>9.966425239610707</v>
+        <v>8.59557866894725</v>
       </c>
       <c r="F18">
-        <v>4.734033836455168</v>
+        <v>4.706826350590939</v>
       </c>
       <c r="G18">
-        <v>17.17269066039714</v>
+        <v>16.58780481885685</v>
       </c>
       <c r="H18">
-        <v>0.5799750900492464</v>
+        <v>0.5824635913981563</v>
       </c>
       <c r="I18" t="str">
         <v/>
       </c>
       <c r="J18">
-        <v>8.290074510960608</v>
+        <v>9.645688105869175</v>
       </c>
       <c r="K18">
-        <v>3.9231220684610317</v>
+        <v>4.692863125850719</v>
       </c>
       <c r="L18">
-        <v>17.057557258182666</v>
+        <v>16.289877051561724</v>
       </c>
       <c r="M18">
-        <v>0.5557191067968404</v>
+        <v>0.5299223345935101</v>
       </c>
       <c r="N18" t="str">
         <v/>
       </c>
       <c r="O18">
-        <v>7.9523279719127435</v>
+        <v>7.052185064806615</v>
       </c>
       <c r="P18">
-        <v>3.6878895536054626</v>
+        <v>3.7746916353359903</v>
       </c>
       <c r="Q18">
-        <v>12.478377289035137</v>
+        <v>12.392623074843884</v>
       </c>
       <c r="R18">
-        <v>0.5282393342976428</v>
+        <v>0.5302328875734261</v>
       </c>
     </row>
     <row r="19">
@@ -1425,46 +1425,46 @@
         <v/>
       </c>
       <c r="E19">
-        <v>9.767619752954257</v>
+        <v>9.248451455166517</v>
       </c>
       <c r="F19">
-        <v>4.817905530642235</v>
+        <v>5.140007828150244</v>
       </c>
       <c r="G19">
-        <v>17.062614841150683</v>
+        <v>16.413012726115646</v>
       </c>
       <c r="H19">
-        <v>0.5144433350244292</v>
+        <v>0.5245711791478334</v>
       </c>
       <c r="I19" t="str">
         <v/>
       </c>
       <c r="J19">
-        <v>7.942162634049533</v>
+        <v>8.8860842745278</v>
       </c>
       <c r="K19">
-        <v>4.6477044508021</v>
+        <v>4.784079020327381</v>
       </c>
       <c r="L19">
-        <v>15.255397669133503</v>
+        <v>15.44199759185373</v>
       </c>
       <c r="M19">
-        <v>0.5282667404382885</v>
+        <v>0.5341793150130046</v>
       </c>
       <c r="N19" t="str">
         <v/>
       </c>
       <c r="O19">
-        <v>7.052777031933765</v>
+        <v>7.483524700786214</v>
       </c>
       <c r="P19">
-        <v>3.725657901011739</v>
+        <v>3.6392739632439515</v>
       </c>
       <c r="Q19">
-        <v>12.568333493145236</v>
+        <v>12.719493412047285</v>
       </c>
       <c r="R19">
-        <v>0.5374411327406361</v>
+        <v>0.5348059989419218</v>
       </c>
     </row>
     <row r="20">
@@ -1481,46 +1481,46 @@
         <v/>
       </c>
       <c r="E20">
-        <v>8.925658444505702</v>
+        <v>10.387849588248182</v>
       </c>
       <c r="F20">
-        <v>4.225950031274283</v>
+        <v>4.865899853951385</v>
       </c>
       <c r="G20">
-        <v>16.36875235393963</v>
+        <v>16.178678922550993</v>
       </c>
       <c r="H20">
-        <v>0.5425329361170296</v>
+        <v>0.5562176249690022</v>
       </c>
       <c r="I20" t="str">
         <v/>
       </c>
       <c r="J20">
-        <v>9.192695662361434</v>
+        <v>9.2209526033134</v>
       </c>
       <c r="K20">
-        <v>4.126908671072094</v>
+        <v>4.634910192972166</v>
       </c>
       <c r="L20">
-        <v>15.244402969985824</v>
+        <v>16.23196538783096</v>
       </c>
       <c r="M20">
-        <v>0.575423885522899</v>
+        <v>0.5863912702613965</v>
       </c>
       <c r="N20" t="str">
         <v/>
       </c>
       <c r="O20">
-        <v>6.711198564880504</v>
+        <v>7.263137628026849</v>
       </c>
       <c r="P20">
-        <v>3.976839449330586</v>
+        <v>3.2937836091936163</v>
       </c>
       <c r="Q20">
-        <v>13.162614216781874</v>
+        <v>13.448888184438598</v>
       </c>
       <c r="R20">
-        <v>0.5708011275226565</v>
+        <v>0.5032140155208806</v>
       </c>
     </row>
     <row r="21">
@@ -1537,46 +1537,46 @@
         <v/>
       </c>
       <c r="E21">
-        <v>10.229734778691213</v>
+        <v>9.621588545647732</v>
       </c>
       <c r="F21">
-        <v>4.285686460593996</v>
+        <v>5.0734450840420156</v>
       </c>
       <c r="G21">
-        <v>17.723664862812278</v>
+        <v>17.38486393809882</v>
       </c>
       <c r="H21">
-        <v>0.5608648450077026</v>
+        <v>0.5580130330954753</v>
       </c>
       <c r="I21" t="str">
         <v/>
       </c>
       <c r="J21">
-        <v>8.652225118381267</v>
+        <v>9.330110347258408</v>
       </c>
       <c r="K21">
-        <v>4.6719501496088265</v>
+        <v>4.10294957080733</v>
       </c>
       <c r="L21">
-        <v>16.046732561399676</v>
+        <v>16.30317551819943</v>
       </c>
       <c r="M21">
-        <v>0.5832737979675064</v>
+        <v>0.5887859756752001</v>
       </c>
       <c r="N21" t="str">
         <v/>
       </c>
       <c r="O21">
-        <v>7.67454528074467</v>
+        <v>6.59892315501163</v>
       </c>
       <c r="P21">
-        <v>3.6133592258981495</v>
+        <v>3.5395340444995966</v>
       </c>
       <c r="Q21">
-        <v>13.499259383082117</v>
+        <v>12.550657282496987</v>
       </c>
       <c r="R21">
-        <v>0.5133668023296021</v>
+        <v>0.5014214097056423</v>
       </c>
     </row>
     <row r="22">
@@ -1593,46 +1593,46 @@
         <v/>
       </c>
       <c r="E22">
-        <v>10.253231134077996</v>
+        <v>9.853998623267543</v>
       </c>
       <c r="F22">
-        <v>4.2182336204016675</v>
+        <v>5.03562651949385</v>
       </c>
       <c r="G22">
-        <v>16.71533228494345</v>
+        <v>17.28161748313032</v>
       </c>
       <c r="H22">
-        <v>0.5423395055365258</v>
+        <v>0.5171613146191396</v>
       </c>
       <c r="I22" t="str">
         <v/>
       </c>
       <c r="J22">
-        <v>8.51732198581433</v>
+        <v>9.050424888786615</v>
       </c>
       <c r="K22">
-        <v>3.9841177861331003</v>
+        <v>4.256056429805879</v>
       </c>
       <c r="L22">
-        <v>15.791723924401571</v>
+        <v>15.703139670290513</v>
       </c>
       <c r="M22">
-        <v>0.5490668771887272</v>
+        <v>0.5554264776148083</v>
       </c>
       <c r="N22" t="str">
         <v/>
       </c>
       <c r="O22">
-        <v>7.481695916739408</v>
+        <v>7.320394829216463</v>
       </c>
       <c r="P22">
-        <v>3.2262380811758216</v>
+        <v>3.403475324208346</v>
       </c>
       <c r="Q22">
-        <v>13.123273290111456</v>
+        <v>13.233778342309872</v>
       </c>
       <c r="R22">
-        <v>0.5448441315057434</v>
+        <v>0.5715964533632831</v>
       </c>
     </row>
     <row r="23">
@@ -1649,46 +1649,46 @@
         <v/>
       </c>
       <c r="E23">
-        <v>9.38507401376092</v>
+        <v>9.095097876325124</v>
       </c>
       <c r="F23">
-        <v>4.598605429220312</v>
+        <v>4.616662192427799</v>
       </c>
       <c r="G23">
-        <v>16.715140283472934</v>
+        <v>17.34217217459627</v>
       </c>
       <c r="H23">
-        <v>0.5199875725253049</v>
+        <v>0.5066331254635423</v>
       </c>
       <c r="I23" t="str">
         <v/>
       </c>
       <c r="J23">
-        <v>9.101607957905323</v>
+        <v>8.00333781428581</v>
       </c>
       <c r="K23">
-        <v>4.732781244841226</v>
+        <v>4.298808575017171</v>
       </c>
       <c r="L23">
-        <v>15.759689570254274</v>
+        <v>16.45882217031726</v>
       </c>
       <c r="M23">
-        <v>0.5442213093658559</v>
+        <v>0.5296850065646168</v>
       </c>
       <c r="N23" t="str">
         <v/>
       </c>
       <c r="O23">
-        <v>7.476137117455097</v>
+        <v>7.476970919900877</v>
       </c>
       <c r="P23">
-        <v>3.4466018090954442</v>
+        <v>3.227177123575971</v>
       </c>
       <c r="Q23">
-        <v>12.470594532675975</v>
+        <v>12.454340297962567</v>
       </c>
       <c r="R23">
-        <v>0.5616405132954619</v>
+        <v>0.5611971662140885</v>
       </c>
     </row>
     <row r="24">
@@ -1705,46 +1705,46 @@
         <v/>
       </c>
       <c r="E24">
-        <v>8.667315716544277</v>
+        <v>10.20794824625215</v>
       </c>
       <c r="F24">
-        <v>4.68499795503043</v>
+        <v>4.218274434811212</v>
       </c>
       <c r="G24">
-        <v>17.36607246259243</v>
+        <v>16.81966970169846</v>
       </c>
       <c r="H24">
-        <v>0.5216818203057187</v>
+        <v>0.5282831795899308</v>
       </c>
       <c r="I24" t="str">
         <v/>
       </c>
       <c r="J24">
-        <v>9.050753214201395</v>
+        <v>9.33421993562669</v>
       </c>
       <c r="K24">
-        <v>4.647335095323891</v>
+        <v>4.673383055804196</v>
       </c>
       <c r="L24">
-        <v>15.486134537229226</v>
+        <v>15.82278754838461</v>
       </c>
       <c r="M24">
-        <v>0.5454943214115809</v>
+        <v>0.4980012871971249</v>
       </c>
       <c r="N24" t="str">
         <v/>
       </c>
       <c r="O24">
-        <v>7.9871689096325955</v>
+        <v>6.731007484226553</v>
       </c>
       <c r="P24">
-        <v>3.3791809359698037</v>
+        <v>3.426091621557241</v>
       </c>
       <c r="Q24">
-        <v>13.570077319877887</v>
+        <v>12.891772527676347</v>
       </c>
       <c r="R24">
-        <v>0.573541612325708</v>
+        <v>0.537319359377432</v>
       </c>
     </row>
     <row r="25">
@@ -1761,46 +1761,46 @@
         <v/>
       </c>
       <c r="E25">
-        <v>10.217945052741289</v>
+        <v>10.066091505724732</v>
       </c>
       <c r="F25">
-        <v>4.462924369362575</v>
+        <v>4.492005307989815</v>
       </c>
       <c r="G25">
-        <v>18.09883351423739</v>
+        <v>16.994118294844778</v>
       </c>
       <c r="H25">
-        <v>0.5066200813460591</v>
+        <v>0.5678025434320522</v>
       </c>
       <c r="I25" t="str">
         <v/>
       </c>
       <c r="J25">
-        <v>9.691835716598794</v>
+        <v>9.16707459493948</v>
       </c>
       <c r="K25">
-        <v>4.138508924775939</v>
+        <v>4.66660356260163</v>
       </c>
       <c r="L25">
-        <v>16.0689519465586</v>
+        <v>15.300895500125215</v>
       </c>
       <c r="M25">
-        <v>0.5061920128049211</v>
+        <v>0.5009342792696244</v>
       </c>
       <c r="N25" t="str">
         <v/>
       </c>
       <c r="O25">
-        <v>7.381367232743108</v>
+        <v>7.270495578001102</v>
       </c>
       <c r="P25">
-        <v>3.5402760341693202</v>
+        <v>3.8831598528175872</v>
       </c>
       <c r="Q25">
-        <v>13.439786848608348</v>
+        <v>12.180656229607752</v>
       </c>
       <c r="R25">
-        <v>0.5134422334023999</v>
+        <v>0.4890503782246188</v>
       </c>
     </row>
     <row r="26">
@@ -1817,46 +1817,46 @@
         <v/>
       </c>
       <c r="E26">
-        <v>9.996783985415663</v>
+        <v>10.328008639701007</v>
       </c>
       <c r="F26">
-        <v>4.563395895368483</v>
+        <v>4.834046836072155</v>
       </c>
       <c r="G26">
-        <v>16.45110755113595</v>
+        <v>16.98271718780764</v>
       </c>
       <c r="H26">
-        <v>0.546256149169632</v>
+        <v>0.5060457928961613</v>
       </c>
       <c r="I26" t="str">
         <v/>
       </c>
       <c r="J26">
-        <v>8.771109426427639</v>
+        <v>7.826252147606313</v>
       </c>
       <c r="K26">
-        <v>4.069571176779293</v>
+        <v>4.23939818794326</v>
       </c>
       <c r="L26">
-        <v>16.974704147181168</v>
+        <v>16.26935712450077</v>
       </c>
       <c r="M26">
-        <v>0.5875892805299717</v>
+        <v>0.5146768579436632</v>
       </c>
       <c r="N26" t="str">
         <v/>
       </c>
       <c r="O26">
-        <v>7.059599150079948</v>
+        <v>7.449366644344939</v>
       </c>
       <c r="P26">
-        <v>3.3821838006747553</v>
+        <v>3.971747820032155</v>
       </c>
       <c r="Q26">
-        <v>12.792298009005684</v>
+        <v>12.611474015929955</v>
       </c>
       <c r="R26">
-        <v>0.5402210502258178</v>
+        <v>0.4952561846511468</v>
       </c>
     </row>
     <row r="27">
@@ -1873,46 +1873,46 @@
         <v/>
       </c>
       <c r="E27">
-        <v>10.036604203878682</v>
+        <v>9.900186720760852</v>
       </c>
       <c r="F27">
-        <v>4.461783255964593</v>
+        <v>4.784140301560927</v>
       </c>
       <c r="G27">
-        <v>17.50944509558804</v>
+        <v>18.080870927910805</v>
       </c>
       <c r="H27">
-        <v>0.5440585914837007</v>
+        <v>0.5693231207057978</v>
       </c>
       <c r="I27" t="str">
         <v/>
       </c>
       <c r="J27">
-        <v>9.23242894483856</v>
+        <v>9.723137123535654</v>
       </c>
       <c r="K27">
-        <v>4.524065678714591</v>
+        <v>4.277997297609106</v>
       </c>
       <c r="L27">
-        <v>16.004302765436215</v>
+        <v>16.753348615974286</v>
       </c>
       <c r="M27">
-        <v>0.5198961008770517</v>
+        <v>0.5335832832711869</v>
       </c>
       <c r="N27" t="str">
         <v/>
       </c>
       <c r="O27">
-        <v>7.3431532347699315</v>
+        <v>7.365448218035809</v>
       </c>
       <c r="P27">
-        <v>3.406755495543352</v>
+        <v>3.8112838028851894</v>
       </c>
       <c r="Q27">
-        <v>12.81053159927983</v>
+        <v>12.482550251703591</v>
       </c>
       <c r="R27">
-        <v>0.571919360320509</v>
+        <v>0.49298943327660594</v>
       </c>
     </row>
     <row r="28">
@@ -1929,46 +1929,46 @@
         <v/>
       </c>
       <c r="E28">
-        <v>9.756261872937637</v>
+        <v>10.12911908380886</v>
       </c>
       <c r="F28">
-        <v>4.987131489305716</v>
+        <v>4.253943036141313</v>
       </c>
       <c r="G28">
-        <v>16.63431348237822</v>
+        <v>17.6695216857701</v>
       </c>
       <c r="H28">
-        <v>0.5537269713560518</v>
+        <v>0.5162267675920011</v>
       </c>
       <c r="I28" t="str">
         <v/>
       </c>
       <c r="J28">
-        <v>8.473766042875083</v>
+        <v>8.140524147244463</v>
       </c>
       <c r="K28">
-        <v>4.875093620903228</v>
+        <v>4.084827944869476</v>
       </c>
       <c r="L28">
-        <v>15.609915115546107</v>
+        <v>17.041266139789474</v>
       </c>
       <c r="M28">
-        <v>0.5588499628402962</v>
+        <v>0.5000612624198479</v>
       </c>
       <c r="N28" t="str">
         <v/>
       </c>
       <c r="O28">
-        <v>7.879953196230106</v>
+        <v>6.6356050746756505</v>
       </c>
       <c r="P28">
-        <v>3.798553436281022</v>
+        <v>3.950175263147324</v>
       </c>
       <c r="Q28">
-        <v>12.497715287223594</v>
+        <v>12.9772875274838</v>
       </c>
       <c r="R28">
-        <v>0.5378513551707186</v>
+        <v>0.48571423075594966</v>
       </c>
     </row>
     <row r="29">
@@ -1985,46 +1985,46 @@
         <v/>
       </c>
       <c r="E29">
-        <v>8.589530196553236</v>
+        <v>9.568918723422934</v>
       </c>
       <c r="F29">
-        <v>4.491913251316739</v>
+        <v>4.203726425825796</v>
       </c>
       <c r="G29">
-        <v>16.19257275805485</v>
+        <v>17.94952745270664</v>
       </c>
       <c r="H29">
-        <v>0.5359350455280916</v>
+        <v>0.5957805287783543</v>
       </c>
       <c r="I29" t="str">
         <v/>
       </c>
       <c r="J29">
-        <v>8.138336105843045</v>
+        <v>8.99659197390881</v>
       </c>
       <c r="K29">
-        <v>4.3132185100906195</v>
+        <v>4.199644127804834</v>
       </c>
       <c r="L29">
-        <v>15.927957278183532</v>
+        <v>15.667076046704622</v>
       </c>
       <c r="M29">
-        <v>0.5710748813397635</v>
+        <v>0.49885739781964283</v>
       </c>
       <c r="N29" t="str">
         <v/>
       </c>
       <c r="O29">
-        <v>6.725307292880875</v>
+        <v>6.7420536308778445</v>
       </c>
       <c r="P29">
-        <v>3.955222138886622</v>
+        <v>3.8447526878466807</v>
       </c>
       <c r="Q29">
-        <v>13.17036400688035</v>
+        <v>12.927154889389573</v>
       </c>
       <c r="R29">
-        <v>0.5553906312411376</v>
+        <v>0.48831996603890415</v>
       </c>
     </row>
     <row r="30">
@@ -2041,46 +2041,46 @@
         <v/>
       </c>
       <c r="E30">
-        <v>9.304901138573086</v>
+        <v>8.740480548404737</v>
       </c>
       <c r="F30">
-        <v>4.658414772230708</v>
+        <v>4.270903909222156</v>
       </c>
       <c r="G30">
-        <v>17.50230408416781</v>
+        <v>17.569372675734837</v>
       </c>
       <c r="H30">
-        <v>0.5434302527941387</v>
+        <v>0.5305485829723037</v>
       </c>
       <c r="I30" t="str">
         <v/>
       </c>
       <c r="J30">
-        <v>8.28689100333604</v>
+        <v>9.184345593929356</v>
       </c>
       <c r="K30">
-        <v>4.005716382349902</v>
+        <v>4.079725625094628</v>
       </c>
       <c r="L30">
-        <v>15.664650659108737</v>
+        <v>17.169350907150278</v>
       </c>
       <c r="M30">
-        <v>0.5152684757474443</v>
+        <v>0.5001342534588552</v>
       </c>
       <c r="N30" t="str">
         <v/>
       </c>
       <c r="O30">
-        <v>7.652462735405818</v>
+        <v>7.151712693407482</v>
       </c>
       <c r="P30">
-        <v>3.440975931701281</v>
+        <v>3.7599982045523603</v>
       </c>
       <c r="Q30">
-        <v>12.957845206627495</v>
+        <v>13.262950772633996</v>
       </c>
       <c r="R30">
-        <v>0.4885068797103458</v>
+        <v>0.5153496454291541</v>
       </c>
     </row>
     <row r="31">
@@ -2097,46 +2097,46 @@
         <v/>
       </c>
       <c r="E31">
-        <v>9.541103127304616</v>
+        <v>9.389107925623216</v>
       </c>
       <c r="F31">
-        <v>4.2053508960903265</v>
+        <v>4.954624118388006</v>
       </c>
       <c r="G31">
-        <v>17.263020626415987</v>
+        <v>18.096631696299045</v>
       </c>
       <c r="H31">
-        <v>0.5608005411058954</v>
+        <v>0.5925271609041698</v>
       </c>
       <c r="I31" t="str">
         <v/>
       </c>
       <c r="J31">
-        <v>9.035905067332262</v>
+        <v>9.081551054936895</v>
       </c>
       <c r="K31">
-        <v>3.9391643119850457</v>
+        <v>4.800024018571641</v>
       </c>
       <c r="L31">
-        <v>16.776459495342213</v>
+        <v>17.022143714242038</v>
       </c>
       <c r="M31">
-        <v>0.5611853678315802</v>
+        <v>0.5421778409734413</v>
       </c>
       <c r="N31" t="str">
         <v/>
       </c>
       <c r="O31">
-        <v>7.948524034184543</v>
+        <v>7.877305840811749</v>
       </c>
       <c r="P31">
-        <v>3.6492198760778076</v>
+        <v>3.4598181000799237</v>
       </c>
       <c r="Q31">
-        <v>13.405404958015495</v>
+        <v>12.817667715376858</v>
       </c>
       <c r="R31">
-        <v>0.5423770810033065</v>
+        <v>0.554372918495317</v>
       </c>
     </row>
     <row r="32">
@@ -2153,46 +2153,46 @@
         <v/>
       </c>
       <c r="E32">
-        <v>10.060972577574393</v>
+        <v>8.64423771799345</v>
       </c>
       <c r="F32">
-        <v>4.623837209531875</v>
+        <v>4.851840811035446</v>
       </c>
       <c r="G32">
-        <v>17.569888232097036</v>
+        <v>17.392114035964234</v>
       </c>
       <c r="H32">
-        <v>0.5312761247486628</v>
+        <v>0.5601703715375528</v>
       </c>
       <c r="I32" t="str">
         <v/>
       </c>
       <c r="J32">
-        <v>8.543762898286978</v>
+        <v>8.819953189328418</v>
       </c>
       <c r="K32">
-        <v>4.441367831504565</v>
+        <v>4.862679497415081</v>
       </c>
       <c r="L32">
-        <v>15.53889174346469</v>
+        <v>15.381761834523855</v>
       </c>
       <c r="M32">
-        <v>0.5178880107484211</v>
+        <v>0.5612542574548146</v>
       </c>
       <c r="N32" t="str">
         <v/>
       </c>
       <c r="O32">
-        <v>7.623100607419497</v>
+        <v>7.095490771727732</v>
       </c>
       <c r="P32">
-        <v>3.8862583292002024</v>
+        <v>3.9151707854397544</v>
       </c>
       <c r="Q32">
-        <v>12.674769143610302</v>
+        <v>12.276430992366132</v>
       </c>
       <c r="R32">
-        <v>0.5351220918363079</v>
+        <v>0.4953132422808053</v>
       </c>
     </row>
     <row r="33">
@@ -2209,46 +2209,46 @@
         <v/>
       </c>
       <c r="E33">
-        <v>8.69353460497618</v>
+        <v>9.04957044074949</v>
       </c>
       <c r="F33">
-        <v>4.2873692648109625</v>
+        <v>4.3469234549277544</v>
       </c>
       <c r="G33">
-        <v>17.18896935543167</v>
+        <v>17.14220817111386</v>
       </c>
       <c r="H33">
-        <v>0.5113380491835895</v>
+        <v>0.5541089792967521</v>
       </c>
       <c r="I33" t="str">
         <v/>
       </c>
       <c r="J33">
-        <v>8.46634291707002</v>
+        <v>8.288904760654438</v>
       </c>
       <c r="K33">
-        <v>4.526572597850238</v>
+        <v>4.652660209659999</v>
       </c>
       <c r="L33">
-        <v>16.29428965415421</v>
+        <v>17.020113680104377</v>
       </c>
       <c r="M33">
-        <v>0.55860159057688</v>
+        <v>0.54105801424404</v>
       </c>
       <c r="N33" t="str">
         <v/>
       </c>
       <c r="O33">
-        <v>7.749797456965489</v>
+        <v>7.407316197116667</v>
       </c>
       <c r="P33">
-        <v>3.3649190239911215</v>
+        <v>3.3681650332121023</v>
       </c>
       <c r="Q33">
-        <v>13.285147494861025</v>
+        <v>12.381459144550456</v>
       </c>
       <c r="R33">
-        <v>0.4901596342646192</v>
+        <v>0.5493708980601264</v>
       </c>
     </row>
     <row r="34">
@@ -2265,46 +2265,46 @@
         <v/>
       </c>
       <c r="E34">
-        <v>9.140256745991751</v>
+        <v>10.451603578699881</v>
       </c>
       <c r="F34">
-        <v>4.377269824460811</v>
+        <v>4.247418568323814</v>
       </c>
       <c r="G34">
-        <v>17.982881296391586</v>
+        <v>16.23951132093737</v>
       </c>
       <c r="H34">
-        <v>0.521819352159246</v>
+        <v>0.5238354340655597</v>
       </c>
       <c r="I34" t="str">
         <v/>
       </c>
       <c r="J34">
-        <v>8.562307084437947</v>
+        <v>9.35679772384781</v>
       </c>
       <c r="K34">
-        <v>4.206799780931254</v>
+        <v>4.344171255433784</v>
       </c>
       <c r="L34">
-        <v>15.21939157897986</v>
+        <v>16.077726978306103</v>
       </c>
       <c r="M34">
-        <v>0.5392559099063317</v>
+        <v>0.5207768739362479</v>
       </c>
       <c r="N34" t="str">
         <v/>
       </c>
       <c r="O34">
-        <v>7.37908755223786</v>
+        <v>7.339717870023824</v>
       </c>
       <c r="P34">
-        <v>3.344723679986817</v>
+        <v>3.4828137021602865</v>
       </c>
       <c r="Q34">
-        <v>13.098307121563133</v>
+        <v>12.17493463416451</v>
       </c>
       <c r="R34">
-        <v>0.5365826425774884</v>
+        <v>0.5269074270856282</v>
       </c>
     </row>
     <row r="35">
@@ -2321,46 +2321,46 @@
         <v/>
       </c>
       <c r="E35">
-        <v>10.364944655492435</v>
+        <v>8.657007307528536</v>
       </c>
       <c r="F35">
-        <v>4.272670987323693</v>
+        <v>4.840464998767392</v>
       </c>
       <c r="G35">
-        <v>16.914136881475127</v>
+        <v>17.858725008872465</v>
       </c>
       <c r="H35">
-        <v>0.5577723969375664</v>
+        <v>0.5312201267581546</v>
       </c>
       <c r="I35" t="str">
         <v/>
       </c>
       <c r="J35">
-        <v>8.318681460716128</v>
+        <v>8.25648588670879</v>
       </c>
       <c r="K35">
-        <v>4.1207236182888405</v>
+        <v>4.163642813538237</v>
       </c>
       <c r="L35">
-        <v>16.509110847730103</v>
+        <v>15.456748521515523</v>
       </c>
       <c r="M35">
-        <v>0.5639549056748725</v>
+        <v>0.5204907223990862</v>
       </c>
       <c r="N35" t="str">
         <v/>
       </c>
       <c r="O35">
-        <v>7.684758868726161</v>
+        <v>7.277976676413711</v>
       </c>
       <c r="P35">
-        <v>3.653469743762933</v>
+        <v>3.5581804962224384</v>
       </c>
       <c r="Q35">
-        <v>13.513511037414876</v>
+        <v>12.20305939415058</v>
       </c>
       <c r="R35">
-        <v>0.5795857670353356</v>
+        <v>0.5115337443581224</v>
       </c>
     </row>
     <row r="36">
@@ -2377,46 +2377,46 @@
         <v/>
       </c>
       <c r="E36">
-        <v>8.948783448649946</v>
+        <v>9.498106538254822</v>
       </c>
       <c r="F36">
-        <v>4.829669118062611</v>
+        <v>4.809112227609905</v>
       </c>
       <c r="G36">
-        <v>17.956254210556278</v>
+        <v>17.025525086323803</v>
       </c>
       <c r="H36">
-        <v>0.5618310311288851</v>
+        <v>0.5920748951930581</v>
       </c>
       <c r="I36" t="str">
         <v/>
       </c>
       <c r="J36">
-        <v>8.831227335505965</v>
+        <v>8.196808548872268</v>
       </c>
       <c r="K36">
-        <v>4.758245703397466</v>
+        <v>4.720141557851542</v>
       </c>
       <c r="L36">
-        <v>16.02126693551922</v>
+        <v>16.1060658372758</v>
       </c>
       <c r="M36">
-        <v>0.5027171703681039</v>
+        <v>0.5422750873057549</v>
       </c>
       <c r="N36" t="str">
         <v/>
       </c>
       <c r="O36">
-        <v>7.62226467633072</v>
+        <v>6.96667338458006</v>
       </c>
       <c r="P36">
-        <v>3.6543889099294318</v>
+        <v>3.78147501364046</v>
       </c>
       <c r="Q36">
-        <v>12.454878259704248</v>
+        <v>12.998790614325417</v>
       </c>
       <c r="R36">
-        <v>0.506974486232755</v>
+        <v>0.575392714033764</v>
       </c>
     </row>
     <row r="37">
@@ -2433,46 +2433,46 @@
         <v/>
       </c>
       <c r="E37">
-        <v>9.533483026389927</v>
+        <v>8.74985324094935</v>
       </c>
       <c r="F37">
-        <v>5.132684920496776</v>
+        <v>4.506272583853953</v>
       </c>
       <c r="G37">
-        <v>16.39605539087894</v>
+        <v>18.000580557859035</v>
       </c>
       <c r="H37">
-        <v>0.5439434854022666</v>
+        <v>0.5802854352001946</v>
       </c>
       <c r="I37" t="str">
         <v/>
       </c>
       <c r="J37">
-        <v>7.994607091555122</v>
+        <v>8.52772679096619</v>
       </c>
       <c r="K37">
-        <v>4.379388364676492</v>
+        <v>4.742451605500819</v>
       </c>
       <c r="L37">
-        <v>16.290574005407862</v>
+        <v>16.686453820749676</v>
       </c>
       <c r="M37">
-        <v>0.5081811317636921</v>
+        <v>0.552618646474405</v>
       </c>
       <c r="N37" t="str">
         <v/>
       </c>
       <c r="O37">
-        <v>7.044436569764973</v>
+        <v>7.755509456837507</v>
       </c>
       <c r="P37">
-        <v>3.9168676938920743</v>
+        <v>3.4673601282845397</v>
       </c>
       <c r="Q37">
-        <v>13.1730981929243</v>
+        <v>12.227720103145097</v>
       </c>
       <c r="R37">
-        <v>0.5532584823758159</v>
+        <v>0.5700778371308206</v>
       </c>
     </row>
     <row r="38">
@@ -2489,46 +2489,46 @@
         <v/>
       </c>
       <c r="E38">
-        <v>8.586795814054934</v>
+        <v>9.078756266512109</v>
       </c>
       <c r="F38">
-        <v>5.184248554045529</v>
+        <v>4.45154577796796</v>
       </c>
       <c r="G38">
-        <v>18.043256862779135</v>
+        <v>18.04064735070706</v>
       </c>
       <c r="H38">
-        <v>0.5582853864178063</v>
+        <v>0.5070794065537024</v>
       </c>
       <c r="I38" t="str">
         <v/>
       </c>
       <c r="J38">
-        <v>9.522282575424212</v>
+        <v>8.522356965819627</v>
       </c>
       <c r="K38">
-        <v>3.9898896894742504</v>
+        <v>4.3480750844169656</v>
       </c>
       <c r="L38">
-        <v>16.955681317105146</v>
+        <v>15.307915672542789</v>
       </c>
       <c r="M38">
-        <v>0.49605139698682604</v>
+        <v>0.5114636479314258</v>
       </c>
       <c r="N38" t="str">
         <v/>
       </c>
       <c r="O38">
-        <v>6.632583553951388</v>
+        <v>7.415509221457128</v>
       </c>
       <c r="P38">
-        <v>3.4920438068588306</v>
+        <v>3.746140290818372</v>
       </c>
       <c r="Q38">
-        <v>13.000741187688167</v>
+        <v>12.188885231298807</v>
       </c>
       <c r="R38">
-        <v>0.5609597139967775</v>
+        <v>0.5153373167858745</v>
       </c>
     </row>
     <row r="39">
@@ -2545,46 +2545,46 @@
         <v/>
       </c>
       <c r="E39">
-        <v>9.803511843206865</v>
+        <v>9.026236793049252</v>
       </c>
       <c r="F39">
-        <v>4.295862322055623</v>
+        <v>4.753080508826842</v>
       </c>
       <c r="G39">
-        <v>17.200372838359538</v>
+        <v>17.588892898289018</v>
       </c>
       <c r="H39">
-        <v>0.5977047852380439</v>
+        <v>0.5137804754204923</v>
       </c>
       <c r="I39" t="str">
         <v/>
       </c>
       <c r="J39">
-        <v>9.793366771908518</v>
+        <v>9.79979895167922</v>
       </c>
       <c r="K39">
-        <v>4.2255300530445705</v>
+        <v>3.942894859158191</v>
       </c>
       <c r="L39">
-        <v>16.922564801624723</v>
+        <v>15.361706180955467</v>
       </c>
       <c r="M39">
-        <v>0.5596582822820284</v>
+        <v>0.5026002698220594</v>
       </c>
       <c r="N39" t="str">
         <v/>
       </c>
       <c r="O39">
-        <v>6.982580405971595</v>
+        <v>6.86964506741816</v>
       </c>
       <c r="P39">
-        <v>3.679531714873604</v>
+        <v>3.3326258857371025</v>
       </c>
       <c r="Q39">
-        <v>12.834619983222014</v>
+        <v>13.083470505158411</v>
       </c>
       <c r="R39">
-        <v>0.579781371438439</v>
+        <v>0.536608106068276</v>
       </c>
     </row>
     <row r="40">
@@ -2601,46 +2601,46 @@
         <v/>
       </c>
       <c r="E40">
-        <v>9.474565743171773</v>
+        <v>8.782837885456853</v>
       </c>
       <c r="F40">
-        <v>5.085592029183051</v>
+        <v>5.024869085082332</v>
       </c>
       <c r="G40">
-        <v>17.69506447812562</v>
+        <v>17.609576609500575</v>
       </c>
       <c r="H40">
-        <v>0.5777502883966469</v>
+        <v>0.5706796246995061</v>
       </c>
       <c r="I40" t="str">
         <v/>
       </c>
       <c r="J40">
-        <v>8.365052810542913</v>
+        <v>9.563562102296572</v>
       </c>
       <c r="K40">
-        <v>4.642017650360726</v>
+        <v>4.106991956426863</v>
       </c>
       <c r="L40">
-        <v>16.414342220484734</v>
+        <v>15.254410893206506</v>
       </c>
       <c r="M40">
-        <v>0.5474281419451429</v>
+        <v>0.5506672842647549</v>
       </c>
       <c r="N40" t="str">
         <v/>
       </c>
       <c r="O40">
-        <v>7.467035891522745</v>
+        <v>6.527074861212816</v>
       </c>
       <c r="P40">
-        <v>3.5952240260182498</v>
+        <v>3.8721757206264504</v>
       </c>
       <c r="Q40">
-        <v>13.264552232505588</v>
+        <v>12.68477425968263</v>
       </c>
       <c r="R40">
-        <v>0.5782582242784803</v>
+        <v>0.5637886021782476</v>
       </c>
     </row>
     <row r="41">
@@ -2657,46 +2657,46 @@
         <v/>
       </c>
       <c r="E41">
-        <v>10.19556710520868</v>
+        <v>8.776391408239055</v>
       </c>
       <c r="F41">
-        <v>4.8787579726693675</v>
+        <v>4.7794015383811175</v>
       </c>
       <c r="G41">
-        <v>16.261284298110535</v>
+        <v>17.105027345932893</v>
       </c>
       <c r="H41">
-        <v>0.5796179109583787</v>
+        <v>0.5640042986340217</v>
       </c>
       <c r="I41" t="str">
         <v/>
       </c>
       <c r="J41">
-        <v>8.12841681455992</v>
+        <v>9.640672680083558</v>
       </c>
       <c r="K41">
-        <v>3.984983462516689</v>
+        <v>4.336013240302193</v>
       </c>
       <c r="L41">
-        <v>15.280388834244437</v>
+        <v>15.888850607874804</v>
       </c>
       <c r="M41">
-        <v>0.5520890200825566</v>
+        <v>0.5191125355852235</v>
       </c>
       <c r="N41" t="str">
         <v/>
       </c>
       <c r="O41">
-        <v>7.525840741351396</v>
+        <v>7.84690379499554</v>
       </c>
       <c r="P41">
-        <v>3.642621778048538</v>
+        <v>3.790098865162319</v>
       </c>
       <c r="Q41">
-        <v>12.680219076278819</v>
+        <v>12.531674730491037</v>
       </c>
       <c r="R41">
-        <v>0.48916928024323714</v>
+        <v>0.5667015380667091</v>
       </c>
     </row>
     <row r="42">
@@ -2713,46 +2713,46 @@
         <v/>
       </c>
       <c r="E42">
-        <v>9.549351917747439</v>
+        <v>9.637532001137464</v>
       </c>
       <c r="F42">
-        <v>5.086344367549514</v>
+        <v>4.669582462844685</v>
       </c>
       <c r="G42">
-        <v>17.65320635668287</v>
+        <v>16.29269345796217</v>
       </c>
       <c r="H42">
-        <v>0.5474559588977508</v>
+        <v>0.5688131429585968</v>
       </c>
       <c r="I42" t="str">
         <v/>
       </c>
       <c r="J42">
-        <v>9.529163261969645</v>
+        <v>9.648510328770838</v>
       </c>
       <c r="K42">
-        <v>4.389912372670374</v>
+        <v>4.117758705398833</v>
       </c>
       <c r="L42">
-        <v>15.600034326171837</v>
+        <v>15.405233515595157</v>
       </c>
       <c r="M42">
-        <v>0.5505363587222272</v>
+        <v>0.5419374210881758</v>
       </c>
       <c r="N42" t="str">
         <v/>
       </c>
       <c r="O42">
-        <v>7.989596666736526</v>
+        <v>7.171934471546632</v>
       </c>
       <c r="P42">
-        <v>3.293628260944886</v>
+        <v>3.231126117585997</v>
       </c>
       <c r="Q42">
-        <v>12.617984223312249</v>
+        <v>12.217130710262621</v>
       </c>
       <c r="R42">
-        <v>0.48948071916727703</v>
+        <v>0.48870225486856683</v>
       </c>
     </row>
     <row r="43">
@@ -2769,46 +2769,46 @@
         <v/>
       </c>
       <c r="E43">
-        <v>10.077202686820737</v>
+        <v>9.207865088369667</v>
       </c>
       <c r="F43">
-        <v>4.778709515514971</v>
+        <v>4.752256674383624</v>
       </c>
       <c r="G43">
-        <v>16.763091191234505</v>
+        <v>16.50570733331605</v>
       </c>
       <c r="H43">
-        <v>0.5873647585222648</v>
+        <v>0.5381030663392954</v>
       </c>
       <c r="I43" t="str">
         <v/>
       </c>
       <c r="J43">
-        <v>8.59648278532867</v>
+        <v>8.23332013960093</v>
       </c>
       <c r="K43">
-        <v>4.702074010950706</v>
+        <v>4.596654664665287</v>
       </c>
       <c r="L43">
-        <v>16.89584737877562</v>
+        <v>16.930100475554777</v>
       </c>
       <c r="M43">
-        <v>0.5430942151175446</v>
+        <v>0.5016536670803642</v>
       </c>
       <c r="N43" t="str">
         <v/>
       </c>
       <c r="O43">
-        <v>7.209094373505758</v>
+        <v>7.989502235252685</v>
       </c>
       <c r="P43">
-        <v>3.8135822514883926</v>
+        <v>3.209682739143708</v>
       </c>
       <c r="Q43">
-        <v>12.910344198064543</v>
+        <v>12.111912404891704</v>
       </c>
       <c r="R43">
-        <v>0.5152371105982535</v>
+        <v>0.5641087441077897</v>
       </c>
     </row>
     <row r="44">
@@ -2825,46 +2825,46 @@
         <v/>
       </c>
       <c r="E44">
-        <v>9.499424144239317</v>
+        <v>8.934218856323767</v>
       </c>
       <c r="F44">
-        <v>4.610092270529298</v>
+        <v>4.771832710247995</v>
       </c>
       <c r="G44">
-        <v>16.64719622536645</v>
+        <v>16.75259718010117</v>
       </c>
       <c r="H44">
-        <v>0.5196651114454464</v>
+        <v>0.5506005317151202</v>
       </c>
       <c r="I44" t="str">
         <v/>
       </c>
       <c r="J44">
-        <v>8.612876727728032</v>
+        <v>9.437742522755507</v>
       </c>
       <c r="K44">
-        <v>4.365911051779112</v>
+        <v>4.574317000681621</v>
       </c>
       <c r="L44">
-        <v>15.84420492689867</v>
+        <v>16.124954663399393</v>
       </c>
       <c r="M44">
-        <v>0.5328745422954171</v>
+        <v>0.5142120492852489</v>
       </c>
       <c r="N44" t="str">
         <v/>
       </c>
       <c r="O44">
-        <v>7.009914383747221</v>
+        <v>6.914438913763004</v>
       </c>
       <c r="P44">
-        <v>3.8384423457717647</v>
+        <v>3.3156843650367995</v>
       </c>
       <c r="Q44">
-        <v>12.910284984073106</v>
+        <v>12.646343131810989</v>
       </c>
       <c r="R44">
-        <v>0.5149106803237911</v>
+        <v>0.4964632239436615</v>
       </c>
     </row>
     <row r="45">
@@ -2881,46 +2881,46 @@
         <v/>
       </c>
       <c r="E45">
-        <v>9.582027280154808</v>
+        <v>9.8412875800431</v>
       </c>
       <c r="F45">
-        <v>4.464762230639137</v>
+        <v>4.917500235020009</v>
       </c>
       <c r="G45">
-        <v>16.748564244376425</v>
+        <v>17.778478191464913</v>
       </c>
       <c r="H45">
-        <v>0.532413461907918</v>
+        <v>0.5206850449326011</v>
       </c>
       <c r="I45" t="str">
         <v/>
       </c>
       <c r="J45">
-        <v>8.677366648709876</v>
+        <v>9.70228487674213</v>
       </c>
       <c r="K45">
-        <v>4.697167412305107</v>
+        <v>4.629294000763428</v>
       </c>
       <c r="L45">
-        <v>15.890827582220476</v>
+        <v>16.61083144895373</v>
       </c>
       <c r="M45">
-        <v>0.5514177588964283</v>
+        <v>0.5101368837460807</v>
       </c>
       <c r="N45" t="str">
         <v/>
       </c>
       <c r="O45">
-        <v>6.712767281402583</v>
+        <v>7.7898908298771445</v>
       </c>
       <c r="P45">
-        <v>3.3431093770058755</v>
+        <v>3.815510003033316</v>
       </c>
       <c r="Q45">
-        <v>12.697306744514188</v>
+        <v>13.527013502001992</v>
       </c>
       <c r="R45">
-        <v>0.5721675519919451</v>
+        <v>0.5579632203703598</v>
       </c>
     </row>
     <row r="46">
@@ -2937,46 +2937,46 @@
         <v/>
       </c>
       <c r="E46">
-        <v>9.983462381991682</v>
+        <v>10.158696621943417</v>
       </c>
       <c r="F46">
-        <v>4.21412789037065</v>
+        <v>4.7910623690761485</v>
       </c>
       <c r="G46">
-        <v>16.407024144753837</v>
+        <v>17.71743367844529</v>
       </c>
       <c r="H46">
-        <v>0.5995758396681398</v>
+        <v>0.5165743046516147</v>
       </c>
       <c r="I46" t="str">
         <v/>
       </c>
       <c r="J46">
-        <v>9.14156643051589</v>
+        <v>9.036528511278517</v>
       </c>
       <c r="K46">
-        <v>4.411475186624611</v>
+        <v>4.142845599546464</v>
       </c>
       <c r="L46">
-        <v>16.849300093137472</v>
+        <v>16.137818013508298</v>
       </c>
       <c r="M46">
-        <v>0.5035573679276764</v>
+        <v>0.5684336871895254</v>
       </c>
       <c r="N46" t="str">
         <v/>
       </c>
       <c r="O46">
-        <v>7.441324529048438</v>
+        <v>7.356490696029632</v>
       </c>
       <c r="P46">
-        <v>3.6784129243405648</v>
+        <v>3.8093832589313665</v>
       </c>
       <c r="Q46">
-        <v>12.401536627190492</v>
+        <v>13.140524162857046</v>
       </c>
       <c r="R46">
-        <v>0.49280998637279394</v>
+        <v>0.5500780839637404</v>
       </c>
     </row>
     <row r="47">
@@ -2993,46 +2993,46 @@
         <v/>
       </c>
       <c r="E47">
-        <v>10.450267771372282</v>
+        <v>9.604653492184838</v>
       </c>
       <c r="F47">
-        <v>5.155243608863016</v>
+        <v>4.940735234525081</v>
       </c>
       <c r="G47">
-        <v>16.613320040528837</v>
+        <v>17.68445572298279</v>
       </c>
       <c r="H47">
-        <v>0.5439057561264986</v>
+        <v>0.5604942551672328</v>
       </c>
       <c r="I47" t="str">
         <v/>
       </c>
       <c r="J47">
-        <v>7.951164087041872</v>
+        <v>9.790478916889874</v>
       </c>
       <c r="K47">
-        <v>4.301970270018838</v>
+        <v>4.428867589059583</v>
       </c>
       <c r="L47">
-        <v>16.472068224315336</v>
+        <v>16.014848439677323</v>
       </c>
       <c r="M47">
-        <v>0.5268839097371112</v>
+        <v>0.49877668826592353</v>
       </c>
       <c r="N47" t="str">
         <v/>
       </c>
       <c r="O47">
-        <v>7.695562515903177</v>
+        <v>7.813840141990063</v>
       </c>
       <c r="P47">
-        <v>3.8129748665734895</v>
+        <v>3.990483478726661</v>
       </c>
       <c r="Q47">
-        <v>12.745557713231491</v>
+        <v>12.253800194344386</v>
       </c>
       <c r="R47">
-        <v>0.49946796904611307</v>
+        <v>0.517249990999338</v>
       </c>
     </row>
     <row r="48">
@@ -3049,46 +3049,46 @@
         <v/>
       </c>
       <c r="E48">
-        <v>9.007334738075432</v>
+        <v>9.47678404338111</v>
       </c>
       <c r="F48">
-        <v>4.5332220485479935</v>
+        <v>5.1298236129463906</v>
       </c>
       <c r="G48">
-        <v>17.125808713354928</v>
+        <v>17.129604212169752</v>
       </c>
       <c r="H48">
-        <v>0.5433181014332384</v>
+        <v>0.5041694570068456</v>
       </c>
       <c r="I48" t="str">
         <v/>
       </c>
       <c r="J48">
-        <v>9.050115228507412</v>
+        <v>8.723346042014992</v>
       </c>
       <c r="K48">
-        <v>4.178386537747832</v>
+        <v>4.4042920101063014</v>
       </c>
       <c r="L48">
-        <v>15.38759393623966</v>
+        <v>16.954551432780026</v>
       </c>
       <c r="M48">
-        <v>0.5871262890794179</v>
+        <v>0.5380230463428947</v>
       </c>
       <c r="N48" t="str">
         <v/>
       </c>
       <c r="O48">
-        <v>6.568787202544417</v>
+        <v>7.751985128819182</v>
       </c>
       <c r="P48">
-        <v>3.776522092295986</v>
+        <v>3.3203522242131167</v>
       </c>
       <c r="Q48">
-        <v>12.845718264384882</v>
+        <v>12.743786958608847</v>
       </c>
       <c r="R48">
-        <v>0.5371924368533673</v>
+        <v>0.563966643999246</v>
       </c>
     </row>
     <row r="49">
@@ -3105,46 +3105,46 @@
         <v/>
       </c>
       <c r="E49">
-        <v>9.831861323994744</v>
+        <v>9.327028232594898</v>
       </c>
       <c r="F49">
-        <v>4.8599630792052775</v>
+        <v>4.726268151388105</v>
       </c>
       <c r="G49">
-        <v>16.578941261552945</v>
+        <v>17.92102585439353</v>
       </c>
       <c r="H49">
-        <v>0.5455234513248458</v>
+        <v>0.5431533099075989</v>
       </c>
       <c r="I49" t="str">
         <v/>
       </c>
       <c r="J49">
-        <v>7.890595784012489</v>
+        <v>9.028740001244852</v>
       </c>
       <c r="K49">
-        <v>4.119739827943118</v>
+        <v>4.3849273632787895</v>
       </c>
       <c r="L49">
-        <v>17.031968987031675</v>
+        <v>15.306348973698208</v>
       </c>
       <c r="M49">
-        <v>0.5601409743027091</v>
+        <v>0.5393593819390228</v>
       </c>
       <c r="N49" t="str">
         <v/>
       </c>
       <c r="O49">
-        <v>6.655395614541062</v>
+        <v>7.7874881609931</v>
       </c>
       <c r="P49">
-        <v>3.658126948615738</v>
+        <v>3.9380591667410108</v>
       </c>
       <c r="Q49">
-        <v>12.727612749347475</v>
+        <v>13.016108609044919</v>
       </c>
       <c r="R49">
-        <v>0.5478405324081892</v>
+        <v>0.566575790394065</v>
       </c>
     </row>
     <row r="50">
@@ -3161,46 +3161,46 @@
         <v/>
       </c>
       <c r="E50">
-        <v>8.832223698550534</v>
+        <v>10.034481241031283</v>
       </c>
       <c r="F50">
-        <v>4.985055525359675</v>
+        <v>4.59440772311198</v>
       </c>
       <c r="G50">
-        <v>16.42831711366116</v>
+        <v>16.357510781667568</v>
       </c>
       <c r="H50">
-        <v>0.5631135495112662</v>
+        <v>0.565915047225972</v>
       </c>
       <c r="I50" t="str">
         <v/>
       </c>
       <c r="J50">
-        <v>9.28477916940886</v>
+        <v>8.360043051748626</v>
       </c>
       <c r="K50">
-        <v>4.593174443638386</v>
+        <v>4.053110239718702</v>
       </c>
       <c r="L50">
-        <v>16.360474445629766</v>
+        <v>15.964998198916149</v>
       </c>
       <c r="M50">
-        <v>0.5110033543519533</v>
+        <v>0.5509262330984985</v>
       </c>
       <c r="N50" t="str">
         <v/>
       </c>
       <c r="O50">
-        <v>7.149901535111988</v>
+        <v>6.606574876331535</v>
       </c>
       <c r="P50">
-        <v>3.56956273817465</v>
+        <v>3.718570916438869</v>
       </c>
       <c r="Q50">
-        <v>12.46015811227765</v>
+        <v>12.315629322724353</v>
       </c>
       <c r="R50">
-        <v>0.48548364246442294</v>
+        <v>0.5084373496632458</v>
       </c>
     </row>
     <row r="51">
@@ -3352,7 +3352,7 @@
         <v/>
       </c>
       <c r="G2">
-        <v>49.42763511197316</v>
+        <v>49.840576964230024</v>
       </c>
       <c r="H2" t="str">
         <v/>
@@ -3370,7 +3370,7 @@
         <v/>
       </c>
       <c r="M2">
-        <v>52.455314186217656</v>
+        <v>49.075624775575996</v>
       </c>
       <c r="N2" t="str">
         <v/>
@@ -3388,7 +3388,7 @@
         <v/>
       </c>
       <c r="S2">
-        <v>39.955746373192554</v>
+        <v>38.65804846359627</v>
       </c>
     </row>
     <row r="3">
@@ -3411,7 +3411,7 @@
         <v/>
       </c>
       <c r="G3">
-        <v>50.09800053116695</v>
+        <v>54.37892373785384</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -3429,7 +3429,7 @@
         <v/>
       </c>
       <c r="M3">
-        <v>50.28944034938305</v>
+        <v>51.03133974010222</v>
       </c>
       <c r="N3" t="str">
         <v/>
@@ -3447,7 +3447,7 @@
         <v/>
       </c>
       <c r="S3">
-        <v>40.40421389867618</v>
+        <v>45.40155495929521</v>
       </c>
     </row>
     <row r="4">
@@ -3470,7 +3470,7 @@
         <v/>
       </c>
       <c r="G4">
-        <v>48.96116858382221</v>
+        <v>50.8613369218989</v>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -3488,7 +3488,7 @@
         <v/>
       </c>
       <c r="M4">
-        <v>46.586418718680264</v>
+        <v>44.99909483793231</v>
       </c>
       <c r="N4" t="str">
         <v/>
@@ -3506,7 +3506,7 @@
         <v/>
       </c>
       <c r="S4">
-        <v>44.04266232989725</v>
+        <v>41.04936406461505</v>
       </c>
     </row>
     <row r="5">
@@ -3529,7 +3529,7 @@
         <v/>
       </c>
       <c r="G5">
-        <v>49.052872490271476</v>
+        <v>52.042083665395396</v>
       </c>
       <c r="H5" t="str">
         <v/>
@@ -3547,7 +3547,7 @@
         <v/>
       </c>
       <c r="M5">
-        <v>48.099711620083035</v>
+        <v>45.53187009304468</v>
       </c>
       <c r="N5" t="str">
         <v/>
@@ -3565,7 +3565,7 @@
         <v/>
       </c>
       <c r="S5">
-        <v>44.06209405119817</v>
+        <v>40.91666665514565</v>
       </c>
     </row>
     <row r="6">
@@ -3588,7 +3588,7 @@
         <v/>
       </c>
       <c r="G6">
-        <v>50.99751567089476</v>
+        <v>53.176693830256355</v>
       </c>
       <c r="H6" t="str">
         <v/>
@@ -3606,7 +3606,7 @@
         <v/>
       </c>
       <c r="M6">
-        <v>47.93018328119957</v>
+        <v>47.1774723328745</v>
       </c>
       <c r="N6" t="str">
         <v/>
@@ -3624,7 +3624,7 @@
         <v/>
       </c>
       <c r="S6">
-        <v>43.51249858495219</v>
+        <v>39.66517600948995</v>
       </c>
     </row>
     <row r="7">
@@ -3647,7 +3647,7 @@
         <v/>
       </c>
       <c r="G7">
-        <v>52.99982077248394</v>
+        <v>48.700964701068656</v>
       </c>
       <c r="H7" t="str">
         <v/>
@@ -3665,7 +3665,7 @@
         <v/>
       </c>
       <c r="M7">
-        <v>47.98395649034834</v>
+        <v>45.34164843714983</v>
       </c>
       <c r="N7" t="str">
         <v/>
@@ -3683,7 +3683,7 @@
         <v/>
       </c>
       <c r="S7">
-        <v>43.054087469852675</v>
+        <v>40.394418850774315</v>
       </c>
     </row>
     <row r="8">
@@ -3706,7 +3706,7 @@
         <v/>
       </c>
       <c r="G8">
-        <v>49.115783693973235</v>
+        <v>50.214075030701764</v>
       </c>
       <c r="H8" t="str">
         <v/>
@@ -3724,7 +3724,7 @@
         <v/>
       </c>
       <c r="M8">
-        <v>43.54406373564431</v>
+        <v>46.61300910084237</v>
       </c>
       <c r="N8" t="str">
         <v/>
@@ -3742,7 +3742,7 @@
         <v/>
       </c>
       <c r="S8">
-        <v>46.42898897279961</v>
+        <v>44.71944251198232</v>
       </c>
     </row>
     <row r="9">
@@ -3765,7 +3765,7 @@
         <v/>
       </c>
       <c r="G9">
-        <v>47.110600505638345</v>
+        <v>47.34470930627625</v>
       </c>
       <c r="H9" t="str">
         <v/>
@@ -3783,7 +3783,7 @@
         <v/>
       </c>
       <c r="M9">
-        <v>46.83701622991458</v>
+        <v>50.04839959492506</v>
       </c>
       <c r="N9" t="str">
         <v/>
@@ -3801,7 +3801,7 @@
         <v/>
       </c>
       <c r="S9">
-        <v>42.88188730008475</v>
+        <v>40.578428081858064</v>
       </c>
     </row>
     <row r="10">
@@ -3824,7 +3824,7 @@
         <v/>
       </c>
       <c r="G10">
-        <v>45.35778772261802</v>
+        <v>54.57501554866689</v>
       </c>
       <c r="H10" t="str">
         <v/>
@@ -3842,7 +3842,7 @@
         <v/>
       </c>
       <c r="M10">
-        <v>49.61188601215326</v>
+        <v>52.04067898678105</v>
       </c>
       <c r="N10" t="str">
         <v/>
@@ -3860,7 +3860,7 @@
         <v/>
       </c>
       <c r="S10">
-        <v>39.45018263184124</v>
+        <v>43.554282893238316</v>
       </c>
     </row>
     <row r="11">
@@ -3883,7 +3883,7 @@
         <v/>
       </c>
       <c r="G11">
-        <v>51.573208850321464</v>
+        <v>45.23169334487296</v>
       </c>
       <c r="H11" t="str">
         <v/>
@@ -3901,7 +3901,7 @@
         <v/>
       </c>
       <c r="M11">
-        <v>48.57479980226539</v>
+        <v>46.767503033966776</v>
       </c>
       <c r="N11" t="str">
         <v/>
@@ -3919,7 +3919,7 @@
         <v/>
       </c>
       <c r="S11">
-        <v>39.20040431099746</v>
+        <v>42.1428538031856</v>
       </c>
     </row>
     <row r="12">
@@ -3942,7 +3942,7 @@
         <v/>
       </c>
       <c r="G12">
-        <v>45.53559745721631</v>
+        <v>53.879417144490645</v>
       </c>
       <c r="H12" t="str">
         <v/>
@@ -3960,7 +3960,7 @@
         <v/>
       </c>
       <c r="M12">
-        <v>46.61297409247642</v>
+        <v>52.19953011467369</v>
       </c>
       <c r="N12" t="str">
         <v/>
@@ -3978,7 +3978,7 @@
         <v/>
       </c>
       <c r="S12">
-        <v>40.36457283284539</v>
+        <v>43.368136127806636</v>
       </c>
     </row>
     <row r="13">
@@ -4001,7 +4001,7 @@
         <v/>
       </c>
       <c r="G13">
-        <v>55.13226366325132</v>
+        <v>53.23708869427162</v>
       </c>
       <c r="H13" t="str">
         <v/>
@@ -4019,7 +4019,7 @@
         <v/>
       </c>
       <c r="M13">
-        <v>45.55130929192699</v>
+        <v>42.911475384958585</v>
       </c>
       <c r="N13" t="str">
         <v/>
@@ -4037,7 +4037,7 @@
         <v/>
       </c>
       <c r="S13">
-        <v>41.359222305299085</v>
+        <v>42.244919511304666</v>
       </c>
     </row>
     <row r="14">
@@ -4060,7 +4060,7 @@
         <v/>
       </c>
       <c r="G14">
-        <v>54.70723639898268</v>
+        <v>54.22126261959811</v>
       </c>
       <c r="H14" t="str">
         <v/>
@@ -4078,7 +4078,7 @@
         <v/>
       </c>
       <c r="M14">
-        <v>46.0606827998326</v>
+        <v>44.11776891932017</v>
       </c>
       <c r="N14" t="str">
         <v/>
@@ -4096,7 +4096,7 @@
         <v/>
       </c>
       <c r="S14">
-        <v>43.79974559526443</v>
+        <v>45.06900032412874</v>
       </c>
     </row>
     <row r="15">
@@ -4119,7 +4119,7 @@
         <v/>
       </c>
       <c r="G15">
-        <v>45.30611411347109</v>
+        <v>55.028808345319874</v>
       </c>
       <c r="H15" t="str">
         <v/>
@@ -4137,7 +4137,7 @@
         <v/>
       </c>
       <c r="M15">
-        <v>48.5310595810064</v>
+        <v>48.1060956974019</v>
       </c>
       <c r="N15" t="str">
         <v/>
@@ -4155,7 +4155,7 @@
         <v/>
       </c>
       <c r="S15">
-        <v>39.685083113319976</v>
+        <v>39.271448511275224</v>
       </c>
     </row>
     <row r="16">
@@ -4178,7 +4178,7 @@
         <v/>
       </c>
       <c r="G16">
-        <v>47.68477522646253</v>
+        <v>47.653708209384575</v>
       </c>
       <c r="H16" t="str">
         <v/>
@@ -4196,7 +4196,7 @@
         <v/>
       </c>
       <c r="M16">
-        <v>44.49247888559448</v>
+        <v>49.656116698964425</v>
       </c>
       <c r="N16" t="str">
         <v/>
@@ -4214,7 +4214,7 @@
         <v/>
       </c>
       <c r="S16">
-        <v>40.545262656133545</v>
+        <v>40.88259874812271</v>
       </c>
     </row>
     <row r="17">
@@ -4237,7 +4237,7 @@
         <v/>
       </c>
       <c r="G17">
-        <v>48.629183056147575</v>
+        <v>46.77672857820777</v>
       </c>
       <c r="H17" t="str">
         <v/>
@@ -4255,7 +4255,7 @@
         <v/>
       </c>
       <c r="M17">
-        <v>44.614164187725414</v>
+        <v>48.166903455137316</v>
       </c>
       <c r="N17" t="str">
         <v/>
@@ -4273,7 +4273,7 @@
         <v/>
       </c>
       <c r="S17">
-        <v>41.69472801503769</v>
+        <v>44.20251378142125</v>
       </c>
     </row>
     <row r="18">
@@ -4296,7 +4296,7 @@
         <v/>
       </c>
       <c r="G18">
-        <v>53.370498131666</v>
+        <v>52.4714621071675</v>
       </c>
       <c r="H18" t="str">
         <v/>
@@ -4314,7 +4314,7 @@
         <v/>
       </c>
       <c r="M18">
-        <v>50.620836897733604</v>
+        <v>50.70421101275005</v>
       </c>
       <c r="N18" t="str">
         <v/>
@@ -4332,7 +4332,7 @@
         <v/>
       </c>
       <c r="S18">
-        <v>39.037975341716184</v>
+        <v>40.423604301895125</v>
       </c>
     </row>
     <row r="19">
@@ -4355,7 +4355,7 @@
         <v/>
       </c>
       <c r="G19">
-        <v>51.97251273943515</v>
+        <v>46.42822512243283</v>
       </c>
       <c r="H19" t="str">
         <v/>
@@ -4373,7 +4373,7 @@
         <v/>
       </c>
       <c r="M19">
-        <v>43.082869471627895</v>
+        <v>45.300143778552595</v>
       </c>
       <c r="N19" t="str">
         <v/>
@@ -4391,7 +4391,7 @@
         <v/>
       </c>
       <c r="S19">
-        <v>41.20757582554017</v>
+        <v>44.20251765934693</v>
       </c>
     </row>
     <row r="20">
@@ -4414,7 +4414,7 @@
         <v/>
       </c>
       <c r="G20">
-        <v>46.87986926900526</v>
+        <v>48.03560364938048</v>
       </c>
       <c r="H20" t="str">
         <v/>
@@ -4432,7 +4432,7 @@
         <v/>
       </c>
       <c r="M20">
-        <v>52.05941534660474</v>
+        <v>48.19025600565797</v>
       </c>
       <c r="N20" t="str">
         <v/>
@@ -4450,7 +4450,7 @@
         <v/>
       </c>
       <c r="S20">
-        <v>42.17321748846993</v>
+        <v>40.67468978833597</v>
       </c>
     </row>
     <row r="21">
@@ -4473,7 +4473,7 @@
         <v/>
       </c>
       <c r="G21">
-        <v>47.70621777334443</v>
+        <v>54.583961243152594</v>
       </c>
       <c r="H21" t="str">
         <v/>
@@ -4491,7 +4491,7 @@
         <v/>
       </c>
       <c r="M21">
-        <v>45.00121867015578</v>
+        <v>47.19549180292744</v>
       </c>
       <c r="N21" t="str">
         <v/>
@@ -4509,7 +4509,7 @@
         <v/>
       </c>
       <c r="S21">
-        <v>41.62689887171869</v>
+        <v>39.648952143158056</v>
       </c>
     </row>
     <row r="22">
@@ -4532,7 +4532,7 @@
         <v/>
       </c>
       <c r="G22">
-        <v>47.96766431773255</v>
+        <v>49.84138523944021</v>
       </c>
       <c r="H22" t="str">
         <v/>
@@ -4550,7 +4550,7 @@
         <v/>
       </c>
       <c r="M22">
-        <v>44.49947270922644</v>
+        <v>49.12212752384305</v>
       </c>
       <c r="N22" t="str">
         <v/>
@@ -4568,7 +4568,7 @@
         <v/>
       </c>
       <c r="S22">
-        <v>40.41462641999761</v>
+        <v>43.978362531512914</v>
       </c>
     </row>
     <row r="23">
@@ -4591,7 +4591,7 @@
         <v/>
       </c>
       <c r="G23">
-        <v>48.72358615464392</v>
+        <v>51.5990076504434</v>
       </c>
       <c r="H23" t="str">
         <v/>
@@ -4609,7 +4609,7 @@
         <v/>
       </c>
       <c r="M23">
-        <v>44.844541030911316</v>
+        <v>44.51192068281126</v>
       </c>
       <c r="N23" t="str">
         <v/>
@@ -4627,7 +4627,7 @@
         <v/>
       </c>
       <c r="S23">
-        <v>39.293355431410184</v>
+        <v>41.224745628233826</v>
       </c>
     </row>
     <row r="24">
@@ -4650,7 +4650,7 @@
         <v/>
       </c>
       <c r="G24">
-        <v>45.49251475951473</v>
+        <v>50.032569394869185</v>
       </c>
       <c r="H24" t="str">
         <v/>
@@ -4668,7 +4668,7 @@
         <v/>
       </c>
       <c r="M24">
-        <v>48.903461394696315</v>
+        <v>46.251741285878495</v>
       </c>
       <c r="N24" t="str">
         <v/>
@@ -4686,7 +4686,7 @@
         <v/>
       </c>
       <c r="S24">
-        <v>41.91202255497997</v>
+        <v>40.46641074503948</v>
       </c>
     </row>
     <row r="25">
@@ -4709,7 +4709,7 @@
         <v/>
       </c>
       <c r="G25">
-        <v>54.1091123128735</v>
+        <v>47.74570383393399</v>
       </c>
       <c r="H25" t="str">
         <v/>
@@ -4727,7 +4727,7 @@
         <v/>
       </c>
       <c r="M25">
-        <v>48.16750674403616</v>
+        <v>47.57529528536362</v>
       </c>
       <c r="N25" t="str">
         <v/>
@@ -4745,7 +4745,7 @@
         <v/>
       </c>
       <c r="S25">
-        <v>46.30423696628382</v>
+        <v>46.19010715561491</v>
       </c>
     </row>
     <row r="26">
@@ -4768,7 +4768,7 @@
         <v/>
       </c>
       <c r="G26">
-        <v>54.402830322385746</v>
+        <v>46.59489613298643</v>
       </c>
       <c r="H26" t="str">
         <v/>
@@ -4786,7 +4786,7 @@
         <v/>
       </c>
       <c r="M26">
-        <v>50.984120374073605</v>
+        <v>45.648640220699896</v>
       </c>
       <c r="N26" t="str">
         <v/>
@@ -4804,7 +4804,7 @@
         <v/>
       </c>
       <c r="S26">
-        <v>40.53991172954838</v>
+        <v>43.059633235242934</v>
       </c>
     </row>
     <row r="27">
@@ -4827,7 +4827,7 @@
         <v/>
       </c>
       <c r="G27">
-        <v>53.38332583519702</v>
+        <v>49.162475938975355</v>
       </c>
       <c r="H27" t="str">
         <v/>
@@ -4845,7 +4845,7 @@
         <v/>
       </c>
       <c r="M27">
-        <v>48.57866675258636</v>
+        <v>49.129087422323906</v>
       </c>
       <c r="N27" t="str">
         <v/>
@@ -4863,7 +4863,7 @@
         <v/>
       </c>
       <c r="S27">
-        <v>41.974146059673885</v>
+        <v>42.09381838315819</v>
       </c>
     </row>
     <row r="28">
@@ -4886,7 +4886,7 @@
         <v/>
       </c>
       <c r="G28">
-        <v>50.540995138865796</v>
+        <v>49.560730343702396</v>
       </c>
       <c r="H28" t="str">
         <v/>
@@ -4904,7 +4904,7 @@
         <v/>
       </c>
       <c r="M28">
-        <v>45.37029014803934</v>
+        <v>51.78771879596236</v>
       </c>
       <c r="N28" t="str">
         <v/>
@@ -4922,7 +4922,7 @@
         <v/>
       </c>
       <c r="S28">
-        <v>44.23301076147891</v>
+        <v>43.88539900588365</v>
       </c>
     </row>
     <row r="29">
@@ -4945,7 +4945,7 @@
         <v/>
       </c>
       <c r="G29">
-        <v>49.18606606153606</v>
+        <v>49.33734571852721</v>
       </c>
       <c r="H29" t="str">
         <v/>
@@ -4963,7 +4963,7 @@
         <v/>
       </c>
       <c r="M29">
-        <v>45.99120824712232</v>
+        <v>50.79711827665723</v>
       </c>
       <c r="N29" t="str">
         <v/>
@@ -4981,7 +4981,7 @@
         <v/>
       </c>
       <c r="S29">
-        <v>40.57092138377021</v>
+        <v>42.8195115902096</v>
       </c>
     </row>
     <row r="30">
@@ -5004,7 +5004,7 @@
         <v/>
       </c>
       <c r="G30">
-        <v>49.50607854289086</v>
+        <v>47.083228377943584</v>
       </c>
       <c r="H30" t="str">
         <v/>
@@ -5022,7 +5022,7 @@
         <v/>
       </c>
       <c r="M30">
-        <v>44.80956955103379</v>
+        <v>45.12167065790326</v>
       </c>
       <c r="N30" t="str">
         <v/>
@@ -5040,7 +5040,7 @@
         <v/>
       </c>
       <c r="S30">
-        <v>40.57917797479901</v>
+        <v>44.68237667735433</v>
       </c>
     </row>
     <row r="31">
@@ -5063,7 +5063,7 @@
         <v/>
       </c>
       <c r="G31">
-        <v>51.153975811472336</v>
+        <v>50.71760131480614</v>
       </c>
       <c r="H31" t="str">
         <v/>
@@ -5081,7 +5081,7 @@
         <v/>
       </c>
       <c r="M31">
-        <v>50.646733415561755</v>
+        <v>48.853308036079035</v>
       </c>
       <c r="N31" t="str">
         <v/>
@@ -5099,7 +5099,7 @@
         <v/>
       </c>
       <c r="S31">
-        <v>46.300844822705514</v>
+        <v>39.47104361892085</v>
       </c>
     </row>
     <row r="32">
@@ -5122,7 +5122,7 @@
         <v/>
       </c>
       <c r="G32">
-        <v>52.620967280537165</v>
+        <v>50.44823548153416</v>
       </c>
       <c r="H32" t="str">
         <v/>
@@ -5140,7 +5140,7 @@
         <v/>
       </c>
       <c r="M32">
-        <v>47.86339880532037</v>
+        <v>44.90355242979004</v>
       </c>
       <c r="N32" t="str">
         <v/>
@@ -5158,7 +5158,7 @@
         <v/>
       </c>
       <c r="S32">
-        <v>40.27450372531635</v>
+        <v>43.2828265821983</v>
       </c>
     </row>
     <row r="33">
@@ -5181,7 +5181,7 @@
         <v/>
       </c>
       <c r="G33">
-        <v>51.84944061744528</v>
+        <v>47.315184790226894</v>
       </c>
       <c r="H33" t="str">
         <v/>
@@ -5199,7 +5199,7 @@
         <v/>
       </c>
       <c r="M33">
-        <v>44.98957742204439</v>
+        <v>50.21475590963026</v>
       </c>
       <c r="N33" t="str">
         <v/>
@@ -5217,7 +5217,7 @@
         <v/>
       </c>
       <c r="S33">
-        <v>38.68057879787189</v>
+        <v>43.62135043770949</v>
       </c>
     </row>
     <row r="34">
@@ -5240,7 +5240,7 @@
         <v/>
       </c>
       <c r="G34">
-        <v>53.37622294892312</v>
+        <v>51.97741849655264</v>
       </c>
       <c r="H34" t="str">
         <v/>
@@ -5258,7 +5258,7 @@
         <v/>
       </c>
       <c r="M34">
-        <v>46.0462889308675</v>
+        <v>44.92963130744586</v>
       </c>
       <c r="N34" t="str">
         <v/>
@@ -5276,7 +5276,7 @@
         <v/>
       </c>
       <c r="S34">
-        <v>38.9361873255138</v>
+        <v>44.54502806981589</v>
       </c>
     </row>
     <row r="35">
@@ -5299,7 +5299,7 @@
         <v/>
       </c>
       <c r="G35">
-        <v>47.63081495554006</v>
+        <v>48.12224137686094</v>
       </c>
       <c r="H35" t="str">
         <v/>
@@ -5317,7 +5317,7 @@
         <v/>
       </c>
       <c r="M35">
-        <v>45.074688528647606</v>
+        <v>52.11891846091949</v>
       </c>
       <c r="N35" t="str">
         <v/>
@@ -5335,7 +5335,7 @@
         <v/>
       </c>
       <c r="S35">
-        <v>40.92780712877597</v>
+        <v>44.63863790106094</v>
       </c>
     </row>
     <row r="36">
@@ -5358,7 +5358,7 @@
         <v/>
       </c>
       <c r="G36">
-        <v>51.45007610556587</v>
+        <v>48.14567868854014</v>
       </c>
       <c r="H36" t="str">
         <v/>
@@ -5376,7 +5376,7 @@
         <v/>
       </c>
       <c r="M36">
-        <v>44.590502967317896</v>
+        <v>50.08064919540472</v>
       </c>
       <c r="N36" t="str">
         <v/>
@@ -5394,7 +5394,7 @@
         <v/>
       </c>
       <c r="S36">
-        <v>43.41478258586556</v>
+        <v>45.83198462271481</v>
       </c>
     </row>
     <row r="37">
@@ -5417,7 +5417,7 @@
         <v/>
       </c>
       <c r="G37">
-        <v>50.639683477488994</v>
+        <v>49.47237300963813</v>
       </c>
       <c r="H37" t="str">
         <v/>
@@ -5435,7 +5435,7 @@
         <v/>
       </c>
       <c r="M37">
-        <v>52.09285166730199</v>
+        <v>46.401380418743926</v>
       </c>
       <c r="N37" t="str">
         <v/>
@@ -5453,7 +5453,7 @@
         <v/>
       </c>
       <c r="S37">
-        <v>44.10154040756977</v>
+        <v>38.981744043631295</v>
       </c>
     </row>
     <row r="38">
@@ -5476,7 +5476,7 @@
         <v/>
       </c>
       <c r="G38">
-        <v>50.577949287480045</v>
+        <v>48.237144088164065</v>
       </c>
       <c r="H38" t="str">
         <v/>
@@ -5494,7 +5494,7 @@
         <v/>
       </c>
       <c r="M38">
-        <v>47.00594491645188</v>
+        <v>44.42445595132125</v>
       </c>
       <c r="N38" t="str">
         <v/>
@@ -5512,7 +5512,7 @@
         <v/>
       </c>
       <c r="S38">
-        <v>45.356723999295376</v>
+        <v>38.923425115102084</v>
       </c>
     </row>
     <row r="39">
@@ -5535,7 +5535,7 @@
         <v/>
       </c>
       <c r="G39">
-        <v>45.8028518064862</v>
+        <v>51.127800777622525</v>
       </c>
       <c r="H39" t="str">
         <v/>
@@ -5553,7 +5553,7 @@
         <v/>
       </c>
       <c r="M39">
-        <v>48.376819604043924</v>
+        <v>47.56883277459971</v>
       </c>
       <c r="N39" t="str">
         <v/>
@@ -5571,7 +5571,7 @@
         <v/>
       </c>
       <c r="S39">
-        <v>41.10930998189455</v>
+        <v>46.1332064628099</v>
       </c>
     </row>
     <row r="40">
@@ -5594,7 +5594,7 @@
         <v/>
       </c>
       <c r="G40">
-        <v>54.86990132917187</v>
+        <v>49.04080281491018</v>
       </c>
       <c r="H40" t="str">
         <v/>
@@ -5612,7 +5612,7 @@
         <v/>
       </c>
       <c r="M40">
-        <v>52.058448229950685</v>
+        <v>46.885915081833986</v>
       </c>
       <c r="N40" t="str">
         <v/>
@@ -5630,7 +5630,7 @@
         <v/>
       </c>
       <c r="S40">
-        <v>43.683499052913454</v>
+        <v>40.21003024798357</v>
       </c>
     </row>
     <row r="41">
@@ -5653,7 +5653,7 @@
         <v/>
       </c>
       <c r="G41">
-        <v>54.093891813862626</v>
+        <v>52.929172431035525</v>
       </c>
       <c r="H41" t="str">
         <v/>
@@ -5671,7 +5671,7 @@
         <v/>
       </c>
       <c r="M41">
-        <v>45.75464760543013</v>
+        <v>51.37993621729228</v>
       </c>
       <c r="N41" t="str">
         <v/>
@@ -5689,7 +5689,7 @@
         <v/>
       </c>
       <c r="S41">
-        <v>40.14181958332547</v>
+        <v>39.0772448033146</v>
       </c>
     </row>
     <row r="42">
@@ -5712,7 +5712,7 @@
         <v/>
       </c>
       <c r="G42">
-        <v>47.83217119631583</v>
+        <v>51.55937382963877</v>
       </c>
       <c r="H42" t="str">
         <v/>
@@ -5730,7 +5730,7 @@
         <v/>
       </c>
       <c r="M42">
-        <v>46.54144811263626</v>
+        <v>48.25378235710251</v>
       </c>
       <c r="N42" t="str">
         <v/>
@@ -5748,7 +5748,7 @@
         <v/>
       </c>
       <c r="S42">
-        <v>44.984959435198206</v>
+        <v>43.6573091013358</v>
       </c>
     </row>
     <row r="43">
@@ -5771,7 +5771,7 @@
         <v/>
       </c>
       <c r="G43">
-        <v>54.55552656539735</v>
+        <v>51.63996183894594</v>
       </c>
       <c r="H43" t="str">
         <v/>
@@ -5789,7 +5789,7 @@
         <v/>
       </c>
       <c r="M43">
-        <v>52.52610097830062</v>
+        <v>46.71956972662285</v>
       </c>
       <c r="N43" t="str">
         <v/>
@@ -5807,7 +5807,7 @@
         <v/>
       </c>
       <c r="S43">
-        <v>44.94853768181892</v>
+        <v>40.9709134683142</v>
       </c>
     </row>
     <row r="44">
@@ -5830,7 +5830,7 @@
         <v/>
       </c>
       <c r="G44">
-        <v>50.48265320512077</v>
+        <v>48.49875766860558</v>
       </c>
       <c r="H44" t="str">
         <v/>
@@ -5848,7 +5848,7 @@
         <v/>
       </c>
       <c r="M44">
-        <v>52.362666107299916</v>
+        <v>45.83255598412085</v>
       </c>
       <c r="N44" t="str">
         <v/>
@@ -5866,7 +5866,7 @@
         <v/>
       </c>
       <c r="S44">
-        <v>42.72065063190793</v>
+        <v>45.749884598649565</v>
       </c>
     </row>
     <row r="45">
@@ -5889,7 +5889,7 @@
         <v/>
       </c>
       <c r="G45">
-        <v>45.650522267688146</v>
+        <v>48.79122627272922</v>
       </c>
       <c r="H45" t="str">
         <v/>
@@ -5907,7 +5907,7 @@
         <v/>
       </c>
       <c r="M45">
-        <v>45.31525259061344</v>
+        <v>49.05119699208868</v>
       </c>
       <c r="N45" t="str">
         <v/>
@@ -5925,7 +5925,7 @@
         <v/>
       </c>
       <c r="S45">
-        <v>42.272025299712645</v>
+        <v>41.053963342023124</v>
       </c>
     </row>
     <row r="46">
@@ -5948,7 +5948,7 @@
         <v/>
       </c>
       <c r="G46">
-        <v>48.835552403401564</v>
+        <v>47.90769441930645</v>
       </c>
       <c r="H46" t="str">
         <v/>
@@ -5966,7 +5966,7 @@
         <v/>
       </c>
       <c r="M46">
-        <v>49.0008544574271</v>
+        <v>48.67491573094492</v>
       </c>
       <c r="N46" t="str">
         <v/>
@@ -5984,7 +5984,7 @@
         <v/>
       </c>
       <c r="S46">
-        <v>46.269195777149335</v>
+        <v>38.55156404738935</v>
       </c>
     </row>
     <row r="47">
@@ -6007,7 +6007,7 @@
         <v/>
       </c>
       <c r="G47">
-        <v>46.56778267630679</v>
+        <v>45.728944257121576</v>
       </c>
       <c r="H47" t="str">
         <v/>
@@ -6025,7 +6025,7 @@
         <v/>
       </c>
       <c r="M47">
-        <v>43.49800947910513</v>
+        <v>43.07958279017785</v>
       </c>
       <c r="N47" t="str">
         <v/>
@@ -6043,7 +6043,7 @@
         <v/>
       </c>
       <c r="S47">
-        <v>39.326702269403434</v>
+        <v>41.77358663971283</v>
       </c>
     </row>
     <row r="48">
@@ -6066,7 +6066,7 @@
         <v/>
       </c>
       <c r="G48">
-        <v>45.638426735697855</v>
+        <v>54.14168084024345</v>
       </c>
       <c r="H48" t="str">
         <v/>
@@ -6084,7 +6084,7 @@
         <v/>
       </c>
       <c r="M48">
-        <v>48.59605045346241</v>
+        <v>51.844805074322906</v>
       </c>
       <c r="N48" t="str">
         <v/>
@@ -6102,7 +6102,7 @@
         <v/>
       </c>
       <c r="S48">
-        <v>42.81128033506619</v>
+        <v>42.39521360306644</v>
       </c>
     </row>
     <row r="49">
@@ -6125,7 +6125,7 @@
         <v/>
       </c>
       <c r="G49">
-        <v>52.09905008787595</v>
+        <v>50.62638786958744</v>
       </c>
       <c r="H49" t="str">
         <v/>
@@ -6143,7 +6143,7 @@
         <v/>
       </c>
       <c r="M49">
-        <v>51.06203455642046</v>
+        <v>49.562566991686</v>
       </c>
       <c r="N49" t="str">
         <v/>
@@ -6161,7 +6161,7 @@
         <v/>
       </c>
       <c r="S49">
-        <v>39.90509730544293</v>
+        <v>45.52666929060267</v>
       </c>
     </row>
     <row r="50">
@@ -6184,7 +6184,7 @@
         <v/>
       </c>
       <c r="G50">
-        <v>53.113617146592645</v>
+        <v>52.424125811870866</v>
       </c>
       <c r="H50" t="str">
         <v/>
@@ -6202,7 +6202,7 @@
         <v/>
       </c>
       <c r="M50">
-        <v>49.87348266362866</v>
+        <v>48.284633242054284</v>
       </c>
       <c r="N50" t="str">
         <v/>
@@ -6220,7 +6220,7 @@
         <v/>
       </c>
       <c r="S50">
-        <v>40.91630382393551</v>
+        <v>39.28432767653774</v>
       </c>
     </row>
     <row r="51">

</xml_diff>